<commit_message>
Reorganised Case Study project and functions Fixed bug where the last route in the archive would not be added to the archive routes
</commit_message>
<xml_diff>
--- a/vrp_case_study/Solve Times Summary.xlsx
+++ b/vrp_case_study/Solve Times Summary.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Aaron\Documents\Git Repositories\VRP-DSS\vrp_dss\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Aaron\Documents\Git Repositories\VRP-Case-Study\vrp_case_study\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{140A615A-C713-4823-8019-A1535E71DA7E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14FF6A23-01E5-4412-8E1B-8661DF9D9079}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="270">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="277" uniqueCount="271">
   <si>
     <t># Customers</t>
   </si>
@@ -3035,9 +3035,6 @@
   </si>
   <si>
     <t>Difference (%)</t>
-  </si>
-  <si>
-    <t>Aspects added</t>
   </si>
   <si>
     <t>{"2": [[[17, 24], [164, 4]], [[44, 30]], [[111, 3], [77, 27]], [[149, 28], [148, 2]], [[165, 30]], [[159, 19], [194, 11]], [[41, 30]], [[172, 30]], [[79, 30]], [[104, 30]], [[6, 23], [187, 7]], [[176, 30]], [[153, 30]], [[208, 30]], [[35, 30]], [[100, 30]], [[83, 20]], [[40, 30]], [[117, 7], [126, 14], [125, 9]], [[121, 12], [143, 11], [193, 7]], [[80, 20], [168, 9]], [[135, 5], [182, 15], [95, 10]], [[81, 30]], [[193, 12], [143, 18]], [[121, 19], [135, 10]]], "1": [[[75, 18]], [[149, 22]], [[24, 8], [25, 14]], [[207, 21]], [[72, 22]], [[119, 10], [2, 12]], [[157, 22]], [[46, 20]], [[188, 22]], [[186, 9], [53, 12]], [[130, 22]], [[83, 20]], [[116, 10], [177, 11], [203, 1]], [[27, 22]]], "0": [[[194, 16]], [[16, 10], [165, 4]], [[156, 16]], [[77, 11]], [[120, 11], [198, 5]], [[151, 16]], [[196, 8], [48, 5]], [[34, 14]], [[9, 15]], [[154, 13]], [[8, 16]], [[108, 11]], [[152, 15]], [[120, 12]], [[199, 1], [91, 6], [81, 6]], [[197, 14]], [[131, 16]], [[151, 9], [173, 7]], [[144, 12]], [[166, 6], [28, 2], [3, 8]], [[97, 13]], [[66, 15]]]}</t>
@@ -4687,6 +4684,12 @@
   </si>
   <si>
     <t>Seeded solutions will be split again if customer completion changed their chromosomes (I am also regenerating the model data sheets just in case of errors).</t>
+  </si>
+  <si>
+    <t>Fixed last route in archive not being added to routes JSON</t>
+  </si>
+  <si>
+    <t>Aspects changed</t>
   </si>
 </sst>
 </file>
@@ -12923,6 +12926,189 @@
     </row>
   </sheetData>
   <mergeCells count="207">
+    <mergeCell ref="H31:I31"/>
+    <mergeCell ref="H12:I12"/>
+    <mergeCell ref="H13:I13"/>
+    <mergeCell ref="H14:I14"/>
+    <mergeCell ref="H15:I15"/>
+    <mergeCell ref="H16:I16"/>
+    <mergeCell ref="H17:I17"/>
+    <mergeCell ref="H18:I18"/>
+    <mergeCell ref="H19:I19"/>
+    <mergeCell ref="H20:I20"/>
+    <mergeCell ref="H21:I21"/>
+    <mergeCell ref="H23:I23"/>
+    <mergeCell ref="H24:I24"/>
+    <mergeCell ref="H22:I22"/>
+    <mergeCell ref="H25:I25"/>
+    <mergeCell ref="H26:I26"/>
+    <mergeCell ref="H27:I27"/>
+    <mergeCell ref="H28:I28"/>
+    <mergeCell ref="H29:I29"/>
+    <mergeCell ref="H30:I30"/>
+    <mergeCell ref="H205:I205"/>
+    <mergeCell ref="H206:I206"/>
+    <mergeCell ref="H207:I207"/>
+    <mergeCell ref="H208:I208"/>
+    <mergeCell ref="H178:I178"/>
+    <mergeCell ref="H179:I179"/>
+    <mergeCell ref="H180:I180"/>
+    <mergeCell ref="H199:I199"/>
+    <mergeCell ref="H200:I200"/>
+    <mergeCell ref="H201:I201"/>
+    <mergeCell ref="H202:I202"/>
+    <mergeCell ref="H203:I203"/>
+    <mergeCell ref="H204:I204"/>
+    <mergeCell ref="H184:I184"/>
+    <mergeCell ref="H185:I185"/>
+    <mergeCell ref="H186:I186"/>
+    <mergeCell ref="H187:I187"/>
+    <mergeCell ref="H188:I188"/>
+    <mergeCell ref="H189:I189"/>
+    <mergeCell ref="H190:I190"/>
+    <mergeCell ref="H191:I191"/>
+    <mergeCell ref="H192:I192"/>
+    <mergeCell ref="H193:I193"/>
+    <mergeCell ref="H194:I194"/>
+    <mergeCell ref="H174:I174"/>
+    <mergeCell ref="H175:I175"/>
+    <mergeCell ref="H176:I176"/>
+    <mergeCell ref="H177:I177"/>
+    <mergeCell ref="H173:I173"/>
+    <mergeCell ref="H130:I130"/>
+    <mergeCell ref="H170:I170"/>
+    <mergeCell ref="H171:I171"/>
+    <mergeCell ref="H172:I172"/>
+    <mergeCell ref="H137:I137"/>
+    <mergeCell ref="H138:I138"/>
+    <mergeCell ref="H139:I139"/>
+    <mergeCell ref="H158:I158"/>
+    <mergeCell ref="H159:I159"/>
+    <mergeCell ref="H160:I160"/>
+    <mergeCell ref="H161:I161"/>
+    <mergeCell ref="H162:I162"/>
+    <mergeCell ref="H149:I149"/>
+    <mergeCell ref="H150:I150"/>
+    <mergeCell ref="H155:I155"/>
+    <mergeCell ref="H156:I156"/>
+    <mergeCell ref="H157:I157"/>
+    <mergeCell ref="H10:I10"/>
+    <mergeCell ref="H11:I11"/>
+    <mergeCell ref="H32:I32"/>
+    <mergeCell ref="H33:I33"/>
+    <mergeCell ref="H34:I34"/>
+    <mergeCell ref="H35:I35"/>
+    <mergeCell ref="H36:I36"/>
+    <mergeCell ref="H120:I120"/>
+    <mergeCell ref="H81:I81"/>
+    <mergeCell ref="H82:I82"/>
+    <mergeCell ref="H83:I83"/>
+    <mergeCell ref="H90:I90"/>
+    <mergeCell ref="H91:I91"/>
+    <mergeCell ref="H92:I92"/>
+    <mergeCell ref="H99:I99"/>
+    <mergeCell ref="H100:I100"/>
+    <mergeCell ref="H116:I116"/>
+    <mergeCell ref="H117:I117"/>
+    <mergeCell ref="H118:I118"/>
+    <mergeCell ref="H119:I119"/>
+    <mergeCell ref="H112:I112"/>
+    <mergeCell ref="H113:I113"/>
+    <mergeCell ref="H114:I114"/>
+    <mergeCell ref="H115:I115"/>
+    <mergeCell ref="H2:I2"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="H4:I4"/>
+    <mergeCell ref="H5:I5"/>
+    <mergeCell ref="H6:I6"/>
+    <mergeCell ref="H68:I68"/>
+    <mergeCell ref="H69:I69"/>
+    <mergeCell ref="H70:I70"/>
+    <mergeCell ref="H71:I71"/>
+    <mergeCell ref="H63:I63"/>
+    <mergeCell ref="H7:I7"/>
+    <mergeCell ref="H8:I8"/>
+    <mergeCell ref="H9:I9"/>
+    <mergeCell ref="H51:I51"/>
+    <mergeCell ref="H39:I39"/>
+    <mergeCell ref="H37:I37"/>
+    <mergeCell ref="H38:I38"/>
+    <mergeCell ref="H64:I64"/>
+    <mergeCell ref="H65:I65"/>
+    <mergeCell ref="H66:I66"/>
+    <mergeCell ref="H67:I67"/>
+    <mergeCell ref="H62:I62"/>
+    <mergeCell ref="H60:I60"/>
+    <mergeCell ref="H61:I61"/>
+    <mergeCell ref="H125:I125"/>
+    <mergeCell ref="H126:I126"/>
+    <mergeCell ref="H127:I127"/>
+    <mergeCell ref="H128:I128"/>
+    <mergeCell ref="H129:I129"/>
+    <mergeCell ref="H121:I121"/>
+    <mergeCell ref="H122:I122"/>
+    <mergeCell ref="H123:I123"/>
+    <mergeCell ref="H124:I124"/>
+    <mergeCell ref="H110:I110"/>
+    <mergeCell ref="H111:I111"/>
+    <mergeCell ref="H101:I101"/>
+    <mergeCell ref="H102:I102"/>
+    <mergeCell ref="H103:I103"/>
+    <mergeCell ref="H105:I105"/>
+    <mergeCell ref="H106:I106"/>
+    <mergeCell ref="H107:I107"/>
+    <mergeCell ref="H108:I108"/>
+    <mergeCell ref="H109:I109"/>
+    <mergeCell ref="H104:I104"/>
+    <mergeCell ref="H49:I49"/>
+    <mergeCell ref="H52:I52"/>
+    <mergeCell ref="H53:I53"/>
+    <mergeCell ref="H54:I54"/>
+    <mergeCell ref="H55:I55"/>
+    <mergeCell ref="H56:I56"/>
+    <mergeCell ref="H57:I57"/>
+    <mergeCell ref="H58:I58"/>
+    <mergeCell ref="H59:I59"/>
+    <mergeCell ref="H50:I50"/>
+    <mergeCell ref="H40:I40"/>
+    <mergeCell ref="H41:I41"/>
+    <mergeCell ref="H42:I42"/>
+    <mergeCell ref="H43:I43"/>
+    <mergeCell ref="H44:I44"/>
+    <mergeCell ref="H45:I45"/>
+    <mergeCell ref="H152:I152"/>
+    <mergeCell ref="H153:I153"/>
+    <mergeCell ref="H154:I154"/>
+    <mergeCell ref="H140:I140"/>
+    <mergeCell ref="H141:I141"/>
+    <mergeCell ref="H142:I142"/>
+    <mergeCell ref="H143:I143"/>
+    <mergeCell ref="H144:I144"/>
+    <mergeCell ref="H145:I145"/>
+    <mergeCell ref="H46:I46"/>
+    <mergeCell ref="H47:I47"/>
+    <mergeCell ref="H48:I48"/>
+    <mergeCell ref="H93:I93"/>
+    <mergeCell ref="H94:I94"/>
+    <mergeCell ref="H95:I95"/>
+    <mergeCell ref="H96:I96"/>
+    <mergeCell ref="H97:I97"/>
+    <mergeCell ref="H98:I98"/>
+    <mergeCell ref="H72:I72"/>
+    <mergeCell ref="H73:I73"/>
+    <mergeCell ref="H74:I74"/>
+    <mergeCell ref="H75:I75"/>
+    <mergeCell ref="H86:I86"/>
+    <mergeCell ref="H87:I87"/>
+    <mergeCell ref="H88:I88"/>
+    <mergeCell ref="H89:I89"/>
+    <mergeCell ref="H76:I76"/>
+    <mergeCell ref="H84:I84"/>
+    <mergeCell ref="H85:I85"/>
+    <mergeCell ref="H77:I77"/>
+    <mergeCell ref="H78:I78"/>
+    <mergeCell ref="H79:I79"/>
+    <mergeCell ref="H80:I80"/>
     <mergeCell ref="H195:I195"/>
     <mergeCell ref="H196:I196"/>
     <mergeCell ref="H197:I197"/>
@@ -12947,189 +13133,6 @@
     <mergeCell ref="H147:I147"/>
     <mergeCell ref="H148:I148"/>
     <mergeCell ref="H151:I151"/>
-    <mergeCell ref="H72:I72"/>
-    <mergeCell ref="H73:I73"/>
-    <mergeCell ref="H74:I74"/>
-    <mergeCell ref="H75:I75"/>
-    <mergeCell ref="H86:I86"/>
-    <mergeCell ref="H87:I87"/>
-    <mergeCell ref="H88:I88"/>
-    <mergeCell ref="H89:I89"/>
-    <mergeCell ref="H76:I76"/>
-    <mergeCell ref="H84:I84"/>
-    <mergeCell ref="H85:I85"/>
-    <mergeCell ref="H77:I77"/>
-    <mergeCell ref="H78:I78"/>
-    <mergeCell ref="H79:I79"/>
-    <mergeCell ref="H80:I80"/>
-    <mergeCell ref="H40:I40"/>
-    <mergeCell ref="H41:I41"/>
-    <mergeCell ref="H42:I42"/>
-    <mergeCell ref="H43:I43"/>
-    <mergeCell ref="H44:I44"/>
-    <mergeCell ref="H45:I45"/>
-    <mergeCell ref="H152:I152"/>
-    <mergeCell ref="H153:I153"/>
-    <mergeCell ref="H154:I154"/>
-    <mergeCell ref="H140:I140"/>
-    <mergeCell ref="H141:I141"/>
-    <mergeCell ref="H142:I142"/>
-    <mergeCell ref="H143:I143"/>
-    <mergeCell ref="H144:I144"/>
-    <mergeCell ref="H145:I145"/>
-    <mergeCell ref="H46:I46"/>
-    <mergeCell ref="H47:I47"/>
-    <mergeCell ref="H48:I48"/>
-    <mergeCell ref="H93:I93"/>
-    <mergeCell ref="H94:I94"/>
-    <mergeCell ref="H95:I95"/>
-    <mergeCell ref="H96:I96"/>
-    <mergeCell ref="H97:I97"/>
-    <mergeCell ref="H98:I98"/>
-    <mergeCell ref="H49:I49"/>
-    <mergeCell ref="H52:I52"/>
-    <mergeCell ref="H53:I53"/>
-    <mergeCell ref="H54:I54"/>
-    <mergeCell ref="H55:I55"/>
-    <mergeCell ref="H56:I56"/>
-    <mergeCell ref="H57:I57"/>
-    <mergeCell ref="H58:I58"/>
-    <mergeCell ref="H59:I59"/>
-    <mergeCell ref="H50:I50"/>
-    <mergeCell ref="H110:I110"/>
-    <mergeCell ref="H111:I111"/>
-    <mergeCell ref="H101:I101"/>
-    <mergeCell ref="H102:I102"/>
-    <mergeCell ref="H103:I103"/>
-    <mergeCell ref="H105:I105"/>
-    <mergeCell ref="H106:I106"/>
-    <mergeCell ref="H107:I107"/>
-    <mergeCell ref="H108:I108"/>
-    <mergeCell ref="H109:I109"/>
-    <mergeCell ref="H104:I104"/>
-    <mergeCell ref="H125:I125"/>
-    <mergeCell ref="H126:I126"/>
-    <mergeCell ref="H127:I127"/>
-    <mergeCell ref="H128:I128"/>
-    <mergeCell ref="H129:I129"/>
-    <mergeCell ref="H121:I121"/>
-    <mergeCell ref="H122:I122"/>
-    <mergeCell ref="H123:I123"/>
-    <mergeCell ref="H124:I124"/>
-    <mergeCell ref="H2:I2"/>
-    <mergeCell ref="H3:I3"/>
-    <mergeCell ref="H4:I4"/>
-    <mergeCell ref="H5:I5"/>
-    <mergeCell ref="H6:I6"/>
-    <mergeCell ref="H68:I68"/>
-    <mergeCell ref="H69:I69"/>
-    <mergeCell ref="H70:I70"/>
-    <mergeCell ref="H71:I71"/>
-    <mergeCell ref="H63:I63"/>
-    <mergeCell ref="H7:I7"/>
-    <mergeCell ref="H8:I8"/>
-    <mergeCell ref="H9:I9"/>
-    <mergeCell ref="H51:I51"/>
-    <mergeCell ref="H39:I39"/>
-    <mergeCell ref="H37:I37"/>
-    <mergeCell ref="H38:I38"/>
-    <mergeCell ref="H64:I64"/>
-    <mergeCell ref="H65:I65"/>
-    <mergeCell ref="H66:I66"/>
-    <mergeCell ref="H67:I67"/>
-    <mergeCell ref="H62:I62"/>
-    <mergeCell ref="H60:I60"/>
-    <mergeCell ref="H61:I61"/>
-    <mergeCell ref="H10:I10"/>
-    <mergeCell ref="H11:I11"/>
-    <mergeCell ref="H32:I32"/>
-    <mergeCell ref="H33:I33"/>
-    <mergeCell ref="H34:I34"/>
-    <mergeCell ref="H35:I35"/>
-    <mergeCell ref="H36:I36"/>
-    <mergeCell ref="H120:I120"/>
-    <mergeCell ref="H81:I81"/>
-    <mergeCell ref="H82:I82"/>
-    <mergeCell ref="H83:I83"/>
-    <mergeCell ref="H90:I90"/>
-    <mergeCell ref="H91:I91"/>
-    <mergeCell ref="H92:I92"/>
-    <mergeCell ref="H99:I99"/>
-    <mergeCell ref="H100:I100"/>
-    <mergeCell ref="H116:I116"/>
-    <mergeCell ref="H117:I117"/>
-    <mergeCell ref="H118:I118"/>
-    <mergeCell ref="H119:I119"/>
-    <mergeCell ref="H112:I112"/>
-    <mergeCell ref="H113:I113"/>
-    <mergeCell ref="H114:I114"/>
-    <mergeCell ref="H115:I115"/>
-    <mergeCell ref="H174:I174"/>
-    <mergeCell ref="H175:I175"/>
-    <mergeCell ref="H176:I176"/>
-    <mergeCell ref="H177:I177"/>
-    <mergeCell ref="H173:I173"/>
-    <mergeCell ref="H130:I130"/>
-    <mergeCell ref="H170:I170"/>
-    <mergeCell ref="H171:I171"/>
-    <mergeCell ref="H172:I172"/>
-    <mergeCell ref="H137:I137"/>
-    <mergeCell ref="H138:I138"/>
-    <mergeCell ref="H139:I139"/>
-    <mergeCell ref="H158:I158"/>
-    <mergeCell ref="H159:I159"/>
-    <mergeCell ref="H160:I160"/>
-    <mergeCell ref="H161:I161"/>
-    <mergeCell ref="H162:I162"/>
-    <mergeCell ref="H149:I149"/>
-    <mergeCell ref="H150:I150"/>
-    <mergeCell ref="H155:I155"/>
-    <mergeCell ref="H156:I156"/>
-    <mergeCell ref="H157:I157"/>
-    <mergeCell ref="H205:I205"/>
-    <mergeCell ref="H206:I206"/>
-    <mergeCell ref="H207:I207"/>
-    <mergeCell ref="H208:I208"/>
-    <mergeCell ref="H178:I178"/>
-    <mergeCell ref="H179:I179"/>
-    <mergeCell ref="H180:I180"/>
-    <mergeCell ref="H199:I199"/>
-    <mergeCell ref="H200:I200"/>
-    <mergeCell ref="H201:I201"/>
-    <mergeCell ref="H202:I202"/>
-    <mergeCell ref="H203:I203"/>
-    <mergeCell ref="H204:I204"/>
-    <mergeCell ref="H184:I184"/>
-    <mergeCell ref="H185:I185"/>
-    <mergeCell ref="H186:I186"/>
-    <mergeCell ref="H187:I187"/>
-    <mergeCell ref="H188:I188"/>
-    <mergeCell ref="H189:I189"/>
-    <mergeCell ref="H190:I190"/>
-    <mergeCell ref="H191:I191"/>
-    <mergeCell ref="H192:I192"/>
-    <mergeCell ref="H193:I193"/>
-    <mergeCell ref="H194:I194"/>
-    <mergeCell ref="H31:I31"/>
-    <mergeCell ref="H12:I12"/>
-    <mergeCell ref="H13:I13"/>
-    <mergeCell ref="H14:I14"/>
-    <mergeCell ref="H15:I15"/>
-    <mergeCell ref="H16:I16"/>
-    <mergeCell ref="H17:I17"/>
-    <mergeCell ref="H18:I18"/>
-    <mergeCell ref="H19:I19"/>
-    <mergeCell ref="H20:I20"/>
-    <mergeCell ref="H21:I21"/>
-    <mergeCell ref="H23:I23"/>
-    <mergeCell ref="H24:I24"/>
-    <mergeCell ref="H22:I22"/>
-    <mergeCell ref="H25:I25"/>
-    <mergeCell ref="H26:I26"/>
-    <mergeCell ref="H27:I27"/>
-    <mergeCell ref="H28:I28"/>
-    <mergeCell ref="H29:I29"/>
-    <mergeCell ref="H30:I30"/>
   </mergeCells>
   <conditionalFormatting sqref="R2:R61 R63:R1048576">
     <cfRule type="cellIs" dxfId="15" priority="21" operator="notBetween">
@@ -13206,10 +13209,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:L18"/>
+  <dimension ref="A1:L19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J19" sqref="J19"/>
+      <selection activeCell="L2" sqref="L2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13225,7 +13228,7 @@
     <col min="9" max="9" width="12.85546875" style="11" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="13.5703125" style="11" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="14" style="11" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="38.7109375" style="11" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="41.7109375" style="11" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
@@ -13263,7 +13266,7 @@
         <v>217</v>
       </c>
       <c r="L1" s="5" t="s">
-        <v>218</v>
+        <v>270</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
@@ -13271,13 +13274,13 @@
         <v>43745</v>
       </c>
       <c r="B2" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="C2">
         <v>469154.88979999977</v>
       </c>
       <c r="F2" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="G2">
         <v>3603.7618333999999</v>
@@ -13299,13 +13302,13 @@
         <v>43768</v>
       </c>
       <c r="B3" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="C3">
         <v>592286.43533333309</v>
       </c>
       <c r="F3" s="7" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="G3">
         <v>3600.6243162000001</v>
@@ -13322,7 +13325,7 @@
         <v>-2.8570731981184649E-2</v>
       </c>
       <c r="L3" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
@@ -13330,16 +13333,16 @@
         <v>43775</v>
       </c>
       <c r="B4" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="C4">
         <v>471229.1394000001</v>
       </c>
       <c r="E4" t="s">
+        <v>224</v>
+      </c>
+      <c r="F4" t="s">
         <v>225</v>
-      </c>
-      <c r="F4" t="s">
-        <v>226</v>
       </c>
       <c r="G4">
         <v>3893.4923675999999</v>
@@ -13361,16 +13364,16 @@
         <v>43775</v>
       </c>
       <c r="B5" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C5">
         <v>1428685.831666667</v>
       </c>
       <c r="E5" t="s">
+        <v>227</v>
+      </c>
+      <c r="F5" t="s">
         <v>228</v>
-      </c>
-      <c r="F5" t="s">
-        <v>229</v>
       </c>
       <c r="G5">
         <v>3661.4549959999999</v>
@@ -13387,7 +13390,7 @@
         <v>0.11307985414694049</v>
       </c>
       <c r="L5" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
@@ -13395,16 +13398,16 @@
         <v>43768</v>
       </c>
       <c r="B6" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="C6">
         <v>592286.43533333309</v>
       </c>
       <c r="E6" t="s">
+        <v>230</v>
+      </c>
+      <c r="F6" t="s">
         <v>231</v>
-      </c>
-      <c r="F6" t="s">
-        <v>232</v>
       </c>
       <c r="G6">
         <v>3786.4904317999999</v>
@@ -13426,16 +13429,16 @@
         <v>43745</v>
       </c>
       <c r="B7" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="C7">
         <v>469154.88979999977</v>
       </c>
       <c r="E7" t="s">
+        <v>232</v>
+      </c>
+      <c r="F7" t="s">
         <v>233</v>
-      </c>
-      <c r="F7" t="s">
-        <v>234</v>
       </c>
       <c r="G7">
         <v>3601.0539597000002</v>
@@ -13457,16 +13460,16 @@
         <v>43795</v>
       </c>
       <c r="B8" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="C8">
         <v>1275847.0800666669</v>
       </c>
       <c r="E8" t="s">
+        <v>235</v>
+      </c>
+      <c r="F8" t="s">
         <v>236</v>
-      </c>
-      <c r="F8" t="s">
-        <v>237</v>
       </c>
       <c r="G8">
         <v>3902.6114637000001</v>
@@ -13488,16 +13491,16 @@
         <v>43768</v>
       </c>
       <c r="B9" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="C9">
         <v>592286.43533333309</v>
       </c>
       <c r="E9" t="s">
+        <v>237</v>
+      </c>
+      <c r="F9" t="s">
         <v>238</v>
-      </c>
-      <c r="F9" t="s">
-        <v>239</v>
       </c>
       <c r="G9">
         <v>7200.1489792000002</v>
@@ -13519,16 +13522,16 @@
         <v>43745</v>
       </c>
       <c r="B10" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="C10">
         <v>475403.35446666653</v>
       </c>
       <c r="E10" t="s">
+        <v>240</v>
+      </c>
+      <c r="F10" t="s">
         <v>241</v>
-      </c>
-      <c r="F10" t="s">
-        <v>242</v>
       </c>
       <c r="G10">
         <v>3601.0659418</v>
@@ -13545,7 +13548,7 @@
         <v>0.12671645898302314</v>
       </c>
       <c r="L10" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
@@ -13553,16 +13556,16 @@
         <v>43768</v>
       </c>
       <c r="B11" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="C11">
         <v>600912.63166666601</v>
       </c>
       <c r="E11" t="s">
+        <v>244</v>
+      </c>
+      <c r="F11" t="s">
         <v>245</v>
-      </c>
-      <c r="F11" t="s">
-        <v>246</v>
       </c>
       <c r="G11">
         <v>3600.2064667</v>
@@ -13584,16 +13587,16 @@
         <v>43745</v>
       </c>
       <c r="B12" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="C12">
         <v>494345.58179999999</v>
       </c>
       <c r="E12" t="s">
+        <v>247</v>
+      </c>
+      <c r="F12" t="s">
         <v>248</v>
-      </c>
-      <c r="F12" t="s">
-        <v>249</v>
       </c>
       <c r="G12">
         <v>7170.8296077000005</v>
@@ -13610,7 +13613,7 @@
         <v>6.5150951451266648E-2</v>
       </c>
       <c r="L12" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
@@ -13618,16 +13621,16 @@
         <v>43768</v>
       </c>
       <c r="B13" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="C13">
         <v>593149.57433333329</v>
       </c>
       <c r="E13" t="s">
+        <v>251</v>
+      </c>
+      <c r="F13" t="s">
         <v>252</v>
-      </c>
-      <c r="F13" t="s">
-        <v>253</v>
       </c>
       <c r="G13">
         <v>5056.3446751000001</v>
@@ -13649,16 +13652,16 @@
         <v>43795</v>
       </c>
       <c r="B14" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="C14">
         <v>1372973.317933334</v>
       </c>
       <c r="E14" t="s">
+        <v>254</v>
+      </c>
+      <c r="F14" t="s">
         <v>255</v>
-      </c>
-      <c r="F14" t="s">
-        <v>256</v>
       </c>
       <c r="G14">
         <v>7318.0830248000002</v>
@@ -13680,16 +13683,16 @@
         <v>43754</v>
       </c>
       <c r="B15" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="C15">
         <v>636315.92813333333</v>
       </c>
       <c r="E15" t="s">
+        <v>257</v>
+      </c>
+      <c r="F15" t="s">
         <v>258</v>
-      </c>
-      <c r="F15" t="s">
-        <v>259</v>
       </c>
       <c r="G15">
         <v>4347.3198690999998</v>
@@ -13711,16 +13714,16 @@
         <v>43745</v>
       </c>
       <c r="B16" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="C16">
         <v>538213.87013333349</v>
       </c>
       <c r="E16" t="s">
+        <v>260</v>
+      </c>
+      <c r="F16" t="s">
         <v>261</v>
-      </c>
-      <c r="F16" t="s">
-        <v>262</v>
       </c>
       <c r="G16">
         <v>7527.1272962000003</v>
@@ -13737,24 +13740,24 @@
         <v>0.13716106668719871</v>
       </c>
       <c r="L16" t="s">
-        <v>269</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" s="10">
         <v>43768</v>
       </c>
       <c r="B17" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="C17">
         <v>632705.85299999989</v>
       </c>
       <c r="E17" t="s">
+        <v>263</v>
+      </c>
+      <c r="F17" t="s">
         <v>264</v>
-      </c>
-      <c r="F17" t="s">
-        <v>265</v>
       </c>
       <c r="G17">
         <v>6666.2375192999998</v>
@@ -13771,21 +13774,21 @@
         <v>6.6456467568034458E-2</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" s="8">
         <v>43795</v>
       </c>
       <c r="B18" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="C18">
         <v>1432583.6294</v>
       </c>
       <c r="E18" t="s">
+        <v>266</v>
+      </c>
+      <c r="F18" t="s">
         <v>267</v>
-      </c>
-      <c r="F18" t="s">
-        <v>268</v>
       </c>
       <c r="G18">
         <v>7733.803919</v>
@@ -13800,6 +13803,11 @@
       <c r="K18" s="12">
         <f t="shared" si="0"/>
         <v>0.12408410691373345</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L19" s="11" t="s">
+        <v>269</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added consideration for 150km max local range of SPAR's own fleet Added check if decompositions have time to run before running them Reran case study instances
</commit_message>
<xml_diff>
--- a/vrp_case_study/Solve Times Summary.xlsx
+++ b/vrp_case_study/Solve Times Summary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Aaron\Documents\Git Repositories\VRP-Case-Study\vrp_case_study\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07D58FFC-B774-4FD6-A0CA-D171E0F1552C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26C4949D-9D08-408B-8010-87AD6EBD625C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,6 +28,7 @@
         <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="308" uniqueCount="296">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="318" uniqueCount="303">
   <si>
     <t># Customers</t>
   </si>
@@ -3014,6 +3015,9 @@
   </si>
   <si>
     <t>Archive Routes</t>
+  </si>
+  <si>
+    <t>Archive Routes (Pretty)</t>
   </si>
   <si>
     <t>Archive Cost</t>
@@ -5403,6 +5407,9 @@
 </t>
   </si>
   <si>
+    <t>Customer completion bugfixes</t>
+  </si>
+  <si>
     <t>{"0": [[[151, 15]], [[199, 10]], [[155, 1], [62, 1], [57, 13]], [[188, 15], [39, 1]]], "1": [[[192, 22]], [[38, 22]], [[82, 22]], [[207, 20]]], "2": [[[96, 16], [42, 12]], [[2, 14], [119, 12]], [[46, 16], [91, 13]], [[63, 16], [53, 13]], [[131, 12], [4, 11]], [[33, 30]], [[121, 6], [143, 5], [17, 15], [8, 4]], [[100, 30]], [[153, 30]], [[120, 17], [112, 1], [198, 6]], [[55, 30]], [[88, 22], [74, 5]], [[97, 7], [101, 10], [75, 6], [19, 6]], [[182, 6], [157, 24]], [[3, 27], [191, 2]], [[9, 10], [163, 17]], [[208, 24]], [[149, 30]], [[172, 30]], [[165, 30]], [[148, 6], [149, 24]], [[16, 30]], [[159, 24], [41, 6]], [[18, 15], [200, 15]], [[150, 8], [172, 20]], [[35, 30]], [[153, 14], [98, 16]], [[6, 14], [194, 8], [187, 8]], [[41, 30]], [[194, 30]], [[140, 30]], [[209, 9], [176, 16], [35, 5]], [[81, 30]], [[164, 1], [49, 24]], [[174, 5], [104, 6], [110, 19]], [[104, 30]], [[37, 10], [93, 9], [70, 7]], [[152, 4], [108, 9], [34, 16]], [[44, 30]], [[1, 3], [154, 15], [68, 10]], [[168, 9], [156, 11], [132, 10]], [[126, 10], [117, 6], [125, 14]], [[40, 30]], [[196, 13], [135, 5], [33, 9]], [[32, 27]], [[92, 30]], [[97, 30]], [[186, 15], [134, 10], [171, 2]], [[24, 25], [25, 4]], [[25, 30]], [[29, 29]], [[59, 28], [81, 2]], [[48, 5], [197, 25]], [[72, 30]], [[4, 30]], [[40, 15], [139, 15]], [[15, 28]], [[193, 4], [28, 6], [95, 15]], [[8, 30]]], "3": [[[123, 2], [87, 1], [94, 5], [83, 31]], [[66, 35]], [[79, 37], [144, 3]], [[77, 37]]]}</t>
   </si>
   <si>
@@ -5622,10 +5629,268 @@
 </t>
   </si>
   <si>
-    <t>Customer completion bugfixes</t>
-  </si>
-  <si>
-    <t>Archive Routes (Pretty)</t>
+    <t>{"0": [[[154, 14]], [[66, 15]]], "1": [[[2, 12], [119, 10]], [[157, 22]], [[27, 22]], [[207, 21]], [[72, 22]], [[24, 8], [25, 14]], [[159, 19]], [[144, 12], [16, 10]]], "2": [[[186, 9], [131, 16]], [[143, 29]], [[152, 15], [53, 12]], [[164, 4], [126, 14], [19, 11]], [[46, 20], [168, 9]], [[80, 20], [91, 6], [199, 1]], [[176, 30]], [[3, 8], [193, 19]], [[120, 23], [198, 5]], [[75, 19], [101, 5]], [[135, 15], [9, 15]], [[28, 2], [95, 10], [182, 15]], [[104, 30]], [[40, 30]], [[6, 23], [173, 7]], [[41, 30]], [[187, 7], [203, 1], [177, 11], [116, 10]], [[194, 27]], [[17, 24], [166, 6]], [[208, 30]], [[8, 16], [97, 13]], [[34, 14], [108, 11]], [[100, 30]], [[130, 22], [196, 8]], [[44, 30]], [[35, 30]], [[172, 30]], [[125, 9], [197, 14], [117, 7]], [[153, 30]], [[149, 19], [77, 9], [111, 2]], [[151, 25]], [[149, 30]], [[79, 30]], [[77, 30]]], "3": [[[48, 5], [121, 31]], [[81, 36]], [[83, 40]], [[156, 15], [188, 22], [39, 1]], [[148, 3], [165, 34]]]}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rigid (capacity 16):
+154-S (14)
+66-G (15)
+8 Metre (capacity 22):
+2-A (12) -&gt; 119-O (10)
+157-S (22)
+27-C (22)
+207-Y (21)
+72-G (22)
+24-B (8) -&gt; 25-C (14)
+159-S (19)
+144-Q (12) -&gt; 16-B (10)
+11 Metre (capacity 30):
+186-V (9) -&gt; 131-P (16)
+143-P (29)
+152-R (15) -&gt; 53-E (12)
+164-S (4) -&gt; 126-P (14) -&gt; 19-B (11)
+46-D (20) -&gt; 168-S (9)
+80-H (20) -&gt; 91-K (6) -&gt; 199-W (1)
+176-T (30)
+3-A (8) -&gt; 193-V (19)
+120-O (23) -&gt; 198-W (5)
+75-H (19) -&gt; 101-L (5)
+135-P (15) -&gt; 9-B (15)
+28-C (2) -&gt; 95-K (10) -&gt; 182-U (15)
+104-M (30)
+40-C (30)
+6-B (23) -&gt; 173-T (7)
+41-C (30)
+187-V (7) -&gt; 203-W (1) -&gt; 177-T (11) -&gt; 116-N (10)
+194-V (27)
+17-B (24) -&gt; 166-S (6)
+208-Z (30)
+8-B (16) -&gt; 97-K (13)
+34-C (14) -&gt; 108-M (11)
+100-L (30)
+130-P (22) -&gt; 196-W (8)
+44-D (30)
+35-C (30)
+172-S (30)
+125-P (9) -&gt; 197-W (14) -&gt; 117-N (7)
+153-S (30)
+149-R (19) -&gt; 77-H (9) -&gt; 111-M (2)
+151-R (25)
+149-R (30)
+79-H (30)
+77-H (30)
+Link (capacity 40):
+48-D (5) -&gt; 121-O (31)
+81-H (36)
+83-H (40)
+156-S (15) -&gt; 188-V (22) -&gt; 39-C (1)
+148-R (3) -&gt; 165-S (34)
+</t>
+  </si>
+  <si>
+    <t>150km local service radius for SPAR's own fleet</t>
+  </si>
+  <si>
+    <t>{"0": [[[123, 2]], [[176, 16]], [[199, 10]]], "1": [[[192, 22]], [[207, 20]], [[82, 22]], [[38, 22]]], "2": [[[96, 16], [42, 12]], [[186, 15]], [[120, 17]], [[55, 30]], [[37, 10]], [[63, 16], [53, 13]], [[2, 14], [171, 2], [134, 10]], [[151, 15], [119, 12]], [[81, 2], [39, 1], [188, 15], [168, 9]], [[32, 27]], [[87, 1], [57, 13], [94, 5], [62, 1], [155, 1]], [[29, 29]], [[163, 17], [4, 11]], [[49, 24], [143, 5]], [[200, 15], [68, 10]], [[72, 30]], [[131, 12], [196, 13]], [[104, 30]], [[16, 30]], [[75, 6], [19, 6], [9, 10], [121, 6]], [[70, 7], [18, 15], [112, 1]], [[174, 5], [104, 6], [110, 19]], [[34, 16], [108, 9]], [[88, 22], [74, 5]], [[44, 30]], [[135, 5], [197, 25]], [[101, 10], [182, 6], [126, 10], [193, 4]], [[154, 15], [1, 3], [198, 6]], [[66, 5], [24, 25]], [[66, 30]], [[172, 20], [150, 8]], [[4, 30]], [[153, 14], [98, 16]], [[164, 1], [132, 10], [17, 15], [8, 4]], [[152, 4], [159, 24]], [[149, 30]], [[59, 28]], [[165, 30]], [[172, 30]], [[139, 15], [40, 15]], [[95, 15], [91, 13]], [[8, 30]], [[153, 30]], [[100, 30]], [[40, 30]], [[6, 14], [194, 8], [187, 8]], [[15, 28]], [[209, 9], [125, 14], [117, 6]], [[81, 30]], [[3, 27], [191, 2]], [[140, 30]], [[148, 6], [149, 24]], [[92, 30]], [[156, 11], [46, 16]], [[194, 30]], [[157, 24], [28, 6]], [[208, 24]]], "3": [[[93, 9], [83, 31]], [[48, 5], [35, 35]], [[25, 34]], [[33, 39]], [[97, 37]], [[79, 37]], [[77, 37], [144, 3]], [[41, 36]]]}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rigid (capacity 16):
+123-O (2)
+176-T (16)
+199-W (10)
+8 Metre (capacity 22):
+192-V (22)
+207-Y (20)
+82-H (22)
+38-C (22)
+11 Metre (capacity 30):
+96-K (16) -&gt; 42-C (12)
+186-V (15)
+120-O (17)
+55-E (30)
+37-C (10)
+63-G (16) -&gt; 53-E (13)
+2-A (14) -&gt; 171-S (2) -&gt; 134-P (10)
+151-R (15) -&gt; 119-O (12)
+81-H (2) -&gt; 39-C (1) -&gt; 188-V (15) -&gt; 168-S (9)
+32-C (27)
+87-K (1) -&gt; 57-F (13) -&gt; 94-K (5) -&gt; 62-G (1) -&gt; 155-S (1)
+29-C (29)
+163-S (17) -&gt; 4-A (11)
+49-D (24) -&gt; 143-P (5)
+200-W (15) -&gt; 68-G (10)
+72-G (30)
+131-P (12) -&gt; 196-W (13)
+104-M (30)
+16-B (30)
+75-H (6) -&gt; 19-B (6) -&gt; 9-B (10) -&gt; 121-O (6)
+70-G (7) -&gt; 18-B (15) -&gt; 112-M (1)
+174-T (5) -&gt; 104-M (6) -&gt; 110-M (19)
+34-C (16) -&gt; 108-M (9)
+88-K (22) -&gt; 74-G (5)
+44-D (30)
+135-P (5) -&gt; 197-W (25)
+101-L (10) -&gt; 182-U (6) -&gt; 126-P (10) -&gt; 193-V (4)
+154-S (15) -&gt; 1-A (3) -&gt; 198-W (6)
+66-G (5) -&gt; 24-B (25)
+66-G (30)
+172-S (20) -&gt; 150-R (8)
+4-A (30)
+153-S (14) -&gt; 98-L (16)
+164-S (1) -&gt; 132-P (10) -&gt; 17-B (15) -&gt; 8-B (4)
+152-R (4) -&gt; 159-S (24)
+149-R (30)
+59-G (28)
+165-S (30)
+172-S (30)
+139-P (15) -&gt; 40-C (15)
+95-K (15) -&gt; 91-K (13)
+8-B (30)
+153-S (30)
+100-L (30)
+40-C (30)
+6-B (14) -&gt; 194-V (8) -&gt; 187-V (8)
+15-B (28)
+209-Z (9) -&gt; 125-P (14) -&gt; 117-N (6)
+81-H (30)
+3-A (27) -&gt; 191-V (2)
+140-P (30)
+148-R (6) -&gt; 149-R (24)
+92-K (30)
+156-S (11) -&gt; 46-D (16)
+194-V (30)
+157-S (24) -&gt; 28-C (6)
+208-Z (24)
+Link (capacity 40):
+93-K (9) -&gt; 83-H (31)
+48-D (5) -&gt; 35-C (35)
+25-C (34)
+33-C (39)
+97-K (37)
+79-H (37)
+77-H (37) -&gt; 144-Q (3)
+41-C (36)
+</t>
+  </si>
+  <si>
+    <t>{"0": [[[156, 16]], [[195, 1], [68, 8]], [[59, 16]], [[100, 15]]], "1": [[[185, 22]], [[151, 18]], [[207, 22]], [[156, 21]], [[95, 22]], [[89, 22]]], "2": [[[83, 8]], [[113, 4], [94, 6], [102, 4], [155, 1], [62, 13], [50, 2]], [[69, 22]], [[22, 13], [58, 15]], [[128, 17], [131, 7]], [[2, 10]], [[83, 30]], [[208, 11], [80, 16]], [[172, 20], [25, 7]], [[91, 22]], [[95, 26]], [[121, 29]], [[19, 14]], [[124, 30]], [[15, 26], [60, 1]], [[39, 5], [66, 19], [7, 4]], [[166, 4], [76, 20], [61, 2]], [[53, 27]], [[105, 5], [168, 24]], [[69, 30]], [[69, 30]], [[42, 1], [57, 21], [87, 2]], [[56, 11], [92, 16]], [[3, 30]], [[29, 28]], [[69, 30]], [[92, 30]], [[142, 26]], [[101, 21]], [[59, 25]], [[33, 10], [182, 17]], [[1, 30]], [[96, 29]], [[139, 30]], [[97, 29]], [[15, 30]], [[157, 26]], [[134, 21]], [[13, 16], [173, 13]], [[208, 30]], [[158, 5], [20, 18], [110, 7]], [[125, 14], [197, 11]], [[24, 9], [144, 21]], [[109, 30]], [[188, 26]], [[158, 30]], [[191, 4], [193, 19], [81, 5]], [[22, 30]], [[152, 4], [40, 22]], [[90, 16], [200, 13]], [[17, 24], [8, 5]], [[135, 30]], [[118, 9], [132, 15]], [[201, 30]], [[116, 5], [84, 22]], [[20, 30]], [[85, 30]], [[72, 29]], [[176, 8], [35, 21]], [[17, 22], [75, 3]], [[143, 3], [175, 23], [11, 3]], [[46, 24]], [[28, 28]], [[9, 11], [163, 18]], [[130, 19]], [[165, 4], [26, 20]], [[47, 12], [164, 2], [115, 7]], [[49, 30]], [[109, 28], [106, 1]], [[150, 30]], [[91, 28]], [[135, 2], [48, 10], [51, 16]], [[40, 30]], [[78, 6], [119, 12]], [[84, 30]], [[18, 24], [112, 2]], [[120, 9], [72, 16]], [[151, 30]], [[198, 13], [126, 14], [117, 2]], [[98, 30]], [[85, 30]], [[23, 10], [150, 19]], [[143, 30]], [[178, 28]], [[93, 10], [1, 11]], [[205, 9], [206, 7], [45, 13]], [[85, 23], [147, 7]], [[104, 30]], [[174, 14], [104, 12]], [[23, 30]]], "3": [[[186, 38]], [[154, 31]], [[153, 33], [171, 5]], [[10, 40]], [[99, 40]], [[12, 31]], [[111, 40]], [[149, 37]], [[29, 40]], [[41, 39]]]}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rigid (capacity 16):
+156-S (16)
+195-W (1) -&gt; 68-G (8)
+59-G (16)
+100-L (15)
+8 Metre (capacity 22):
+185-V (22)
+151-R (18)
+207-Y (22)
+156-S (21)
+95-K (22)
+89-K (22)
+11 Metre (capacity 30):
+83-H (8)
+113-M (4) -&gt; 94-K (6) -&gt; 102-L (4) -&gt; 155-S (1) -&gt; 62-G (13) -&gt; 50-D (2)
+69-G (22)
+22-B (13) -&gt; 58-G (15)
+128-P (17) -&gt; 131-P (7)
+2-A (10)
+83-H (30)
+208-Z (11) -&gt; 80-H (16)
+172-S (20) -&gt; 25-C (7)
+91-K (22)
+95-K (26)
+121-O (29)
+19-B (14)
+124-O (30)
+15-B (26) -&gt; 60-G (1)
+39-C (5) -&gt; 66-G (19) -&gt; 7-B (4)
+166-S (4) -&gt; 76-H (20) -&gt; 61-G (2)
+53-E (27)
+105-M (5) -&gt; 168-S (24)
+69-G (30)
+69-G (30)
+42-C (1) -&gt; 57-F (21) -&gt; 87-K (2)
+56-F (11) -&gt; 92-K (16)
+3-A (30)
+29-C (28)
+69-G (30)
+92-K (30)
+142-P (26)
+101-L (21)
+59-G (25)
+33-C (10) -&gt; 182-U (17)
+1-A (30)
+96-K (29)
+139-P (30)
+97-K (29)
+15-B (30)
+157-S (26)
+134-P (21)
+13-B (16) -&gt; 173-T (13)
+208-Z (30)
+158-S (5) -&gt; 20-B (18) -&gt; 110-M (7)
+125-P (14) -&gt; 197-W (11)
+24-B (9) -&gt; 144-Q (21)
+109-M (30)
+188-V (26)
+158-S (30)
+191-V (4) -&gt; 193-V (19) -&gt; 81-H (5)
+22-B (30)
+152-R (4) -&gt; 40-C (22)
+90-K (16) -&gt; 200-W (13)
+17-B (24) -&gt; 8-B (5)
+135-P (30)
+118-N (9) -&gt; 132-P (15)
+201-W (30)
+116-N (5) -&gt; 84-K (22)
+20-B (30)
+85-K (30)
+72-G (29)
+176-T (8) -&gt; 35-C (21)
+17-B (22) -&gt; 75-H (3)
+143-P (3) -&gt; 175-T (23) -&gt; 11-B (3)
+46-D (24)
+28-C (28)
+9-B (11) -&gt; 163-S (18)
+130-P (19)
+165-S (4) -&gt; 26-C (20)
+47-D (12) -&gt; 164-S (2) -&gt; 115-N (7)
+49-D (30)
+109-M (28) -&gt; 106-M (1)
+150-R (30)
+91-K (28)
+135-P (2) -&gt; 48-D (10) -&gt; 51-D (16)
+40-C (30)
+78-H (6) -&gt; 119-O (12)
+84-K (30)
+18-B (24) -&gt; 112-M (2)
+120-O (9) -&gt; 72-G (16)
+151-R (30)
+198-W (13) -&gt; 126-P (14) -&gt; 117-N (2)
+98-L (30)
+85-K (30)
+23-B (10) -&gt; 150-R (19)
+143-P (30)
+178-T (28)
+93-K (10) -&gt; 1-A (11)
+205-W (9) -&gt; 206-W (7) -&gt; 45-D (13)
+85-K (23) -&gt; 147-R (7)
+104-M (30)
+174-T (14) -&gt; 104-M (12)
+23-B (30)
+Link (capacity 40):
+186-V (38)
+154-S (31)
+153-S (33) -&gt; 171-S (5)
+10-B (40)
+99-L (40)
+12-B (31)
+111-M (40)
+149-R (37)
+29-C (40)
+41-C (39)
+</t>
   </si>
 </sst>
 </file>
@@ -5740,10 +6005,10 @@
     <xf numFmtId="10" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -6036,7 +6301,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-5FD1-482C-AD23-E4441EC1E74F}"/>
+              <c16:uniqueId val="{00000000-1170-47A5-8824-A2882F781394}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -6109,7 +6374,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-5FD1-482C-AD23-E4441EC1E74F}"/>
+              <c16:uniqueId val="{00000001-1170-47A5-8824-A2882F781394}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -6447,7 +6712,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-8B1F-480A-92E2-CBC0285B7552}"/>
+              <c16:uniqueId val="{00000000-9442-46ED-8001-E7363086CCFC}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -6520,7 +6785,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-8B1F-480A-92E2-CBC0285B7552}"/>
+              <c16:uniqueId val="{00000001-9442-46ED-8001-E7363086CCFC}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -6859,7 +7124,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-A669-40B3-8B0B-8B9957DE8672}"/>
+              <c16:uniqueId val="{00000000-2502-4171-A048-A5D83CD769AE}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -6932,7 +7197,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-A669-40B3-8B0B-8B9957DE8672}"/>
+              <c16:uniqueId val="{00000001-2502-4171-A048-A5D83CD769AE}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -7256,7 +7521,7 @@
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-8339-4166-996E-FA4834188B17}"/>
+              <c16:uniqueId val="{00000000-D43D-45E4-8354-632FD88DDA88}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -7315,7 +7580,7 @@
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-8339-4166-996E-FA4834188B17}"/>
+              <c16:uniqueId val="{00000001-D43D-45E4-8354-632FD88DDA88}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -7652,7 +7917,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-59CE-4ACC-AED2-70C3B4E51796}"/>
+              <c16:uniqueId val="{00000000-0628-47F5-A96F-9C0F03045C4B}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -7725,7 +7990,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-59CE-4ACC-AED2-70C3B4E51796}"/>
+              <c16:uniqueId val="{00000001-0628-47F5-A96F-9C0F03045C4B}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -8062,7 +8327,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-36C8-470C-A7FF-D53D94290221}"/>
+              <c16:uniqueId val="{00000000-C3D6-43E6-85C4-3AADB613EBF5}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -8135,7 +8400,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-36C8-470C-A7FF-D53D94290221}"/>
+              <c16:uniqueId val="{00000001-C3D6-43E6-85C4-3AADB613EBF5}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -8189,7 +8454,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000002-36C8-470C-A7FF-D53D94290221}"/>
+              <c16:uniqueId val="{00000002-C3D6-43E6-85C4-3AADB613EBF5}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -8243,7 +8508,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000003-36C8-470C-A7FF-D53D94290221}"/>
+              <c16:uniqueId val="{00000003-C3D6-43E6-85C4-3AADB613EBF5}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -9413,9 +9678,9 @@
     <col min="5" max="5" width="13.28515625" style="11" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="15.28515625" style="11" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="15.28515625" style="11" customWidth="1"/>
-    <col min="8" max="8" width="150.7109375" style="15" customWidth="1"/>
-    <col min="9" max="9" width="9.140625" style="15" customWidth="1"/>
-    <col min="10" max="10" width="12.140625" style="15" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="150.7109375" style="16" customWidth="1"/>
+    <col min="9" max="9" width="9.140625" style="16" customWidth="1"/>
+    <col min="10" max="10" width="12.140625" style="16" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="13.85546875" style="11" customWidth="1"/>
     <col min="12" max="12" width="13.85546875" style="12" hidden="1" customWidth="1"/>
     <col min="13" max="13" width="13.85546875" style="11" customWidth="1"/>
@@ -11516,11 +11781,11 @@
         <v>3</v>
       </c>
       <c r="D34">
-        <f t="shared" ref="D34:D61" si="9">E34/60</f>
+        <f t="shared" ref="D34:D65" si="9">E34/60</f>
         <v>0.43746666666666667</v>
       </c>
       <c r="E34">
-        <f t="shared" ref="E34:E61" si="10">F34/1000</f>
+        <f t="shared" ref="E34:E65" si="10">F34/1000</f>
         <v>26.248000000000001</v>
       </c>
       <c r="F34">
@@ -13863,26 +14128,169 @@
     </row>
   </sheetData>
   <mergeCells count="207">
-    <mergeCell ref="H31:I31"/>
-    <mergeCell ref="H12:I12"/>
-    <mergeCell ref="H13:I13"/>
-    <mergeCell ref="H14:I14"/>
-    <mergeCell ref="H15:I15"/>
-    <mergeCell ref="H16:I16"/>
-    <mergeCell ref="H17:I17"/>
-    <mergeCell ref="H18:I18"/>
-    <mergeCell ref="H19:I19"/>
-    <mergeCell ref="H20:I20"/>
-    <mergeCell ref="H21:I21"/>
-    <mergeCell ref="H23:I23"/>
-    <mergeCell ref="H24:I24"/>
-    <mergeCell ref="H22:I22"/>
-    <mergeCell ref="H25:I25"/>
-    <mergeCell ref="H26:I26"/>
-    <mergeCell ref="H27:I27"/>
-    <mergeCell ref="H28:I28"/>
-    <mergeCell ref="H29:I29"/>
-    <mergeCell ref="H30:I30"/>
+    <mergeCell ref="H195:I195"/>
+    <mergeCell ref="H196:I196"/>
+    <mergeCell ref="H197:I197"/>
+    <mergeCell ref="H198:I198"/>
+    <mergeCell ref="H131:I131"/>
+    <mergeCell ref="H132:I132"/>
+    <mergeCell ref="H133:I133"/>
+    <mergeCell ref="H134:I134"/>
+    <mergeCell ref="H135:I135"/>
+    <mergeCell ref="H136:I136"/>
+    <mergeCell ref="H181:I181"/>
+    <mergeCell ref="H182:I182"/>
+    <mergeCell ref="H183:I183"/>
+    <mergeCell ref="H169:I169"/>
+    <mergeCell ref="H167:I167"/>
+    <mergeCell ref="H168:I168"/>
+    <mergeCell ref="H163:I163"/>
+    <mergeCell ref="H164:I164"/>
+    <mergeCell ref="H165:I165"/>
+    <mergeCell ref="H166:I166"/>
+    <mergeCell ref="H146:I146"/>
+    <mergeCell ref="H147:I147"/>
+    <mergeCell ref="H148:I148"/>
+    <mergeCell ref="H151:I151"/>
+    <mergeCell ref="H72:I72"/>
+    <mergeCell ref="H73:I73"/>
+    <mergeCell ref="H74:I74"/>
+    <mergeCell ref="H75:I75"/>
+    <mergeCell ref="H86:I86"/>
+    <mergeCell ref="H87:I87"/>
+    <mergeCell ref="H88:I88"/>
+    <mergeCell ref="H89:I89"/>
+    <mergeCell ref="H76:I76"/>
+    <mergeCell ref="H84:I84"/>
+    <mergeCell ref="H85:I85"/>
+    <mergeCell ref="H77:I77"/>
+    <mergeCell ref="H78:I78"/>
+    <mergeCell ref="H79:I79"/>
+    <mergeCell ref="H80:I80"/>
+    <mergeCell ref="H40:I40"/>
+    <mergeCell ref="H41:I41"/>
+    <mergeCell ref="H42:I42"/>
+    <mergeCell ref="H43:I43"/>
+    <mergeCell ref="H44:I44"/>
+    <mergeCell ref="H45:I45"/>
+    <mergeCell ref="H152:I152"/>
+    <mergeCell ref="H153:I153"/>
+    <mergeCell ref="H154:I154"/>
+    <mergeCell ref="H140:I140"/>
+    <mergeCell ref="H141:I141"/>
+    <mergeCell ref="H142:I142"/>
+    <mergeCell ref="H143:I143"/>
+    <mergeCell ref="H144:I144"/>
+    <mergeCell ref="H145:I145"/>
+    <mergeCell ref="H46:I46"/>
+    <mergeCell ref="H47:I47"/>
+    <mergeCell ref="H48:I48"/>
+    <mergeCell ref="H93:I93"/>
+    <mergeCell ref="H94:I94"/>
+    <mergeCell ref="H95:I95"/>
+    <mergeCell ref="H96:I96"/>
+    <mergeCell ref="H97:I97"/>
+    <mergeCell ref="H98:I98"/>
+    <mergeCell ref="H49:I49"/>
+    <mergeCell ref="H52:I52"/>
+    <mergeCell ref="H53:I53"/>
+    <mergeCell ref="H54:I54"/>
+    <mergeCell ref="H55:I55"/>
+    <mergeCell ref="H56:I56"/>
+    <mergeCell ref="H57:I57"/>
+    <mergeCell ref="H58:I58"/>
+    <mergeCell ref="H59:I59"/>
+    <mergeCell ref="H50:I50"/>
+    <mergeCell ref="H110:I110"/>
+    <mergeCell ref="H111:I111"/>
+    <mergeCell ref="H101:I101"/>
+    <mergeCell ref="H102:I102"/>
+    <mergeCell ref="H103:I103"/>
+    <mergeCell ref="H105:I105"/>
+    <mergeCell ref="H106:I106"/>
+    <mergeCell ref="H107:I107"/>
+    <mergeCell ref="H108:I108"/>
+    <mergeCell ref="H109:I109"/>
+    <mergeCell ref="H104:I104"/>
+    <mergeCell ref="H125:I125"/>
+    <mergeCell ref="H126:I126"/>
+    <mergeCell ref="H127:I127"/>
+    <mergeCell ref="H128:I128"/>
+    <mergeCell ref="H129:I129"/>
+    <mergeCell ref="H121:I121"/>
+    <mergeCell ref="H122:I122"/>
+    <mergeCell ref="H123:I123"/>
+    <mergeCell ref="H124:I124"/>
+    <mergeCell ref="H2:I2"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="H4:I4"/>
+    <mergeCell ref="H5:I5"/>
+    <mergeCell ref="H6:I6"/>
+    <mergeCell ref="H68:I68"/>
+    <mergeCell ref="H69:I69"/>
+    <mergeCell ref="H70:I70"/>
+    <mergeCell ref="H71:I71"/>
+    <mergeCell ref="H63:I63"/>
+    <mergeCell ref="H7:I7"/>
+    <mergeCell ref="H8:I8"/>
+    <mergeCell ref="H9:I9"/>
+    <mergeCell ref="H51:I51"/>
+    <mergeCell ref="H39:I39"/>
+    <mergeCell ref="H37:I37"/>
+    <mergeCell ref="H38:I38"/>
+    <mergeCell ref="H64:I64"/>
+    <mergeCell ref="H65:I65"/>
+    <mergeCell ref="H66:I66"/>
+    <mergeCell ref="H67:I67"/>
+    <mergeCell ref="H62:I62"/>
+    <mergeCell ref="H60:I60"/>
+    <mergeCell ref="H61:I61"/>
+    <mergeCell ref="H10:I10"/>
+    <mergeCell ref="H11:I11"/>
+    <mergeCell ref="H32:I32"/>
+    <mergeCell ref="H33:I33"/>
+    <mergeCell ref="H34:I34"/>
+    <mergeCell ref="H35:I35"/>
+    <mergeCell ref="H36:I36"/>
+    <mergeCell ref="H120:I120"/>
+    <mergeCell ref="H81:I81"/>
+    <mergeCell ref="H82:I82"/>
+    <mergeCell ref="H83:I83"/>
+    <mergeCell ref="H90:I90"/>
+    <mergeCell ref="H91:I91"/>
+    <mergeCell ref="H92:I92"/>
+    <mergeCell ref="H99:I99"/>
+    <mergeCell ref="H100:I100"/>
+    <mergeCell ref="H116:I116"/>
+    <mergeCell ref="H117:I117"/>
+    <mergeCell ref="H118:I118"/>
+    <mergeCell ref="H119:I119"/>
+    <mergeCell ref="H112:I112"/>
+    <mergeCell ref="H113:I113"/>
+    <mergeCell ref="H114:I114"/>
+    <mergeCell ref="H115:I115"/>
+    <mergeCell ref="H174:I174"/>
+    <mergeCell ref="H175:I175"/>
+    <mergeCell ref="H176:I176"/>
+    <mergeCell ref="H177:I177"/>
+    <mergeCell ref="H173:I173"/>
+    <mergeCell ref="H130:I130"/>
+    <mergeCell ref="H170:I170"/>
+    <mergeCell ref="H171:I171"/>
+    <mergeCell ref="H172:I172"/>
+    <mergeCell ref="H137:I137"/>
+    <mergeCell ref="H138:I138"/>
+    <mergeCell ref="H139:I139"/>
+    <mergeCell ref="H158:I158"/>
+    <mergeCell ref="H159:I159"/>
+    <mergeCell ref="H160:I160"/>
+    <mergeCell ref="H161:I161"/>
+    <mergeCell ref="H162:I162"/>
+    <mergeCell ref="H149:I149"/>
+    <mergeCell ref="H150:I150"/>
+    <mergeCell ref="H155:I155"/>
+    <mergeCell ref="H156:I156"/>
+    <mergeCell ref="H157:I157"/>
     <mergeCell ref="H205:I205"/>
     <mergeCell ref="H206:I206"/>
     <mergeCell ref="H207:I207"/>
@@ -13907,169 +14315,26 @@
     <mergeCell ref="H192:I192"/>
     <mergeCell ref="H193:I193"/>
     <mergeCell ref="H194:I194"/>
-    <mergeCell ref="H174:I174"/>
-    <mergeCell ref="H175:I175"/>
-    <mergeCell ref="H176:I176"/>
-    <mergeCell ref="H177:I177"/>
-    <mergeCell ref="H173:I173"/>
-    <mergeCell ref="H130:I130"/>
-    <mergeCell ref="H170:I170"/>
-    <mergeCell ref="H171:I171"/>
-    <mergeCell ref="H172:I172"/>
-    <mergeCell ref="H137:I137"/>
-    <mergeCell ref="H138:I138"/>
-    <mergeCell ref="H139:I139"/>
-    <mergeCell ref="H158:I158"/>
-    <mergeCell ref="H159:I159"/>
-    <mergeCell ref="H160:I160"/>
-    <mergeCell ref="H161:I161"/>
-    <mergeCell ref="H162:I162"/>
-    <mergeCell ref="H149:I149"/>
-    <mergeCell ref="H150:I150"/>
-    <mergeCell ref="H155:I155"/>
-    <mergeCell ref="H156:I156"/>
-    <mergeCell ref="H157:I157"/>
-    <mergeCell ref="H10:I10"/>
-    <mergeCell ref="H11:I11"/>
-    <mergeCell ref="H32:I32"/>
-    <mergeCell ref="H33:I33"/>
-    <mergeCell ref="H34:I34"/>
-    <mergeCell ref="H35:I35"/>
-    <mergeCell ref="H36:I36"/>
-    <mergeCell ref="H120:I120"/>
-    <mergeCell ref="H81:I81"/>
-    <mergeCell ref="H82:I82"/>
-    <mergeCell ref="H83:I83"/>
-    <mergeCell ref="H90:I90"/>
-    <mergeCell ref="H91:I91"/>
-    <mergeCell ref="H92:I92"/>
-    <mergeCell ref="H99:I99"/>
-    <mergeCell ref="H100:I100"/>
-    <mergeCell ref="H116:I116"/>
-    <mergeCell ref="H117:I117"/>
-    <mergeCell ref="H118:I118"/>
-    <mergeCell ref="H119:I119"/>
-    <mergeCell ref="H112:I112"/>
-    <mergeCell ref="H113:I113"/>
-    <mergeCell ref="H114:I114"/>
-    <mergeCell ref="H115:I115"/>
-    <mergeCell ref="H2:I2"/>
-    <mergeCell ref="H3:I3"/>
-    <mergeCell ref="H4:I4"/>
-    <mergeCell ref="H5:I5"/>
-    <mergeCell ref="H6:I6"/>
-    <mergeCell ref="H68:I68"/>
-    <mergeCell ref="H69:I69"/>
-    <mergeCell ref="H70:I70"/>
-    <mergeCell ref="H71:I71"/>
-    <mergeCell ref="H63:I63"/>
-    <mergeCell ref="H7:I7"/>
-    <mergeCell ref="H8:I8"/>
-    <mergeCell ref="H9:I9"/>
-    <mergeCell ref="H51:I51"/>
-    <mergeCell ref="H39:I39"/>
-    <mergeCell ref="H37:I37"/>
-    <mergeCell ref="H38:I38"/>
-    <mergeCell ref="H64:I64"/>
-    <mergeCell ref="H65:I65"/>
-    <mergeCell ref="H66:I66"/>
-    <mergeCell ref="H67:I67"/>
-    <mergeCell ref="H62:I62"/>
-    <mergeCell ref="H60:I60"/>
-    <mergeCell ref="H61:I61"/>
-    <mergeCell ref="H125:I125"/>
-    <mergeCell ref="H126:I126"/>
-    <mergeCell ref="H127:I127"/>
-    <mergeCell ref="H128:I128"/>
-    <mergeCell ref="H129:I129"/>
-    <mergeCell ref="H121:I121"/>
-    <mergeCell ref="H122:I122"/>
-    <mergeCell ref="H123:I123"/>
-    <mergeCell ref="H124:I124"/>
-    <mergeCell ref="H110:I110"/>
-    <mergeCell ref="H111:I111"/>
-    <mergeCell ref="H101:I101"/>
-    <mergeCell ref="H102:I102"/>
-    <mergeCell ref="H103:I103"/>
-    <mergeCell ref="H105:I105"/>
-    <mergeCell ref="H106:I106"/>
-    <mergeCell ref="H107:I107"/>
-    <mergeCell ref="H108:I108"/>
-    <mergeCell ref="H109:I109"/>
-    <mergeCell ref="H104:I104"/>
-    <mergeCell ref="H49:I49"/>
-    <mergeCell ref="H52:I52"/>
-    <mergeCell ref="H53:I53"/>
-    <mergeCell ref="H54:I54"/>
-    <mergeCell ref="H55:I55"/>
-    <mergeCell ref="H56:I56"/>
-    <mergeCell ref="H57:I57"/>
-    <mergeCell ref="H58:I58"/>
-    <mergeCell ref="H59:I59"/>
-    <mergeCell ref="H50:I50"/>
-    <mergeCell ref="H40:I40"/>
-    <mergeCell ref="H41:I41"/>
-    <mergeCell ref="H42:I42"/>
-    <mergeCell ref="H43:I43"/>
-    <mergeCell ref="H44:I44"/>
-    <mergeCell ref="H45:I45"/>
-    <mergeCell ref="H152:I152"/>
-    <mergeCell ref="H153:I153"/>
-    <mergeCell ref="H154:I154"/>
-    <mergeCell ref="H140:I140"/>
-    <mergeCell ref="H141:I141"/>
-    <mergeCell ref="H142:I142"/>
-    <mergeCell ref="H143:I143"/>
-    <mergeCell ref="H144:I144"/>
-    <mergeCell ref="H145:I145"/>
-    <mergeCell ref="H46:I46"/>
-    <mergeCell ref="H47:I47"/>
-    <mergeCell ref="H48:I48"/>
-    <mergeCell ref="H93:I93"/>
-    <mergeCell ref="H94:I94"/>
-    <mergeCell ref="H95:I95"/>
-    <mergeCell ref="H96:I96"/>
-    <mergeCell ref="H97:I97"/>
-    <mergeCell ref="H98:I98"/>
-    <mergeCell ref="H72:I72"/>
-    <mergeCell ref="H73:I73"/>
-    <mergeCell ref="H74:I74"/>
-    <mergeCell ref="H75:I75"/>
-    <mergeCell ref="H86:I86"/>
-    <mergeCell ref="H87:I87"/>
-    <mergeCell ref="H88:I88"/>
-    <mergeCell ref="H89:I89"/>
-    <mergeCell ref="H76:I76"/>
-    <mergeCell ref="H84:I84"/>
-    <mergeCell ref="H85:I85"/>
-    <mergeCell ref="H77:I77"/>
-    <mergeCell ref="H78:I78"/>
-    <mergeCell ref="H79:I79"/>
-    <mergeCell ref="H80:I80"/>
-    <mergeCell ref="H195:I195"/>
-    <mergeCell ref="H196:I196"/>
-    <mergeCell ref="H197:I197"/>
-    <mergeCell ref="H198:I198"/>
-    <mergeCell ref="H131:I131"/>
-    <mergeCell ref="H132:I132"/>
-    <mergeCell ref="H133:I133"/>
-    <mergeCell ref="H134:I134"/>
-    <mergeCell ref="H135:I135"/>
-    <mergeCell ref="H136:I136"/>
-    <mergeCell ref="H181:I181"/>
-    <mergeCell ref="H182:I182"/>
-    <mergeCell ref="H183:I183"/>
-    <mergeCell ref="H169:I169"/>
-    <mergeCell ref="H167:I167"/>
-    <mergeCell ref="H168:I168"/>
-    <mergeCell ref="H163:I163"/>
-    <mergeCell ref="H164:I164"/>
-    <mergeCell ref="H165:I165"/>
-    <mergeCell ref="H166:I166"/>
-    <mergeCell ref="H146:I146"/>
-    <mergeCell ref="H147:I147"/>
-    <mergeCell ref="H148:I148"/>
-    <mergeCell ref="H151:I151"/>
+    <mergeCell ref="H31:I31"/>
+    <mergeCell ref="H12:I12"/>
+    <mergeCell ref="H13:I13"/>
+    <mergeCell ref="H14:I14"/>
+    <mergeCell ref="H15:I15"/>
+    <mergeCell ref="H16:I16"/>
+    <mergeCell ref="H17:I17"/>
+    <mergeCell ref="H18:I18"/>
+    <mergeCell ref="H19:I19"/>
+    <mergeCell ref="H20:I20"/>
+    <mergeCell ref="H21:I21"/>
+    <mergeCell ref="H23:I23"/>
+    <mergeCell ref="H24:I24"/>
+    <mergeCell ref="H22:I22"/>
+    <mergeCell ref="H25:I25"/>
+    <mergeCell ref="H26:I26"/>
+    <mergeCell ref="H27:I27"/>
+    <mergeCell ref="H28:I28"/>
+    <mergeCell ref="H29:I29"/>
+    <mergeCell ref="H30:I30"/>
   </mergeCells>
   <conditionalFormatting sqref="R2:R61 R63:R1048576">
     <cfRule type="cellIs" dxfId="15" priority="21" operator="notBetween">
@@ -14150,7 +14415,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C2" sqref="C2"/>
+      <selection pane="bottomLeft" activeCell="M31" sqref="M31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14178,40 +14443,40 @@
         <v>209</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>295</v>
+        <v>210</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="F1" s="5" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="G1" s="5" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="H1" s="5" t="s">
         <v>7</v>
       </c>
       <c r="I1" s="5" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="J1" s="5" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="K1" s="5" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="L1" s="5" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="M1" s="5" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="N1" s="5" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
@@ -14219,13 +14484,13 @@
         <v>43745</v>
       </c>
       <c r="B2" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="D2">
         <v>469154.88979999977</v>
       </c>
       <c r="G2" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="H2">
         <v>3603.7618333999999</v>
@@ -14238,7 +14503,7 @@
         <v>13622.672333333176</v>
       </c>
       <c r="L2" s="12">
-        <f t="shared" ref="L2:L27" si="0">K2/D2</f>
+        <f t="shared" ref="L2:L30" si="0">K2/D2</f>
         <v>2.9036620164271349E-2</v>
       </c>
     </row>
@@ -14247,13 +14512,13 @@
         <v>43768</v>
       </c>
       <c r="B3" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="D3">
         <v>592286.43533333309</v>
       </c>
       <c r="G3" s="7" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="H3">
         <v>3600.6243162000001</v>
@@ -14270,7 +14535,7 @@
         <v>-2.8570731981184649E-2</v>
       </c>
       <c r="M3" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
@@ -14278,16 +14543,16 @@
         <v>43775</v>
       </c>
       <c r="B4" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="D4">
         <v>471229.1394000001</v>
       </c>
       <c r="F4" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="G4" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="H4">
         <v>3893.4923675999999</v>
@@ -14296,7 +14561,7 @@
         <v>468885.14206666662</v>
       </c>
       <c r="K4">
-        <f t="shared" ref="K4:K27" si="1">D4-(I4+J4*10)</f>
+        <f t="shared" ref="K4:K30" si="1">D4-(I4+J4*10)</f>
         <v>2343.9973333334783</v>
       </c>
       <c r="L4" s="12">
@@ -14309,16 +14574,16 @@
         <v>43775</v>
       </c>
       <c r="B5" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="D5">
         <v>1428685.831666667</v>
       </c>
       <c r="F5" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="G5" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="H5">
         <v>3661.4549959999999</v>
@@ -14335,7 +14600,7 @@
         <v>0.11307985414694049</v>
       </c>
       <c r="M5" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
@@ -14343,16 +14608,16 @@
         <v>43768</v>
       </c>
       <c r="B6" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="D6">
         <v>592286.43533333309</v>
       </c>
       <c r="F6" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="G6" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="H6">
         <v>3786.4904317999999</v>
@@ -14374,16 +14639,16 @@
         <v>43745</v>
       </c>
       <c r="B7" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="D7">
         <v>469154.88979999977</v>
       </c>
       <c r="F7" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="G7" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="H7">
         <v>3601.0539597000002</v>
@@ -14405,16 +14670,16 @@
         <v>43795</v>
       </c>
       <c r="B8" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="D8">
         <v>1275847.0800666669</v>
       </c>
       <c r="F8" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="G8" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="H8">
         <v>3902.6114637000001</v>
@@ -14436,16 +14701,16 @@
         <v>43768</v>
       </c>
       <c r="B9" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="D9">
         <v>592286.43533333309</v>
       </c>
       <c r="F9" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="G9" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="H9">
         <v>7200.1489792000002</v>
@@ -14467,16 +14732,16 @@
         <v>43745</v>
       </c>
       <c r="B10" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="D10">
         <v>475403.35446666653</v>
       </c>
       <c r="F10" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="G10" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="H10">
         <v>3601.0659418</v>
@@ -14493,7 +14758,7 @@
         <v>0.12671645898302314</v>
       </c>
       <c r="M10" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
@@ -14501,16 +14766,16 @@
         <v>43768</v>
       </c>
       <c r="B11" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="D11">
         <v>600912.63166666601</v>
       </c>
       <c r="F11" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="G11" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="H11">
         <v>3600.2064667</v>
@@ -14532,16 +14797,16 @@
         <v>43745</v>
       </c>
       <c r="B12" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="D12">
         <v>494345.58179999999</v>
       </c>
       <c r="F12" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="G12" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="H12">
         <v>7170.8296077000005</v>
@@ -14558,7 +14823,7 @@
         <v>6.5150951451266648E-2</v>
       </c>
       <c r="M12" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
@@ -14566,16 +14831,16 @@
         <v>43768</v>
       </c>
       <c r="B13" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="D13">
         <v>593149.57433333329</v>
       </c>
       <c r="F13" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="G13" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="H13">
         <v>5056.3446751000001</v>
@@ -14597,16 +14862,16 @@
         <v>43795</v>
       </c>
       <c r="B14" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="D14">
         <v>1372973.317933334</v>
       </c>
       <c r="F14" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="G14" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="H14">
         <v>7318.0830248000002</v>
@@ -14628,16 +14893,16 @@
         <v>43754</v>
       </c>
       <c r="B15" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="D15">
         <v>636315.92813333333</v>
       </c>
       <c r="F15" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="G15" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="H15">
         <v>4347.3198690999998</v>
@@ -14659,16 +14924,16 @@
         <v>43745</v>
       </c>
       <c r="B16" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="D16">
         <v>538213.87013333349</v>
       </c>
       <c r="F16" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="G16" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="H16">
         <v>7527.1272962000003</v>
@@ -14685,7 +14950,7 @@
         <v>0.13716106668719871</v>
       </c>
       <c r="M16" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.25">
@@ -14693,16 +14958,16 @@
         <v>43768</v>
       </c>
       <c r="B17" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="D17">
         <v>632705.85299999989</v>
       </c>
       <c r="F17" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="G17" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="H17">
         <v>6666.2375192999998</v>
@@ -14724,16 +14989,16 @@
         <v>43795</v>
       </c>
       <c r="B18" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="D18">
         <v>1432583.6294</v>
       </c>
       <c r="F18" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="G18" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="H18">
         <v>7733.803919</v>
@@ -14755,16 +15020,16 @@
         <v>43745</v>
       </c>
       <c r="B19" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="D19">
         <v>496052.98146666668</v>
       </c>
       <c r="F19" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="G19" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="H19">
         <v>7561.5297926000003</v>
@@ -14781,7 +15046,7 @@
         <v>6.2898892186371402E-2</v>
       </c>
       <c r="M19" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.25">
@@ -14789,16 +15054,16 @@
         <v>43768</v>
       </c>
       <c r="B20" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="D20">
         <v>595195.38266666664</v>
       </c>
       <c r="F20" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="G20" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="H20">
         <v>3968.0924328999999</v>
@@ -14820,16 +15085,16 @@
         <v>43795</v>
       </c>
       <c r="B21" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="D21">
         <v>1381861.7179333339</v>
       </c>
       <c r="F21" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="G21" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="H21">
         <v>7200.6445293999996</v>
@@ -14851,16 +15116,16 @@
         <v>43745</v>
       </c>
       <c r="B22" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="D22">
         <v>496052.98146666668</v>
       </c>
       <c r="F22" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="G22" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="H22">
         <v>3601.0062647</v>
@@ -14877,7 +15142,7 @@
         <v>6.3194700642623072E-2</v>
       </c>
       <c r="M22" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.25">
@@ -14885,16 +15150,16 @@
         <v>43768</v>
       </c>
       <c r="B23" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="D23">
         <v>595195.38266666664</v>
       </c>
       <c r="F23" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="G23" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="H23">
         <v>3600.8390132</v>
@@ -14916,16 +15181,16 @@
         <v>43795</v>
       </c>
       <c r="B24" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="D24">
         <v>1381861.7179333339</v>
       </c>
       <c r="F24" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="G24" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="H24">
         <v>3601.3254473000002</v>
@@ -14947,25 +15212,25 @@
         <v>43745</v>
       </c>
       <c r="B25" t="s">
-        <v>271</v>
-      </c>
-      <c r="D25" s="16">
+        <v>272</v>
+      </c>
+      <c r="D25" s="15">
         <v>496052.98146666668</v>
       </c>
       <c r="F25" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="G25" t="s">
-        <v>288</v>
-      </c>
-      <c r="H25" s="16">
+        <v>289</v>
+      </c>
+      <c r="H25" s="15">
         <v>7048.7007022999996</v>
       </c>
-      <c r="I25" s="16">
+      <c r="I25" s="15">
         <v>448073.09313333308</v>
       </c>
-      <c r="J25" s="16"/>
-      <c r="K25" s="16">
+      <c r="J25" s="15"/>
+      <c r="K25" s="15">
         <f t="shared" si="1"/>
         <v>47979.888333333598</v>
       </c>
@@ -14974,7 +15239,7 @@
         <v>9.6723314093330792E-2</v>
       </c>
       <c r="M25" t="s">
-        <v>294</v>
+        <v>290</v>
       </c>
       <c r="N25">
         <v>83</v>
@@ -14985,25 +15250,25 @@
         <v>43768</v>
       </c>
       <c r="B26" t="s">
-        <v>275</v>
-      </c>
-      <c r="D26" s="16">
+        <v>276</v>
+      </c>
+      <c r="D26" s="15">
         <v>595195.38266666664</v>
       </c>
       <c r="F26" t="s">
-        <v>289</v>
+        <v>291</v>
       </c>
       <c r="G26" t="s">
-        <v>290</v>
-      </c>
-      <c r="H26" s="16">
+        <v>292</v>
+      </c>
+      <c r="H26" s="15">
         <v>7200.4963602999997</v>
       </c>
-      <c r="I26" s="16">
+      <c r="I26" s="15">
         <v>559057.74033333291</v>
       </c>
-      <c r="J26" s="16"/>
-      <c r="K26" s="16">
+      <c r="J26" s="15"/>
+      <c r="K26" s="15">
         <f t="shared" si="1"/>
         <v>36137.64233333373</v>
       </c>
@@ -15020,25 +15285,25 @@
         <v>43795</v>
       </c>
       <c r="B27" t="s">
-        <v>291</v>
-      </c>
-      <c r="D27" s="16">
+        <v>293</v>
+      </c>
+      <c r="D27" s="15">
         <v>1381861.7179333339</v>
       </c>
       <c r="F27" t="s">
-        <v>292</v>
+        <v>294</v>
       </c>
       <c r="G27" t="s">
-        <v>293</v>
-      </c>
-      <c r="H27" s="16">
+        <v>295</v>
+      </c>
+      <c r="H27" s="15">
         <v>7888.9231545000002</v>
       </c>
-      <c r="I27" s="16">
+      <c r="I27" s="15">
         <v>1204977.810166667</v>
       </c>
-      <c r="J27" s="16"/>
-      <c r="K27" s="16">
+      <c r="J27" s="15"/>
+      <c r="K27" s="15">
         <f t="shared" si="1"/>
         <v>176883.90776666696</v>
       </c>
@@ -15051,21 +15316,116 @@
       </c>
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B28"/>
-      <c r="D28"/>
+      <c r="A28" s="9">
+        <v>43745</v>
+      </c>
+      <c r="B28" t="s">
+        <v>272</v>
+      </c>
+      <c r="D28">
+        <v>588323.39749999973</v>
+      </c>
+      <c r="F28" t="s">
+        <v>296</v>
+      </c>
+      <c r="G28" t="s">
+        <v>297</v>
+      </c>
+      <c r="H28">
+        <v>6176.4342452999999</v>
+      </c>
+      <c r="I28">
+        <v>541168.93666666653</v>
+      </c>
+      <c r="K28" s="15">
+        <f t="shared" si="1"/>
+        <v>47154.4608333332</v>
+      </c>
+      <c r="L28" s="12">
+        <f t="shared" si="0"/>
+        <v>8.0150578803613232E-2</v>
+      </c>
+      <c r="M28" t="s">
+        <v>298</v>
+      </c>
+      <c r="N28">
+        <v>81</v>
+      </c>
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="L29" s="12"/>
+      <c r="A29" s="10">
+        <v>43768</v>
+      </c>
+      <c r="B29" t="s">
+        <v>276</v>
+      </c>
+      <c r="D29">
+        <v>692416.29500000016</v>
+      </c>
+      <c r="F29" t="s">
+        <v>299</v>
+      </c>
+      <c r="G29" t="s">
+        <v>300</v>
+      </c>
+      <c r="H29">
+        <v>7200.3923278000002</v>
+      </c>
+      <c r="I29">
+        <v>661103.9565833332</v>
+      </c>
+      <c r="K29" s="15">
+        <f t="shared" si="1"/>
+        <v>31312.338416666957</v>
+      </c>
+      <c r="L29" s="12">
+        <f t="shared" si="0"/>
+        <v>4.5221839293465717E-2</v>
+      </c>
+      <c r="N29">
+        <v>123</v>
+      </c>
     </row>
     <row r="30" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="L30" s="12"/>
+      <c r="A30" s="8">
+        <v>43795</v>
+      </c>
+      <c r="B30" t="s">
+        <v>293</v>
+      </c>
+      <c r="D30">
+        <v>1565696.622916667</v>
+      </c>
+      <c r="F30" t="s">
+        <v>301</v>
+      </c>
+      <c r="G30" t="s">
+        <v>302</v>
+      </c>
+      <c r="H30">
+        <v>7200.5053572999996</v>
+      </c>
+      <c r="I30">
+        <v>1410468.586666666</v>
+      </c>
+      <c r="K30" s="15">
+        <f t="shared" si="1"/>
+        <v>155228.03625000105</v>
+      </c>
+      <c r="L30" s="12">
+        <f t="shared" si="0"/>
+        <v>9.9143112387145349E-2</v>
+      </c>
+      <c r="N30">
+        <v>165</v>
+      </c>
     </row>
     <row r="31" spans="1:14" x14ac:dyDescent="0.25">
       <c r="L31" s="12"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:A28" xr:uid="{00000000-0009-0000-0000-000002000000}"/>
-  <conditionalFormatting sqref="L1:L28 L32:L1048576 M1:N1">
+  <conditionalFormatting sqref="L32:L1048576 M1:N1 L1:L30">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>

</xml_diff>

<commit_message>
Added function that checks whether a solution meets all mathematical model constraints
</commit_message>
<xml_diff>
--- a/vrp_case_study/Solve Times Summary.xlsx
+++ b/vrp_case_study/Solve Times Summary.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="600" firstSheet="0" activeTab="1" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="28680" yWindow="3615" windowWidth="20730" windowHeight="11160" tabRatio="600" firstSheet="0" activeTab="1" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="Graphs" sheetId="1" state="visible" r:id="rId1"/>
@@ -106,7 +106,7 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left"/>
@@ -122,20 +122,19 @@
     <xf numFmtId="15" fontId="4" fillId="3" borderId="0" pivotButton="0" quotePrefix="0" xfId="3"/>
     <xf numFmtId="15" fontId="3" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="2"/>
     <xf numFmtId="15" fontId="5" fillId="4" borderId="0" pivotButton="0" quotePrefix="0" xfId="4"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="10" fontId="2" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -144,171 +143,7 @@
     <cellStyle name="Bad" xfId="3" builtinId="27"/>
     <cellStyle name="Neutral" xfId="4" builtinId="28"/>
   </cellStyles>
-  <dxfs count="58">
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF6D6D"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF6D6D"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="17">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -346,234 +181,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF6D6D"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF6D6D"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF6D6D"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF6D6D"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -908,7 +515,7 @@
                   <v>61.30619999999999</v>
                 </pt>
                 <pt idx="2">
-                  <v>187.2671</v>
+                  <v>1041.7548</v>
                 </pt>
               </numCache>
             </numRef>
@@ -1228,13 +835,13 @@
                 <formatCode>General</formatCode>
                 <ptCount val="3"/>
                 <pt idx="0">
-                  <v>172.95837812</v>
+                  <v>169.40622469</v>
                 </pt>
                 <pt idx="1">
-                  <v>265.35310027</v>
+                  <v>280.6807104100001</v>
                 </pt>
                 <pt idx="2">
-                  <v>364.21926135</v>
+                  <v>357.49913709</v>
                 </pt>
               </numCache>
             </numRef>
@@ -1296,13 +903,13 @@
                 <formatCode>General</formatCode>
                 <ptCount val="3"/>
                 <pt idx="0">
-                  <v>209.98448915</v>
+                  <v>199.6632517100001</v>
                 </pt>
                 <pt idx="1">
-                  <v>310.78821514</v>
+                  <v>301.29726425</v>
                 </pt>
                 <pt idx="2">
-                  <v>559.6389866999999</v>
+                  <v>558.38841605</v>
                 </pt>
               </numCache>
             </numRef>
@@ -1622,13 +1229,13 @@
                 <formatCode>0.00%</formatCode>
                 <ptCount val="3"/>
                 <pt idx="0">
-                  <v>0.0046</v>
+                  <v>0.004973</v>
                 </pt>
                 <pt idx="1">
-                  <v>0.00932</v>
+                  <v>0.004569999999999999</v>
                 </pt>
                 <pt idx="2">
-                  <v>0.003628999999999999</v>
+                  <v>0.004892</v>
                 </pt>
               </numCache>
             </numRef>
@@ -1693,7 +1300,7 @@
                   <v>-0.005195</v>
                 </pt>
                 <pt idx="1">
-                  <v>0.010691</v>
+                  <v>0.008452000000000001</v>
                 </pt>
                 <pt idx="2">
                   <v>0</v>
@@ -2003,10 +1610,10 @@
                 <formatCode>0</formatCode>
                 <ptCount val="3"/>
                 <pt idx="0">
-                  <v>8</v>
+                  <v>9</v>
                 </pt>
                 <pt idx="1">
-                  <v>8</v>
+                  <v>9</v>
                 </pt>
                 <pt idx="2">
                   <v>7</v>
@@ -2060,7 +1667,7 @@
                   <v>5</v>
                 </pt>
                 <pt idx="1">
-                  <v>4</v>
+                  <v>8</v>
                 </pt>
                 <pt idx="2">
                   <v>0</v>
@@ -2762,13 +2369,13 @@
                 <formatCode>General</formatCode>
                 <ptCount val="3"/>
                 <pt idx="0">
-                  <v>172.95837812</v>
+                  <v>169.40622469</v>
                 </pt>
                 <pt idx="1">
-                  <v>265.35310027</v>
+                  <v>280.6807104100001</v>
                 </pt>
                 <pt idx="2">
-                  <v>364.21926135</v>
+                  <v>357.49913709</v>
                 </pt>
               </numCache>
             </numRef>
@@ -2830,13 +2437,13 @@
                 <formatCode>General</formatCode>
                 <ptCount val="3"/>
                 <pt idx="0">
-                  <v>209.98448915</v>
+                  <v>199.6632517100001</v>
                 </pt>
                 <pt idx="1">
-                  <v>310.78821514</v>
+                  <v>301.29726425</v>
                 </pt>
                 <pt idx="2">
-                  <v>559.6389866999999</v>
+                  <v>558.38841605</v>
                 </pt>
               </numCache>
             </numRef>
@@ -2934,7 +2541,7 @@
                   <v>61.30619999999999</v>
                 </pt>
                 <pt idx="2">
-                  <v>187.2671</v>
+                  <v>1041.7548</v>
                 </pt>
               </numCache>
             </numRef>
@@ -3670,18 +3277,18 @@
   <dimension ref="A1:K7"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L7" sqref="L7"/>
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="8" bestFit="1" customWidth="1" style="18" min="1" max="1"/>
-    <col width="10" bestFit="1" customWidth="1" style="18" min="2" max="2"/>
-    <col width="16" bestFit="1" customWidth="1" style="18" min="3" max="3"/>
-    <col width="12.140625" bestFit="1" customWidth="1" style="18" min="4" max="4"/>
-    <col width="12.42578125" bestFit="1" customWidth="1" style="18" min="5" max="5"/>
-    <col width="9.5703125" customWidth="1" style="18" min="7" max="7"/>
-    <col width="9.42578125" customWidth="1" style="18" min="8" max="8"/>
+    <col width="8" bestFit="1" customWidth="1" style="15" min="1" max="1"/>
+    <col width="10" bestFit="1" customWidth="1" style="15" min="2" max="2"/>
+    <col width="16" bestFit="1" customWidth="1" style="15" min="3" max="3"/>
+    <col width="12.140625" bestFit="1" customWidth="1" style="15" min="4" max="4"/>
+    <col width="12.42578125" bestFit="1" customWidth="1" style="15" min="5" max="5"/>
+    <col width="9.5703125" customWidth="1" style="15" min="7" max="7"/>
+    <col width="9.42578125" customWidth="1" style="15" min="8" max="8"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="1" s="5">
@@ -3766,7 +3373,7 @@
         <f>_xlfn.STDEV.S(OFFSET('Run Data'!$E$2, (ROWS(Graphs!F$1:F2)-2)*10,0,10,1))</f>
         <v/>
       </c>
-      <c r="G2" s="12">
+      <c r="G2" s="11">
         <f>AVERAGE(OFFSET('Run Data'!$M$2, (ROWS(Graphs!G$1:G2)-2)*10,0,10,1))</f>
         <v/>
       </c>
@@ -3812,7 +3419,7 @@
         <f>_xlfn.STDEV.S(OFFSET('Run Data'!$E$2, (ROWS(Graphs!F$1:F3)-2)*10,0,10,1))</f>
         <v/>
       </c>
-      <c r="G3" s="12">
+      <c r="G3" s="11">
         <f>AVERAGE(OFFSET('Run Data'!$M$2, (ROWS(Graphs!G$1:G3)-2)*10,0,10,1))</f>
         <v/>
       </c>
@@ -3858,7 +3465,7 @@
         <f>_xlfn.STDEV.S(OFFSET('Run Data'!$E$2, (ROWS(Graphs!F$1:F4)-2)*10,0,10,1))</f>
         <v/>
       </c>
-      <c r="G4" s="12">
+      <c r="G4" s="11">
         <f>AVERAGE(OFFSET('Run Data'!$M$2, (ROWS(Graphs!G$1:G4)-2)*10,0,10,1))</f>
         <v/>
       </c>
@@ -3904,7 +3511,7 @@
         <f>_xlfn.STDEV.S(OFFSET('Run Data'!$E$2, (ROWS(Graphs!F$1:F5)-2)*10,0,10,1))</f>
         <v/>
       </c>
-      <c r="G5" s="12">
+      <c r="G5" s="11">
         <f>AVERAGE(OFFSET('Run Data'!$M$2, (ROWS(Graphs!G$1:G5)-2)*10,0,10,1))</f>
         <v/>
       </c>
@@ -3950,7 +3557,7 @@
         <f>_xlfn.STDEV.S(OFFSET('Run Data'!$E$2, (ROWS(Graphs!F$1:F6)-2)*10,0,10,1))</f>
         <v/>
       </c>
-      <c r="G6" s="12">
+      <c r="G6" s="11">
         <f>AVERAGE(OFFSET('Run Data'!$M$2, (ROWS(Graphs!G$1:G6)-2)*10,0,10,1))</f>
         <v/>
       </c>
@@ -3996,7 +3603,7 @@
         <f>_xlfn.STDEV.S(OFFSET('Run Data'!$E$2, (ROWS(Graphs!F$1:F7)-2)*10,0,10,1))</f>
         <v/>
       </c>
-      <c r="G7" s="12">
+      <c r="G7" s="11">
         <f>AVERAGE(OFFSET('Run Data'!$M$2, (ROWS(Graphs!G$1:G7)-2)*10,0,10,1))</f>
         <v/>
       </c>
@@ -4026,7 +3633,7 @@
     <cfRule type="cellIs" priority="2" operator="greaterThan" dxfId="4">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" priority="3" operator="lessThan" dxfId="0">
+    <cfRule type="cellIs" priority="3" operator="lessThan" dxfId="3">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4045,35 +3652,35 @@
   <dimension ref="A1:W208"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="I2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C50" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="R24" sqref="R24"/>
+      <selection pane="bottomRight" activeCell="F63" sqref="F63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="8" bestFit="1" customWidth="1" style="18" min="1" max="1"/>
-    <col width="10" customWidth="1" style="18" min="2" max="2"/>
-    <col width="5.85546875" bestFit="1" customWidth="1" style="18" min="3" max="3"/>
-    <col width="14.140625" bestFit="1" customWidth="1" style="18" min="4" max="4"/>
-    <col width="13.28515625" bestFit="1" customWidth="1" style="18" min="5" max="5"/>
-    <col width="15.28515625" bestFit="1" customWidth="1" style="18" min="6" max="6"/>
-    <col width="15.28515625" customWidth="1" style="18" min="7" max="7"/>
+    <col width="8" bestFit="1" customWidth="1" style="15" min="1" max="1"/>
+    <col width="10" customWidth="1" style="15" min="2" max="2"/>
+    <col width="5.85546875" bestFit="1" customWidth="1" style="15" min="3" max="3"/>
+    <col width="14.140625" bestFit="1" customWidth="1" style="15" min="4" max="4"/>
+    <col width="13.28515625" bestFit="1" customWidth="1" style="15" min="5" max="5"/>
+    <col width="15.28515625" bestFit="1" customWidth="1" style="15" min="6" max="6"/>
+    <col width="15.28515625" customWidth="1" style="15" min="7" max="7"/>
     <col width="150.7109375" customWidth="1" style="17" min="8" max="8"/>
     <col width="9.140625" customWidth="1" style="17" min="9" max="9"/>
     <col width="12.140625" bestFit="1" customWidth="1" style="17" min="10" max="10"/>
-    <col width="13.85546875" customWidth="1" style="18" min="11" max="11"/>
-    <col hidden="1" width="13.85546875" customWidth="1" style="12" min="12" max="12"/>
-    <col width="13.85546875" customWidth="1" style="18" min="13" max="14"/>
-    <col width="13.28515625" customWidth="1" style="18" min="15" max="15"/>
-    <col width="16" bestFit="1" customWidth="1" style="18" min="16" max="16"/>
-    <col width="14.85546875" bestFit="1" customWidth="1" style="18" min="17" max="17"/>
-    <col width="19.28515625" customWidth="1" style="18" min="18" max="18"/>
-    <col width="14.140625" customWidth="1" style="18" min="19" max="19"/>
-    <col width="13.5703125" bestFit="1" customWidth="1" style="18" min="20" max="20"/>
-    <col width="14.5703125" bestFit="1" customWidth="1" style="18" min="21" max="22"/>
-    <col width="14.140625" customWidth="1" style="18" min="23" max="23"/>
+    <col width="13.85546875" customWidth="1" style="15" min="11" max="11"/>
+    <col hidden="1" width="13.85546875" customWidth="1" style="11" min="12" max="12"/>
+    <col width="13.85546875" customWidth="1" style="15" min="13" max="14"/>
+    <col width="13.28515625" customWidth="1" style="15" min="15" max="15"/>
+    <col width="16" bestFit="1" customWidth="1" style="15" min="16" max="16"/>
+    <col width="14.85546875" bestFit="1" customWidth="1" style="15" min="17" max="17"/>
+    <col width="19.28515625" customWidth="1" style="15" min="18" max="18"/>
+    <col width="14.140625" customWidth="1" style="15" min="19" max="19"/>
+    <col width="13.5703125" bestFit="1" customWidth="1" style="15" min="20" max="20"/>
+    <col width="14.5703125" bestFit="1" customWidth="1" style="15" min="21" max="22"/>
+    <col width="14.140625" customWidth="1" style="15" min="23" max="23"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -4188,7 +3795,7 @@
         </is>
       </c>
     </row>
-    <row r="2" ht="15" customHeight="1" s="18">
+    <row r="2" ht="15" customHeight="1" s="15">
       <c r="A2" t="n">
         <v>6</v>
       </c>
@@ -4245,11 +3852,11 @@
       <c r="K2" t="n">
         <v>638.4513379340638</v>
       </c>
-      <c r="M2" s="12">
+      <c r="M2" s="11">
         <f>ROUND((K2-G2)/G2,5)</f>
         <v/>
       </c>
-      <c r="N2" s="12" t="inlineStr">
+      <c r="N2" s="11" t="inlineStr">
         <is>
           <t>{"0": [[[5, 4], [4, 11], [1, 1]]], "1": [[[2, 6], [6, 11], [3, 8]]]}</t>
         </is>
@@ -4269,11 +3876,11 @@
       <c r="Q2" t="n">
         <v>638.4513379340638</v>
       </c>
-      <c r="R2" s="12">
+      <c r="R2" s="11">
         <f>ROUND((Q2-G2)/G2,5)</f>
         <v/>
       </c>
-      <c r="S2" s="13">
+      <c r="S2" s="12">
         <f>ROUND((Q2-K2)/K2,5)</f>
         <v/>
       </c>
@@ -4283,12 +3890,12 @@
       <c r="V2" t="n">
         <v>607.8712085577376</v>
       </c>
-      <c r="W2" s="13">
+      <c r="W2" s="12">
         <f>ROUND((V2-U2)/U2,5)</f>
         <v/>
       </c>
     </row>
-    <row r="3" ht="15" customHeight="1" s="18">
+    <row r="3" ht="15" customHeight="1" s="15">
       <c r="A3" t="n">
         <v>6</v>
       </c>
@@ -4346,11 +3953,11 @@
       <c r="K3" t="n">
         <v>813.0586880328467</v>
       </c>
-      <c r="M3" s="12">
+      <c r="M3" s="11">
         <f>ROUND((K3-G3)/G3,5)</f>
         <v/>
       </c>
-      <c r="N3" s="12" t="inlineStr">
+      <c r="N3" s="11" t="inlineStr">
         <is>
           <t>{"0": [[[2, 12]], [[4, 2], [5, 12]]], "1": [[[3, 13], [6, 1], [1, 11]]]}</t>
         </is>
@@ -4371,11 +3978,11 @@
       <c r="Q3" t="n">
         <v>813.0586880328467</v>
       </c>
-      <c r="R3" s="12">
+      <c r="R3" s="11">
         <f>ROUND((Q3-G3)/G3,5)</f>
         <v/>
       </c>
-      <c r="S3" s="13">
+      <c r="S3" s="12">
         <f>ROUND((Q3-K3)/K3,5)</f>
         <v/>
       </c>
@@ -4385,12 +3992,12 @@
       <c r="V3" t="n">
         <v>788.9363954883892</v>
       </c>
-      <c r="W3" s="13">
+      <c r="W3" s="12">
         <f>ROUND((V3-U3)/U3,5)</f>
         <v/>
       </c>
     </row>
-    <row r="4" ht="15" customHeight="1" s="18">
+    <row r="4" ht="15" customHeight="1" s="15">
       <c r="A4" t="n">
         <v>6</v>
       </c>
@@ -4445,13 +4052,13 @@
         </is>
       </c>
       <c r="K4" t="n">
-        <v>789.4920054354812</v>
-      </c>
-      <c r="M4" s="12">
+        <v>779.1938241974813</v>
+      </c>
+      <c r="M4" s="11">
         <f>ROUND((K4-G4)/G4,5)</f>
         <v/>
       </c>
-      <c r="N4" s="12" t="inlineStr">
+      <c r="N4" s="11" t="inlineStr">
         <is>
           <t>{"0": [[[6, 5], [4, 3], [5, 4]]], "1": [[]], "2": [[[1, 11], [2, 9], [3, 4]]]}</t>
         </is>
@@ -4467,16 +4074,16 @@
         </is>
       </c>
       <c r="P4" t="n">
-        <v>191.9536535</v>
+        <v>182.0879502</v>
       </c>
       <c r="Q4" t="n">
-        <v>789.4920054354812</v>
-      </c>
-      <c r="R4" s="12">
+        <v>779.1938241974813</v>
+      </c>
+      <c r="R4" s="11">
         <f>ROUND((Q4-G4)/G4,5)</f>
         <v/>
       </c>
-      <c r="S4" s="13">
+      <c r="S4" s="12">
         <f>ROUND((Q4-K4)/K4,5)</f>
         <v/>
       </c>
@@ -4486,12 +4093,12 @@
       <c r="V4" t="n">
         <v>686.3314631659716</v>
       </c>
-      <c r="W4" s="13">
+      <c r="W4" s="12">
         <f>ROUND((V4-U4)/U4,5)</f>
         <v/>
       </c>
     </row>
-    <row r="5" ht="15" customHeight="1" s="18">
+    <row r="5" ht="15" customHeight="1" s="15">
       <c r="A5" t="n">
         <v>6</v>
       </c>
@@ -4549,11 +4156,11 @@
       <c r="K5" t="n">
         <v>872.8408537938346</v>
       </c>
-      <c r="M5" s="12">
+      <c r="M5" s="11">
         <f>ROUND((K5-G5)/G5,5)</f>
         <v/>
       </c>
-      <c r="N5" s="12" t="inlineStr">
+      <c r="N5" s="11" t="inlineStr">
         <is>
           <t>{"0": [[[5, 10], [1, 9]]], "1": [[[6, 5], [4, 11]]], "2": [[[3, 12], [2, 3]]]}</t>
         </is>
@@ -4575,11 +4182,11 @@
       <c r="Q5" t="n">
         <v>872.8408537938346</v>
       </c>
-      <c r="R5" s="12">
+      <c r="R5" s="11">
         <f>ROUND((Q5-G5)/G5,5)</f>
         <v/>
       </c>
-      <c r="S5" s="13">
+      <c r="S5" s="12">
         <f>ROUND((Q5-K5)/K5,5)</f>
         <v/>
       </c>
@@ -4589,12 +4196,12 @@
       <c r="V5" t="n">
         <v>840.4624628971646</v>
       </c>
-      <c r="W5" s="13">
+      <c r="W5" s="12">
         <f>ROUND((V5-U5)/U5,5)</f>
         <v/>
       </c>
     </row>
-    <row r="6" ht="15" customHeight="1" s="18">
+    <row r="6" ht="15" customHeight="1" s="15">
       <c r="A6" t="n">
         <v>6</v>
       </c>
@@ -4651,11 +4258,11 @@
       <c r="K6" t="n">
         <v>532.0418049721413</v>
       </c>
-      <c r="M6" s="12">
+      <c r="M6" s="11">
         <f>ROUND((K6-G6)/G6,5)</f>
         <v/>
       </c>
-      <c r="N6" s="12" t="inlineStr">
+      <c r="N6" s="11" t="inlineStr">
         <is>
           <t>{"0": [[[4, 8], [2, 1], [1, 12]]], "1": [[]], "2": [[[6, 7], [5, 7], [3, 7]]]}</t>
         </is>
@@ -4676,11 +4283,11 @@
       <c r="Q6" t="n">
         <v>532.0418049721413</v>
       </c>
-      <c r="R6" s="12">
+      <c r="R6" s="11">
         <f>ROUND((Q6-G6)/G6,5)</f>
         <v/>
       </c>
-      <c r="S6" s="13">
+      <c r="S6" s="12">
         <f>ROUND((Q6-K6)/K6,5)</f>
         <v/>
       </c>
@@ -4690,12 +4297,12 @@
       <c r="V6" t="n">
         <v>506.6298814062009</v>
       </c>
-      <c r="W6" s="13">
+      <c r="W6" s="12">
         <f>ROUND((V6-U6)/U6,5)</f>
         <v/>
       </c>
     </row>
-    <row r="7" ht="15" customHeight="1" s="18">
+    <row r="7" ht="15" customHeight="1" s="15">
       <c r="A7" t="n">
         <v>6</v>
       </c>
@@ -4753,11 +4360,11 @@
       <c r="K7" t="n">
         <v>796.5139784858068</v>
       </c>
-      <c r="M7" s="12">
+      <c r="M7" s="11">
         <f>ROUND((K7-G7)/G7,5)</f>
         <v/>
       </c>
-      <c r="N7" s="12" t="inlineStr">
+      <c r="N7" s="11" t="inlineStr">
         <is>
           <t>{"0": [[[1, 9]]], "1": [[[6, 11], [3, 8]], [[5, 12], [4, 11], [2, 5]]]}</t>
         </is>
@@ -4778,11 +4385,11 @@
       <c r="Q7" t="n">
         <v>796.5139784858068</v>
       </c>
-      <c r="R7" s="12">
+      <c r="R7" s="11">
         <f>ROUND((Q7-G7)/G7,5)</f>
         <v/>
       </c>
-      <c r="S7" s="13">
+      <c r="S7" s="12">
         <f>ROUND((Q7-K7)/K7,5)</f>
         <v/>
       </c>
@@ -4792,12 +4399,12 @@
       <c r="V7" t="n">
         <v>760.5100181390749</v>
       </c>
-      <c r="W7" s="13">
+      <c r="W7" s="12">
         <f>ROUND((V7-U7)/U7,5)</f>
         <v/>
       </c>
     </row>
-    <row r="8" ht="15" customHeight="1" s="18">
+    <row r="8" ht="15" customHeight="1" s="15">
       <c r="A8" t="n">
         <v>6</v>
       </c>
@@ -4852,37 +4459,37 @@
         </is>
       </c>
       <c r="K8" t="n">
-        <v>779.8894337260737</v>
-      </c>
-      <c r="M8" s="12">
+        <v>774.2253803153903</v>
+      </c>
+      <c r="M8" s="11">
         <f>ROUND((K8-G8)/G8,5)</f>
         <v/>
       </c>
-      <c r="N8" s="12" t="inlineStr">
-        <is>
-          <t>{"0": [[[3, 1], [4, 10], [2, 7], [5, 3], [6, 5]]], "1": [[[1, 10]]]}</t>
+      <c r="N8" s="11" t="inlineStr">
+        <is>
+          <t>{"0": [[[1, 10], [5, 3], [2, 7], [6, 5]]], "1": [[[4, 10], [3, 1]]]}</t>
         </is>
       </c>
       <c r="O8" t="inlineStr">
         <is>
           <t xml:space="preserve">11 metre (capacity 30):
-3 (1) -&gt; 4 (10) -&gt; 2 (7) -&gt; 5 (3) -&gt; 6 (5)
+1 (10) -&gt; 5 (3) -&gt; 2 (7) -&gt; 6 (5)
 Rigid (capacity 16):
-1 (10)
+4 (10) -&gt; 3 (1)
 </t>
         </is>
       </c>
       <c r="P8" t="n">
-        <v>175.1238964000001</v>
+        <v>169.9795729</v>
       </c>
       <c r="Q8" t="n">
-        <v>772.6741840988848</v>
-      </c>
-      <c r="R8" s="12">
+        <v>774.2253803153903</v>
+      </c>
+      <c r="R8" s="11">
         <f>ROUND((Q8-G8)/G8,5)</f>
         <v/>
       </c>
-      <c r="S8" s="13">
+      <c r="S8" s="12">
         <f>ROUND((Q8-K8)/K8,5)</f>
         <v/>
       </c>
@@ -4890,14 +4497,14 @@
         <v>719.3032455616758</v>
       </c>
       <c r="V8" t="n">
-        <v>715.5619210524117</v>
-      </c>
-      <c r="W8" s="13">
+        <v>719.3032455616758</v>
+      </c>
+      <c r="W8" s="12">
         <f>ROUND((V8-U8)/U8,5)</f>
         <v/>
       </c>
     </row>
-    <row r="9" ht="15" customHeight="1" s="18">
+    <row r="9" ht="15" customHeight="1" s="15">
       <c r="A9" t="n">
         <v>6</v>
       </c>
@@ -4954,11 +4561,11 @@
       <c r="K9" t="n">
         <v>743.3214397132895</v>
       </c>
-      <c r="M9" s="12">
+      <c r="M9" s="11">
         <f>ROUND((K9-G9)/G9,5)</f>
         <v/>
       </c>
-      <c r="N9" s="12" t="inlineStr">
+      <c r="N9" s="11" t="inlineStr">
         <is>
           <t>{"0": [[[4, 5]]], "1": [[[5, 4], [6, 6], [1, 10], [2, 1], [3, 5]]]}</t>
         </is>
@@ -4978,11 +4585,11 @@
       <c r="Q9" t="n">
         <v>743.3214397132895</v>
       </c>
-      <c r="R9" s="12">
+      <c r="R9" s="11">
         <f>ROUND((Q9-G9)/G9,5)</f>
         <v/>
       </c>
-      <c r="S9" s="13">
+      <c r="S9" s="12">
         <f>ROUND((Q9-K9)/K9,5)</f>
         <v/>
       </c>
@@ -4992,12 +4599,12 @@
       <c r="V9" t="n">
         <v>720.7340698970215</v>
       </c>
-      <c r="W9" s="13">
+      <c r="W9" s="12">
         <f>ROUND((V9-U9)/U9,5)</f>
         <v/>
       </c>
     </row>
-    <row r="10" ht="15" customHeight="1" s="18">
+    <row r="10" ht="15" customHeight="1" s="15">
       <c r="A10" t="n">
         <v>6</v>
       </c>
@@ -5052,13 +4659,13 @@
         </is>
       </c>
       <c r="K10" t="n">
-        <v>678.5606762090117</v>
-      </c>
-      <c r="M10" s="12">
+        <v>665.3718381867769</v>
+      </c>
+      <c r="M10" s="11">
         <f>ROUND((K10-G10)/G10,5)</f>
         <v/>
       </c>
-      <c r="N10" s="12" t="inlineStr">
+      <c r="N10" s="11" t="inlineStr">
         <is>
           <t>{"0": [[[1, 1], [2, 2], [6, 6], [5, 6], [4, 4]], [[3, 14]]], "1": [[]]}</t>
         </is>
@@ -5073,16 +4680,16 @@
         </is>
       </c>
       <c r="P10" t="n">
-        <v>225.7582986</v>
+        <v>213.2704117</v>
       </c>
       <c r="Q10" t="n">
-        <v>678.5606762090117</v>
-      </c>
-      <c r="R10" s="12">
+        <v>665.3718381867769</v>
+      </c>
+      <c r="R10" s="11">
         <f>ROUND((Q10-G10)/G10,5)</f>
         <v/>
       </c>
-      <c r="S10" s="13">
+      <c r="S10" s="12">
         <f>ROUND((Q10-K10)/K10,5)</f>
         <v/>
       </c>
@@ -5092,12 +4699,12 @@
       <c r="V10" t="n">
         <v>559.7943291449662</v>
       </c>
-      <c r="W10" s="13">
+      <c r="W10" s="12">
         <f>ROUND((V10-U10)/U10,5)</f>
         <v/>
       </c>
     </row>
-    <row r="11" ht="15" customHeight="1" s="18">
+    <row r="11" ht="15" customHeight="1" s="15">
       <c r="A11" t="n">
         <v>6</v>
       </c>
@@ -5153,38 +4760,38 @@
         </is>
       </c>
       <c r="K11" t="n">
-        <v>649.8381449394853</v>
-      </c>
-      <c r="M11" s="12">
+        <v>653.2552840577687</v>
+      </c>
+      <c r="M11" s="11">
         <f>ROUND((K11-G11)/G11,5)</f>
         <v/>
       </c>
-      <c r="N11" s="12" t="inlineStr">
-        <is>
-          <t>{"0": [[[3, 11], [5, 10], [4, 5]]], "1": [[[2, 5]], [[1, 2], [6, 10]]]}</t>
+      <c r="N11" s="11" t="inlineStr">
+        <is>
+          <t>{"0": [[[4, 5], [5, 10], [3, 11]]], "1": [[[1, 2], [6, 10]], [[2, 5]]]}</t>
         </is>
       </c>
       <c r="O11" t="inlineStr">
         <is>
           <t xml:space="preserve">11 metre (capacity 30):
-3 (11) -&gt; 5 (10) -&gt; 4 (5)
+4 (5) -&gt; 5 (10) -&gt; 3 (11)
 Rigid (capacity 16):
+1 (2) -&gt; 6 (10)
 2 (5)
-1 (2) -&gt; 6 (10)
 </t>
         </is>
       </c>
       <c r="P11" t="n">
-        <v>178.3174023000001</v>
+        <v>170.2937817000001</v>
       </c>
       <c r="Q11" t="n">
         <v>685.7417399532771</v>
       </c>
-      <c r="R11" s="12">
+      <c r="R11" s="11">
         <f>ROUND((Q11-G11)/G11,5)</f>
         <v/>
       </c>
-      <c r="S11" s="13">
+      <c r="S11" s="12">
         <f>ROUND((Q11-K11)/K11,5)</f>
         <v/>
       </c>
@@ -5194,12 +4801,12 @@
       <c r="V11" t="n">
         <v>647.2463051245879</v>
       </c>
-      <c r="W11" s="13">
+      <c r="W11" s="12">
         <f>ROUND((V11-U11)/U11,5)</f>
         <v/>
       </c>
     </row>
-    <row r="12" ht="15" customHeight="1" s="18">
+    <row r="12" ht="15" customHeight="1" s="15">
       <c r="A12" t="n">
         <v>9</v>
       </c>
@@ -5263,11 +4870,11 @@
       <c r="K12" t="n">
         <v>667.7763169555091</v>
       </c>
-      <c r="M12" s="12">
+      <c r="M12" s="11">
         <f>ROUND((K12-G12)/G12,5)</f>
         <v/>
       </c>
-      <c r="N12" s="12" t="inlineStr">
+      <c r="N12" s="11" t="inlineStr">
         <is>
           <t>{"0": [[[9, 6], [6, 7], [2, 8], [1, 4], [7, 4]]], "1": [[]], "2": [[[5, 5], [3, 4], [8, 6], [4, 7]]]}</t>
         </is>
@@ -5283,16 +4890,16 @@
         </is>
       </c>
       <c r="P12" t="n">
-        <v>235.8595543</v>
+        <v>234.86645</v>
       </c>
       <c r="Q12" t="n">
         <v>667.7763169555091</v>
       </c>
-      <c r="R12" s="12">
+      <c r="R12" s="11">
         <f>ROUND((Q12-G12)/G12,5)</f>
         <v/>
       </c>
-      <c r="S12" s="13">
+      <c r="S12" s="12">
         <f>ROUND((Q12-K12)/K12,5)</f>
         <v/>
       </c>
@@ -5302,12 +4909,12 @@
       <c r="V12" t="n">
         <v>629.7369311852657</v>
       </c>
-      <c r="W12" s="13">
+      <c r="W12" s="12">
         <f>ROUND((V12-U12)/U12,5)</f>
         <v/>
       </c>
     </row>
-    <row r="13" ht="15" customHeight="1" s="18">
+    <row r="13" ht="15" customHeight="1" s="15">
       <c r="A13" t="n">
         <v>9</v>
       </c>
@@ -5370,11 +4977,11 @@
       <c r="K13" t="n">
         <v>632.2998388405235</v>
       </c>
-      <c r="M13" s="12">
+      <c r="M13" s="11">
         <f>ROUND((K13-G13)/G13,5)</f>
         <v/>
       </c>
-      <c r="N13" s="12" t="inlineStr">
+      <c r="N13" s="11" t="inlineStr">
         <is>
           <t>{"0": [[]], "1": [[[8, 2]]], "2": [[[9, 7], [2, 1], [6, 2], [1, 5], [5, 2], [4, 7], [3, 4], [7, 1]]]}</t>
         </is>
@@ -5395,11 +5002,11 @@
       <c r="Q13" t="n">
         <v>632.2998388405235</v>
       </c>
-      <c r="R13" s="12">
+      <c r="R13" s="11">
         <f>ROUND((Q13-G13)/G13,5)</f>
         <v/>
       </c>
-      <c r="S13" s="13">
+      <c r="S13" s="12">
         <f>ROUND((Q13-K13)/K13,5)</f>
         <v/>
       </c>
@@ -5409,12 +5016,12 @@
       <c r="V13" t="n">
         <v>598.2659663419413</v>
       </c>
-      <c r="W13" s="13">
+      <c r="W13" s="12">
         <f>ROUND((V13-U13)/U13,5)</f>
         <v/>
       </c>
     </row>
-    <row r="14" ht="15" customHeight="1" s="18">
+    <row r="14" ht="15" customHeight="1" s="15">
       <c r="A14" t="n">
         <v>9</v>
       </c>
@@ -5476,13 +5083,13 @@
         </is>
       </c>
       <c r="K14" t="n">
-        <v>934.0682967456817</v>
-      </c>
-      <c r="M14" s="12">
+        <v>932.2962654400412</v>
+      </c>
+      <c r="M14" s="11">
         <f>ROUND((K14-G14)/G14,5)</f>
         <v/>
       </c>
-      <c r="N14" s="12" t="inlineStr">
+      <c r="N14" s="11" t="inlineStr">
         <is>
           <t>{"0": [[[4, 6], [6, 6], [8, 8], [9, 8]]], "1": [[[1, 7], [3, 7]]], "2": [[[5, 6], [2, 6], [7, 4]]]}</t>
         </is>
@@ -5499,16 +5106,16 @@
         </is>
       </c>
       <c r="P14" t="n">
-        <v>287.8112921000001</v>
+        <v>281.4502775999999</v>
       </c>
       <c r="Q14" t="n">
-        <v>934.0682967456817</v>
-      </c>
-      <c r="R14" s="12">
+        <v>932.2962654400412</v>
+      </c>
+      <c r="R14" s="11">
         <f>ROUND((Q14-G14)/G14,5)</f>
         <v/>
       </c>
-      <c r="S14" s="13">
+      <c r="S14" s="12">
         <f>ROUND((Q14-K14)/K14,5)</f>
         <v/>
       </c>
@@ -5518,12 +5125,12 @@
       <c r="V14" t="n">
         <v>875.6021156551393</v>
       </c>
-      <c r="W14" s="13">
+      <c r="W14" s="12">
         <f>ROUND((V14-U14)/U14,5)</f>
         <v/>
       </c>
     </row>
-    <row r="15" ht="15" customHeight="1" s="18">
+    <row r="15" ht="15" customHeight="1" s="15">
       <c r="A15" t="n">
         <v>9</v>
       </c>
@@ -5586,11 +5193,11 @@
       <c r="K15" t="n">
         <v>530.3001190185752</v>
       </c>
-      <c r="M15" s="12">
+      <c r="M15" s="11">
         <f>ROUND((K15-G15)/G15,5)</f>
         <v/>
       </c>
-      <c r="N15" s="12" t="inlineStr">
+      <c r="N15" s="11" t="inlineStr">
         <is>
           <t>{"0": [[[7, 4], [8, 9], [4, 1], [9, 2], [2, 3], [5, 6]], [[1, 4], [6, 8], [3, 7]]], "1": [[]]}</t>
         </is>
@@ -5610,11 +5217,11 @@
       <c r="Q15" t="n">
         <v>530.3001190185752</v>
       </c>
-      <c r="R15" s="12">
+      <c r="R15" s="11">
         <f>ROUND((Q15-G15)/G15,5)</f>
         <v/>
       </c>
-      <c r="S15" s="13">
+      <c r="S15" s="12">
         <f>ROUND((Q15-K15)/K15,5)</f>
         <v/>
       </c>
@@ -5624,12 +5231,12 @@
       <c r="V15" t="n">
         <v>508.0636004548157</v>
       </c>
-      <c r="W15" s="13">
+      <c r="W15" s="12">
         <f>ROUND((V15-U15)/U15,5)</f>
         <v/>
       </c>
     </row>
-    <row r="16" ht="15" customHeight="1" s="18">
+    <row r="16" ht="15" customHeight="1" s="15">
       <c r="A16" t="n">
         <v>9</v>
       </c>
@@ -5692,11 +5299,11 @@
       <c r="K16" t="n">
         <v>795.4260237259559</v>
       </c>
-      <c r="M16" s="12">
+      <c r="M16" s="11">
         <f>ROUND((K16-G16)/G16,5)</f>
         <v/>
       </c>
-      <c r="N16" s="12" t="inlineStr">
+      <c r="N16" s="11" t="inlineStr">
         <is>
           <t>{"0": [[[3, 4], [1, 3], [6, 8], [8, 4]]], "1": [[[7, 2], [2, 3], [9, 1], [4, 7], [5, 6]]]}</t>
         </is>
@@ -5716,11 +5323,11 @@
       <c r="Q16" t="n">
         <v>795.4260237259559</v>
       </c>
-      <c r="R16" s="12">
+      <c r="R16" s="11">
         <f>ROUND((Q16-G16)/G16,5)</f>
         <v/>
       </c>
-      <c r="S16" s="13">
+      <c r="S16" s="12">
         <f>ROUND((Q16-K16)/K16,5)</f>
         <v/>
       </c>
@@ -5730,12 +5337,12 @@
       <c r="V16" t="n">
         <v>752.4949209428721</v>
       </c>
-      <c r="W16" s="13">
+      <c r="W16" s="12">
         <f>ROUND((V16-U16)/U16,5)</f>
         <v/>
       </c>
     </row>
-    <row r="17" ht="15" customHeight="1" s="18">
+    <row r="17" ht="15" customHeight="1" s="15">
       <c r="A17" t="n">
         <v>9</v>
       </c>
@@ -5798,11 +5405,11 @@
       <c r="K17" t="n">
         <v>606.8384365344339</v>
       </c>
-      <c r="M17" s="12">
+      <c r="M17" s="11">
         <f>ROUND((K17-G17)/G17,5)</f>
         <v/>
       </c>
-      <c r="N17" s="12" t="inlineStr">
+      <c r="N17" s="11" t="inlineStr">
         <is>
           <t>{"0": [[]], "1": [[[9, 4], [4, 6], [1, 6], [5, 2], [6, 2], [2, 2], [7, 7]]], "2": [[[3, 5], [8, 7]]]}</t>
         </is>
@@ -5823,11 +5430,11 @@
       <c r="Q17" t="n">
         <v>606.8384365344339</v>
       </c>
-      <c r="R17" s="12">
+      <c r="R17" s="11">
         <f>ROUND((Q17-G17)/G17,5)</f>
         <v/>
       </c>
-      <c r="S17" s="13">
+      <c r="S17" s="12">
         <f>ROUND((Q17-K17)/K17,5)</f>
         <v/>
       </c>
@@ -5837,12 +5444,12 @@
       <c r="V17" t="n">
         <v>578.1636012277588</v>
       </c>
-      <c r="W17" s="13">
+      <c r="W17" s="12">
         <f>ROUND((V17-U17)/U17,5)</f>
         <v/>
       </c>
     </row>
-    <row r="18" ht="15" customHeight="1" s="18">
+    <row r="18" ht="15" customHeight="1" s="15">
       <c r="A18" t="n">
         <v>9</v>
       </c>
@@ -5904,15 +5511,15 @@
         </is>
       </c>
       <c r="K18" t="n">
-        <v>734.7596731476024</v>
-      </c>
-      <c r="M18" s="12">
+        <v>727.2300819071808</v>
+      </c>
+      <c r="M18" s="11">
         <f>ROUND((K18-G18)/G18,5)</f>
         <v/>
       </c>
-      <c r="N18" s="12" t="inlineStr">
-        <is>
-          <t>{"0": [[[4, 3]]], "1": [[[2, 2], [9, 6], [7, 5], [3, 3]], [[8, 1], [5, 7], [1, 2], [6, 5]]]}</t>
+      <c r="N18" s="11" t="inlineStr">
+        <is>
+          <t>{"0": [[[4, 3]]], "1": [[[8, 1], [5, 7], [1, 2], [6, 5]], [[2, 2], [9, 6], [7, 5], [3, 3]]]}</t>
         </is>
       </c>
       <c r="O18" t="inlineStr">
@@ -5920,22 +5527,22 @@
           <t xml:space="preserve">11 metre (capacity 30):
 4 (3)
 Rigid (capacity 16):
+8 (1) -&gt; 5 (7) -&gt; 1 (2) -&gt; 6 (5)
 2 (2) -&gt; 9 (6) -&gt; 7 (5) -&gt; 3 (3)
-8 (1) -&gt; 5 (7) -&gt; 1 (2) -&gt; 6 (5)
 </t>
         </is>
       </c>
       <c r="P18" t="n">
-        <v>281.1863579000001</v>
+        <v>294.8059946000001</v>
       </c>
       <c r="Q18" t="n">
-        <v>734.7596731476024</v>
-      </c>
-      <c r="R18" s="12">
+        <v>727.2300819071808</v>
+      </c>
+      <c r="R18" s="11">
         <f>ROUND((Q18-G18)/G18,5)</f>
         <v/>
       </c>
-      <c r="S18" s="13">
+      <c r="S18" s="12">
         <f>ROUND((Q18-K18)/K18,5)</f>
         <v/>
       </c>
@@ -5945,12 +5552,12 @@
       <c r="V18" t="n">
         <v>660.3633141783124</v>
       </c>
-      <c r="W18" s="13">
+      <c r="W18" s="12">
         <f>ROUND((V18-U18)/U18,5)</f>
         <v/>
       </c>
     </row>
-    <row r="19" ht="15" customHeight="1" s="18">
+    <row r="19" ht="15" customHeight="1" s="15">
       <c r="A19" t="n">
         <v>9</v>
       </c>
@@ -6011,15 +5618,15 @@
         </is>
       </c>
       <c r="K19" t="n">
-        <v>841.3040532242246</v>
-      </c>
-      <c r="M19" s="12">
+        <v>861.0150341339806</v>
+      </c>
+      <c r="M19" s="11">
         <f>ROUND((K19-G19)/G19,5)</f>
         <v/>
       </c>
-      <c r="N19" s="12" t="inlineStr">
-        <is>
-          <t>{"0": [[]], "1": [[[6, 5], [9, 6], [8, 1]]], "2": [[[1, 7], [7, 1], [3, 1], [4, 1], [5, 6], [2, 6]]]}</t>
+      <c r="N19" s="11" t="inlineStr">
+        <is>
+          <t>{"0": [[]], "1": [[[6, 5], [9, 6], [8, 1]]], "2": [[[2, 6], [1, 7], [7, 1], [3, 1], [4, 1], [5, 6]]]}</t>
         </is>
       </c>
       <c r="O19" t="inlineStr">
@@ -6028,21 +5635,21 @@
 Rigid (capacity 16):
 6 (5) -&gt; 9 (6) -&gt; 8 (1)
 8 metre (capacity 22):
-1 (7) -&gt; 7 (1) -&gt; 3 (1) -&gt; 4 (1) -&gt; 5 (6) -&gt; 2 (6)
+2 (6) -&gt; 1 (7) -&gt; 7 (1) -&gt; 3 (1) -&gt; 4 (1) -&gt; 5 (6)
 </t>
         </is>
       </c>
       <c r="P19" t="n">
-        <v>284.8996525</v>
+        <v>279.6937158999999</v>
       </c>
       <c r="Q19" t="n">
-        <v>887.7611151354606</v>
-      </c>
-      <c r="R19" s="12">
+        <v>861.0150341339806</v>
+      </c>
+      <c r="R19" s="11">
         <f>ROUND((Q19-G19)/G19,5)</f>
         <v/>
       </c>
-      <c r="S19" s="13">
+      <c r="S19" s="12">
         <f>ROUND((Q19-K19)/K19,5)</f>
         <v/>
       </c>
@@ -6050,14 +5657,14 @@
         <v>819.5322926332794</v>
       </c>
       <c r="V19" t="n">
-        <v>846.2783736347593</v>
-      </c>
-      <c r="W19" s="13">
+        <v>819.5322926332793</v>
+      </c>
+      <c r="W19" s="12">
         <f>ROUND((V19-U19)/U19,5)</f>
         <v/>
       </c>
     </row>
-    <row r="20" ht="15" customHeight="1" s="18">
+    <row r="20" ht="15" customHeight="1" s="15">
       <c r="A20" t="n">
         <v>9</v>
       </c>
@@ -6119,37 +5726,37 @@
         </is>
       </c>
       <c r="K20" t="n">
-        <v>637.4891259685992</v>
-      </c>
-      <c r="M20" s="12">
+        <v>632.7434936560544</v>
+      </c>
+      <c r="M20" s="11">
         <f>ROUND((K20-G20)/G20,5)</f>
         <v/>
       </c>
-      <c r="N20" s="12" t="inlineStr">
-        <is>
-          <t>{"0": [[[1, 5], [5, 5], [7, 6]], [[4, 4], [3, 4], [9, 3]], [[2, 5], [8, 4], [6, 3]]]}</t>
+      <c r="N20" s="11" t="inlineStr">
+        <is>
+          <t>{"0": [[[4, 4], [3, 4], [9, 3]], [[7, 6], [5, 5], [1, 5]], [[2, 5], [8, 4], [6, 3]]]}</t>
         </is>
       </c>
       <c r="O20" t="inlineStr">
         <is>
           <t xml:space="preserve">Rigid (capacity 16):
-1 (5) -&gt; 5 (5) -&gt; 7 (6)
 4 (4) -&gt; 3 (4) -&gt; 9 (3)
+7 (6) -&gt; 5 (5) -&gt; 1 (5)
 2 (5) -&gt; 8 (4) -&gt; 6 (3)
 </t>
         </is>
       </c>
       <c r="P20" t="n">
-        <v>247.3473273</v>
+        <v>257.9959804</v>
       </c>
       <c r="Q20" t="n">
         <v>661.7039481971021</v>
       </c>
-      <c r="R20" s="12">
+      <c r="R20" s="11">
         <f>ROUND((Q20-G20)/G20,5)</f>
         <v/>
       </c>
-      <c r="S20" s="13">
+      <c r="S20" s="12">
         <f>ROUND((Q20-K20)/K20,5)</f>
         <v/>
       </c>
@@ -6159,12 +5766,12 @@
       <c r="V20" t="n">
         <v>623.7514315590706</v>
       </c>
-      <c r="W20" s="13">
+      <c r="W20" s="12">
         <f>ROUND((V20-U20)/U20,5)</f>
         <v/>
       </c>
     </row>
-    <row r="21" ht="15" customHeight="1" s="18">
+    <row r="21" ht="15" customHeight="1" s="15">
       <c r="A21" t="n">
         <v>9</v>
       </c>
@@ -6228,11 +5835,11 @@
       <c r="K21" t="n">
         <v>935.5446906430152</v>
       </c>
-      <c r="M21" s="12">
+      <c r="M21" s="11">
         <f>ROUND((K21-G21)/G21,5)</f>
         <v/>
       </c>
-      <c r="N21" s="12" t="inlineStr">
+      <c r="N21" s="11" t="inlineStr">
         <is>
           <t>{"0": [[[9, 2], [2, 10], [8, 3]], [[1, 7], [3, 1], [5, 6], [6, 6], [4, 10]], [[7, 9]]]}</t>
         </is>
@@ -6252,11 +5859,11 @@
       <c r="Q21" t="n">
         <v>935.5446906430152</v>
       </c>
-      <c r="R21" s="12">
+      <c r="R21" s="11">
         <f>ROUND((Q21-G21)/G21,5)</f>
         <v/>
       </c>
-      <c r="S21" s="13">
+      <c r="S21" s="12">
         <f>ROUND((Q21-K21)/K21,5)</f>
         <v/>
       </c>
@@ -6266,12 +5873,12 @@
       <c r="V21" t="n">
         <v>847.0028446991276</v>
       </c>
-      <c r="W21" s="13">
+      <c r="W21" s="12">
         <f>ROUND((V21-U21)/U21,5)</f>
         <v/>
       </c>
     </row>
-    <row r="22" ht="15" customHeight="1" s="18">
+    <row r="22" ht="15" customHeight="1" s="15">
       <c r="A22" t="n">
         <v>12</v>
       </c>
@@ -6340,11 +5947,11 @@
       <c r="K22" t="n">
         <v>665.628829734027</v>
       </c>
-      <c r="M22" s="12">
+      <c r="M22" s="11">
         <f>ROUND((K22-G22)/G22,5)</f>
         <v/>
       </c>
-      <c r="N22" s="12" t="inlineStr">
+      <c r="N22" s="11" t="inlineStr">
         <is>
           <t>{"0": [[[3, 5], [11, 4], [10, 5], [8, 2]]], "1": [[[7, 4], [1, 2], [5, 1], [4, 3], [9, 4], [6, 3], [12, 1], [2, 4]]]}</t>
         </is>
@@ -6364,11 +5971,11 @@
       <c r="Q22" t="n">
         <v>665.628829734027</v>
       </c>
-      <c r="R22" s="12">
+      <c r="R22" s="11">
         <f>ROUND((Q22-G22)/G22,5)</f>
         <v/>
       </c>
-      <c r="S22" s="13">
+      <c r="S22" s="12">
         <f>ROUND((Q22-K22)/K22,5)</f>
         <v/>
       </c>
@@ -6378,12 +5985,12 @@
       <c r="V22" t="n">
         <v>614.7655005468939</v>
       </c>
-      <c r="W22" s="13">
+      <c r="W22" s="12">
         <f>ROUND((V22-U22)/U22,5)</f>
         <v/>
       </c>
     </row>
-    <row r="23" ht="15" customHeight="1" s="18">
+    <row r="23" ht="15" customHeight="1" s="15">
       <c r="A23" t="n">
         <v>12</v>
       </c>
@@ -6452,11 +6059,11 @@
       <c r="K23" t="n">
         <v>1189.404777283196</v>
       </c>
-      <c r="M23" s="12">
+      <c r="M23" s="11">
         <f>ROUND((K23-G23)/G23,5)</f>
         <v/>
       </c>
-      <c r="N23" s="12" t="inlineStr">
+      <c r="N23" s="11" t="inlineStr">
         <is>
           <t>{"0": [[[8, 1], [10, 1], [6, 2], [1, 1], [2, 2], [3, 1]], [[12, 2], [9, 5], [5, 6], [7, 1], [4, 4], [11, 6]]], "1": [[]]}</t>
         </is>
@@ -6471,16 +6078,16 @@
         </is>
       </c>
       <c r="P23" t="n">
-        <v>436.2706252</v>
+        <v>441.6552514</v>
       </c>
       <c r="Q23" t="n">
         <v>1189.404777283196</v>
       </c>
-      <c r="R23" s="12">
+      <c r="R23" s="11">
         <f>ROUND((Q23-G23)/G23,5)</f>
         <v/>
       </c>
-      <c r="S23" s="13">
+      <c r="S23" s="12">
         <f>ROUND((Q23-K23)/K23,5)</f>
         <v/>
       </c>
@@ -6490,12 +6097,12 @@
       <c r="V23" t="n">
         <v>1105.825492398589</v>
       </c>
-      <c r="W23" s="13">
+      <c r="W23" s="12">
         <f>ROUND((V23-U23)/U23,5)</f>
         <v/>
       </c>
     </row>
-    <row r="24" ht="15" customHeight="1" s="18">
+    <row r="24" ht="15" customHeight="1" s="15">
       <c r="A24" t="n">
         <v>12</v>
       </c>
@@ -6563,38 +6170,38 @@
         </is>
       </c>
       <c r="K24" t="n">
-        <v>848.4988087327888</v>
-      </c>
-      <c r="M24" s="12">
+        <v>855.5133712082734</v>
+      </c>
+      <c r="M24" s="11">
         <f>ROUND((K24-G24)/G24,5)</f>
         <v/>
       </c>
-      <c r="N24" s="12" t="inlineStr">
-        <is>
-          <t>{"0": [[[2, 5], [6, 6], [9, 2], [8, 3]], [[10, 5], [11, 5]]], "1": [[[7, 3], [5, 3], [12, 6], [4, 6], [3, 6], [1, 6]]]}</t>
+      <c r="N24" s="11" t="inlineStr">
+        <is>
+          <t>{"0": [[[2, 5], [6, 6], [9, 2], [8, 3]], [[11, 5], [10, 5]]], "1": [[[5, 3], [12, 6], [4, 6], [3, 6], [1, 6], [7, 3]]]}</t>
         </is>
       </c>
       <c r="O24" t="inlineStr">
         <is>
           <t xml:space="preserve">Rigid (capacity 16):
 2 (5) -&gt; 6 (6) -&gt; 9 (2) -&gt; 8 (3)
-10 (5) -&gt; 11 (5)
+11 (5) -&gt; 10 (5)
 11 metre (capacity 30):
-7 (3) -&gt; 5 (3) -&gt; 12 (6) -&gt; 4 (6) -&gt; 3 (6) -&gt; 1 (6)
+5 (3) -&gt; 12 (6) -&gt; 4 (6) -&gt; 3 (6) -&gt; 1 (6) -&gt; 7 (3)
 </t>
         </is>
       </c>
       <c r="P24" t="n">
-        <v>346.9195768</v>
+        <v>310.1220506999999</v>
       </c>
       <c r="Q24" t="n">
-        <v>848.4988087327888</v>
-      </c>
-      <c r="R24" s="12">
+        <v>852.0612441589832</v>
+      </c>
+      <c r="R24" s="11">
         <f>ROUND((Q24-G24)/G24,5)</f>
         <v/>
       </c>
-      <c r="S24" s="13">
+      <c r="S24" s="12">
         <f>ROUND((Q24-K24)/K24,5)</f>
         <v/>
       </c>
@@ -6602,14 +6209,14 @@
         <v>798.9569162999314</v>
       </c>
       <c r="V24" t="n">
-        <v>798.9569162999314</v>
-      </c>
-      <c r="W24" s="13">
+        <v>795.5047892506411</v>
+      </c>
+      <c r="W24" s="12">
         <f>ROUND((V24-U24)/U24,5)</f>
         <v/>
       </c>
     </row>
-    <row r="25" ht="15" customHeight="1" s="18">
+    <row r="25" ht="15" customHeight="1" s="15">
       <c r="A25" t="n">
         <v>12</v>
       </c>
@@ -6679,11 +6286,11 @@
       <c r="K25" t="n">
         <v>719.8083018045488</v>
       </c>
-      <c r="M25" s="12">
+      <c r="M25" s="11">
         <f>ROUND((K25-G25)/G25,5)</f>
         <v/>
       </c>
-      <c r="N25" s="12" t="inlineStr">
+      <c r="N25" s="11" t="inlineStr">
         <is>
           <t>{"0": [[[7, 4], [1, 6], [3, 1], [2, 7], [11, 4]]], "1": [[[5, 2], [8, 4], [10, 3], [12, 4], [9, 6], [4, 4], [6, 6]]]}</t>
         </is>
@@ -6703,11 +6310,11 @@
       <c r="Q25" t="n">
         <v>727.5130074671956</v>
       </c>
-      <c r="R25" s="12">
+      <c r="R25" s="11">
         <f>ROUND((Q25-G25)/G25,5)</f>
         <v/>
       </c>
-      <c r="S25" s="13">
+      <c r="S25" s="12">
         <f>ROUND((Q25-K25)/K25,5)</f>
         <v/>
       </c>
@@ -6717,12 +6324,12 @@
       <c r="V25" t="n">
         <v>690.196278882438</v>
       </c>
-      <c r="W25" s="13">
+      <c r="W25" s="12">
         <f>ROUND((V25-U25)/U25,5)</f>
         <v/>
       </c>
     </row>
-    <row r="26" ht="15" customHeight="1" s="18">
+    <row r="26" ht="15" customHeight="1" s="15">
       <c r="A26" t="n">
         <v>12</v>
       </c>
@@ -6792,11 +6399,11 @@
       <c r="K26" t="n">
         <v>1078.299811829309</v>
       </c>
-      <c r="M26" s="12">
+      <c r="M26" s="11">
         <f>ROUND((K26-G26)/G26,5)</f>
         <v/>
       </c>
-      <c r="N26" s="12" t="inlineStr">
+      <c r="N26" s="11" t="inlineStr">
         <is>
           <t>{"0": [[[3, 5], [5, 4], [1, 4], [7, 1], [4, 2], [8, 5]], [[12, 5], [11, 5], [9, 5], [2, 2], [6, 4]]], "1": [[[10, 4]]]}</t>
         </is>
@@ -6817,11 +6424,11 @@
       <c r="Q26" t="n">
         <v>1078.299811829309</v>
       </c>
-      <c r="R26" s="12">
+      <c r="R26" s="11">
         <f>ROUND((Q26-G26)/G26,5)</f>
         <v/>
       </c>
-      <c r="S26" s="13">
+      <c r="S26" s="12">
         <f>ROUND((Q26-K26)/K26,5)</f>
         <v/>
       </c>
@@ -6831,12 +6438,12 @@
       <c r="V26" t="n">
         <v>1034.284180844275</v>
       </c>
-      <c r="W26" s="13">
+      <c r="W26" s="12">
         <f>ROUND((V26-U26)/U26,5)</f>
         <v/>
       </c>
     </row>
-    <row r="27" ht="15" customHeight="1" s="18">
+    <row r="27" ht="15" customHeight="1" s="15">
       <c r="A27" t="n">
         <v>12</v>
       </c>
@@ -6906,11 +6513,11 @@
       <c r="K27" t="n">
         <v>1077.167439794624</v>
       </c>
-      <c r="M27" s="12">
+      <c r="M27" s="11">
         <f>ROUND((K27-G27)/G27,5)</f>
         <v/>
       </c>
-      <c r="N27" s="12" t="inlineStr">
+      <c r="N27" s="11" t="inlineStr">
         <is>
           <t>{"0": [[[5, 3], [9, 5], [4, 1], [2, 6]]], "1": [[[3, 3], [11, 5]]], "2": [[[12, 6], [8, 6], [10, 4], [6, 6], [1, 5], [7, 2]]]}</t>
         </is>
@@ -6932,11 +6539,11 @@
       <c r="Q27" t="n">
         <v>1077.167439794624</v>
       </c>
-      <c r="R27" s="12">
+      <c r="R27" s="11">
         <f>ROUND((Q27-G27)/G27,5)</f>
         <v/>
       </c>
-      <c r="S27" s="13">
+      <c r="S27" s="12">
         <f>ROUND((Q27-K27)/K27,5)</f>
         <v/>
       </c>
@@ -6946,12 +6553,12 @@
       <c r="V27" t="n">
         <v>1022.759507244422</v>
       </c>
-      <c r="W27" s="13">
+      <c r="W27" s="12">
         <f>ROUND((V27-U27)/U27,5)</f>
         <v/>
       </c>
     </row>
-    <row r="28" ht="15" customHeight="1" s="18">
+    <row r="28" ht="15" customHeight="1" s="15">
       <c r="A28" t="n">
         <v>12</v>
       </c>
@@ -7021,11 +6628,11 @@
       <c r="K28" t="n">
         <v>1048.318016484704</v>
       </c>
-      <c r="M28" s="12">
+      <c r="M28" s="11">
         <f>ROUND((K28-G28)/G28,5)</f>
         <v/>
       </c>
-      <c r="N28" s="12" t="inlineStr">
+      <c r="N28" s="11" t="inlineStr">
         <is>
           <t>{"0": [[[11, 6], [1, 3], [9, 2]], [[8, 3], [6, 6], [12, 2]]], "1": [[[3, 4], [5, 4], [4, 4], [2, 2], [10, 3], [7, 3]]]}</t>
         </is>
@@ -7046,11 +6653,11 @@
       <c r="Q28" t="n">
         <v>1048.318016484704</v>
       </c>
-      <c r="R28" s="12">
+      <c r="R28" s="11">
         <f>ROUND((Q28-G28)/G28,5)</f>
         <v/>
       </c>
-      <c r="S28" s="13">
+      <c r="S28" s="12">
         <f>ROUND((Q28-K28)/K28,5)</f>
         <v/>
       </c>
@@ -7060,12 +6667,12 @@
       <c r="V28" t="n">
         <v>1003.589778043422</v>
       </c>
-      <c r="W28" s="13">
+      <c r="W28" s="12">
         <f>ROUND((V28-U28)/U28,5)</f>
         <v/>
       </c>
     </row>
-    <row r="29" ht="15" customHeight="1" s="18">
+    <row r="29" ht="15" customHeight="1" s="15">
       <c r="A29" t="n">
         <v>12</v>
       </c>
@@ -7134,11 +6741,11 @@
       <c r="K29" t="n">
         <v>1136.667756966691</v>
       </c>
-      <c r="M29" s="12">
+      <c r="M29" s="11">
         <f>ROUND((K29-G29)/G29,5)</f>
         <v/>
       </c>
-      <c r="N29" s="12" t="inlineStr">
+      <c r="N29" s="11" t="inlineStr">
         <is>
           <t>{"0": [[[4, 3], [9, 4], [7, 2], [6, 1], [1, 3], [2, 2]], [[12, 1], [5, 2], [10, 3], [11, 1], [3, 3], [8, 3]]]}</t>
         </is>
@@ -7157,11 +6764,11 @@
       <c r="Q29" t="n">
         <v>1136.667756966691</v>
       </c>
-      <c r="R29" s="12">
+      <c r="R29" s="11">
         <f>ROUND((Q29-G29)/G29,5)</f>
         <v/>
       </c>
-      <c r="S29" s="13">
+      <c r="S29" s="12">
         <f>ROUND((Q29-K29)/K29,5)</f>
         <v/>
       </c>
@@ -7171,12 +6778,12 @@
       <c r="V29" t="n">
         <v>1115.457582835203</v>
       </c>
-      <c r="W29" s="13">
+      <c r="W29" s="12">
         <f>ROUND((V29-U29)/U29,5)</f>
         <v/>
       </c>
     </row>
-    <row r="30" ht="15" customHeight="1" s="18">
+    <row r="30" ht="15" customHeight="1" s="15">
       <c r="A30" t="n">
         <v>12</v>
       </c>
@@ -7246,11 +6853,11 @@
       <c r="K30" t="n">
         <v>1272.345104477296</v>
       </c>
-      <c r="M30" s="12">
+      <c r="M30" s="11">
         <f>ROUND((K30-G30)/G30,5)</f>
         <v/>
       </c>
-      <c r="N30" s="12" t="inlineStr">
+      <c r="N30" s="11" t="inlineStr">
         <is>
           <t>{"0": [[[3, 1], [5, 3], [11, 6], [12, 6]]], "1": [[[2, 4], [8, 5], [1, 6], [6, 1], [10, 4]]], "2": [[[4, 4], [7, 3], [9, 4]]]}</t>
         </is>
@@ -7272,11 +6879,11 @@
       <c r="Q30" t="n">
         <v>1272.345104477296</v>
       </c>
-      <c r="R30" s="12">
+      <c r="R30" s="11">
         <f>ROUND((Q30-G30)/G30,5)</f>
         <v/>
       </c>
-      <c r="S30" s="13">
+      <c r="S30" s="12">
         <f>ROUND((Q30-K30)/K30,5)</f>
         <v/>
       </c>
@@ -7286,12 +6893,12 @@
       <c r="V30" t="n">
         <v>1220.227035565441</v>
       </c>
-      <c r="W30" s="13">
+      <c r="W30" s="12">
         <f>ROUND((V30-U30)/U30,5)</f>
         <v/>
       </c>
     </row>
-    <row r="31" ht="15" customHeight="1" s="18">
+    <row r="31" ht="15" customHeight="1" s="15">
       <c r="A31" t="n">
         <v>12</v>
       </c>
@@ -7361,11 +6968,11 @@
       <c r="K31" t="n">
         <v>734.1369792097994</v>
       </c>
-      <c r="M31" s="12">
+      <c r="M31" s="11">
         <f>ROUND((K31-G31)/G31,5)</f>
         <v/>
       </c>
-      <c r="N31" s="12" t="inlineStr">
+      <c r="N31" s="11" t="inlineStr">
         <is>
           <t>{"0": [[[6, 4], [11, 3], [1, 1], [7, 3], [12, 1], [5, 4]], [[10, 3], [3, 2], [9, 1], [4, 4], [2, 2], [8, 4]]]}</t>
         </is>
@@ -7384,11 +6991,11 @@
       <c r="Q31" t="n">
         <v>765.15981731728</v>
       </c>
-      <c r="R31" s="12">
+      <c r="R31" s="11">
         <f>ROUND((Q31-G31)/G31,5)</f>
         <v/>
       </c>
-      <c r="S31" s="13">
+      <c r="S31" s="12">
         <f>ROUND((Q31-K31)/K31,5)</f>
         <v/>
       </c>
@@ -7398,12 +7005,12 @@
       <c r="V31" t="n">
         <v>730.4929250965572</v>
       </c>
-      <c r="W31" s="13">
+      <c r="W31" s="12">
         <f>ROUND((V31-U31)/U31,5)</f>
         <v/>
       </c>
     </row>
-    <row r="32" ht="15" customHeight="1" s="18">
+    <row r="32" ht="15" customHeight="1" s="15">
       <c r="A32" t="n">
         <v>6</v>
       </c>
@@ -7464,11 +7071,11 @@
       <c r="K32" t="n">
         <v>812.2567044500715</v>
       </c>
-      <c r="M32" s="12">
+      <c r="M32" s="11">
         <f>ROUND((K32-G32)/G32,5)</f>
         <v/>
       </c>
-      <c r="N32" s="12" t="inlineStr">
+      <c r="N32" s="11" t="inlineStr">
         <is>
           <t>{"0": [[[4, 16], [6, 5]], [[1, 5]]], "1": [[[5, 2], [2, 2], [3, 12]]], "2": [[]]}</t>
         </is>
@@ -7490,11 +7097,11 @@
       <c r="Q32" t="n">
         <v>825.6680875343193</v>
       </c>
-      <c r="R32" s="12">
+      <c r="R32" s="11">
         <f>ROUND((Q32-G32)/G32,5)</f>
         <v/>
       </c>
-      <c r="S32" s="13">
+      <c r="S32" s="12">
         <f>ROUND((Q32-K32)/K32,5)</f>
         <v/>
       </c>
@@ -7504,12 +7111,12 @@
       <c r="V32" t="n">
         <v>750.3182492647884</v>
       </c>
-      <c r="W32" s="13">
+      <c r="W32" s="12">
         <f>ROUND((V32-U32)/U32,5)</f>
         <v/>
       </c>
     </row>
-    <row r="33" ht="15" customHeight="1" s="18">
+    <row r="33" ht="15" customHeight="1" s="15">
       <c r="A33" t="n">
         <v>6</v>
       </c>
@@ -7567,13 +7174,13 @@
         </is>
       </c>
       <c r="K33" t="n">
-        <v>700.1813452705869</v>
-      </c>
-      <c r="M33" s="12">
+        <v>693.0670489755869</v>
+      </c>
+      <c r="M33" s="11">
         <f>ROUND((K33-G33)/G33,5)</f>
         <v/>
       </c>
-      <c r="N33" s="12" t="inlineStr">
+      <c r="N33" s="11" t="inlineStr">
         <is>
           <t>{"0": [[]], "1": [[[6, 9], [4, 4], [1, 9]], [[3, 10]]], "2": [[[2, 8], [5, 14]]]}</t>
         </is>
@@ -7590,16 +7197,16 @@
         </is>
       </c>
       <c r="P33" t="n">
-        <v>239.3844907999996</v>
+        <v>180.2311289000002</v>
       </c>
       <c r="Q33" t="n">
-        <v>700.1813452705869</v>
-      </c>
-      <c r="R33" s="12">
+        <v>693.0670489755869</v>
+      </c>
+      <c r="R33" s="11">
         <f>ROUND((Q33-G33)/G33,5)</f>
         <v/>
       </c>
-      <c r="S33" s="13">
+      <c r="S33" s="12">
         <f>ROUND((Q33-K33)/K33,5)</f>
         <v/>
       </c>
@@ -7609,12 +7216,12 @@
       <c r="V33" t="n">
         <v>582.0975628366479</v>
       </c>
-      <c r="W33" s="13">
+      <c r="W33" s="12">
         <f>ROUND((V33-U33)/U33,5)</f>
         <v/>
       </c>
     </row>
-    <row r="34" ht="15" customHeight="1" s="18">
+    <row r="34" ht="15" customHeight="1" s="15">
       <c r="A34" t="n">
         <v>6</v>
       </c>
@@ -7674,11 +7281,11 @@
       <c r="K34" t="n">
         <v>744.6053920604409</v>
       </c>
-      <c r="M34" s="12">
+      <c r="M34" s="11">
         <f>ROUND((K34-G34)/G34,5)</f>
         <v/>
       </c>
-      <c r="N34" s="12" t="inlineStr">
+      <c r="N34" s="11" t="inlineStr">
         <is>
           <t>{"0": [[[5, 18]], [[6, 4], [3, 3]]], "1": [[[4, 9], [1, 9], [2, 12]]], "2": [[]]}</t>
         </is>
@@ -7700,11 +7307,11 @@
       <c r="Q34" t="n">
         <v>733.0820870926568</v>
       </c>
-      <c r="R34" s="12">
+      <c r="R34" s="11">
         <f>ROUND((Q34-G34)/G34,5)</f>
         <v/>
       </c>
-      <c r="S34" s="13">
+      <c r="S34" s="12">
         <f>ROUND((Q34-K34)/K34,5)</f>
         <v/>
       </c>
@@ -7714,12 +7321,12 @@
       <c r="V34" t="n">
         <v>663.8094351405824</v>
       </c>
-      <c r="W34" s="13">
+      <c r="W34" s="12">
         <f>ROUND((V34-U34)/U34,5)</f>
         <v/>
       </c>
     </row>
-    <row r="35" ht="15" customHeight="1" s="18">
+    <row r="35" ht="15" customHeight="1" s="15">
       <c r="A35" t="n">
         <v>6</v>
       </c>
@@ -7779,11 +7386,11 @@
       <c r="K35" t="n">
         <v>656.5587838417349</v>
       </c>
-      <c r="M35" s="12">
+      <c r="M35" s="11">
         <f>ROUND((K35-G35)/G35,5)</f>
         <v/>
       </c>
-      <c r="N35" s="12" t="inlineStr">
+      <c r="N35" s="11" t="inlineStr">
         <is>
           <t>{"0": [[[5, 7], [6, 1], [4, 13]], [[1, 17], [2, 4]]], "1": [[[3, 11]]]}</t>
         </is>
@@ -7804,11 +7411,11 @@
       <c r="Q35" t="n">
         <v>642.5531845117245</v>
       </c>
-      <c r="R35" s="12">
+      <c r="R35" s="11">
         <f>ROUND((Q35-G35)/G35,5)</f>
         <v/>
       </c>
-      <c r="S35" s="13">
+      <c r="S35" s="12">
         <f>ROUND((Q35-K35)/K35,5)</f>
         <v/>
       </c>
@@ -7818,12 +7425,12 @@
       <c r="V35" t="n">
         <v>616.4106772089158</v>
       </c>
-      <c r="W35" s="13">
+      <c r="W35" s="12">
         <f>ROUND((V35-U35)/U35,5)</f>
         <v/>
       </c>
     </row>
-    <row r="36" ht="15" customHeight="1" s="18">
+    <row r="36" ht="15" customHeight="1" s="15">
       <c r="A36" t="n">
         <v>6</v>
       </c>
@@ -7881,39 +7488,39 @@
         </is>
       </c>
       <c r="K36" t="n">
-        <v>1208.932192147432</v>
-      </c>
-      <c r="M36" s="12">
+        <v>1195.611144737432</v>
+      </c>
+      <c r="M36" s="11">
         <f>ROUND((K36-G36)/G36,5)</f>
         <v/>
       </c>
-      <c r="N36" s="12" t="inlineStr">
-        <is>
-          <t>{"0": [[]], "1": [[[6, 6]], [[3, 15], [4, 5]]], "2": [[[5, 11], [1, 5], [2, 8]]]}</t>
+      <c r="N36" s="11" t="inlineStr">
+        <is>
+          <t>{"0": [[]], "1": [[[3, 15], [4, 5]], [[6, 6]]], "2": [[[2, 8], [1, 5], [5, 11]]]}</t>
         </is>
       </c>
       <c r="O36" t="inlineStr">
         <is>
           <t xml:space="preserve">Rigid (capacity 16):
 8 metre (capacity 22):
+3 (15) -&gt; 4 (5)
 6 (6)
-3 (15) -&gt; 4 (5)
 11 metre (capacity 30):
-5 (11) -&gt; 1 (5) -&gt; 2 (8)
+2 (8) -&gt; 1 (5) -&gt; 5 (11)
 </t>
         </is>
       </c>
       <c r="P36" t="n">
-        <v>234.3237515999999</v>
+        <v>190.2647391</v>
       </c>
       <c r="Q36" t="n">
-        <v>1208.932192147432</v>
-      </c>
-      <c r="R36" s="12">
+        <v>1195.611144737432</v>
+      </c>
+      <c r="R36" s="11">
         <f>ROUND((Q36-G36)/G36,5)</f>
         <v/>
       </c>
-      <c r="S36" s="13">
+      <c r="S36" s="12">
         <f>ROUND((Q36-K36)/K36,5)</f>
         <v/>
       </c>
@@ -7923,12 +7530,12 @@
       <c r="V36" t="n">
         <v>1075.925812216501</v>
       </c>
-      <c r="W36" s="13">
+      <c r="W36" s="12">
         <f>ROUND((V36-U36)/U36,5)</f>
         <v/>
       </c>
     </row>
-    <row r="37" ht="15" customHeight="1" s="18">
+    <row r="37" ht="15" customHeight="1" s="15">
       <c r="A37" t="n">
         <v>6</v>
       </c>
@@ -7989,11 +7596,11 @@
       <c r="K37" t="n">
         <v>889.265507951744</v>
       </c>
-      <c r="M37" s="12">
+      <c r="M37" s="11">
         <f>ROUND((K37-G37)/G37,5)</f>
         <v/>
       </c>
-      <c r="N37" s="12" t="inlineStr">
+      <c r="N37" s="11" t="inlineStr">
         <is>
           <t>{"0": [[[5, 18]], [[6, 10], [2, 8]]], "1": [[[3, 8], [4, 1], [1, 3]]]}</t>
         </is>
@@ -8014,11 +7621,11 @@
       <c r="Q37" t="n">
         <v>885.2360474818561</v>
       </c>
-      <c r="R37" s="12">
+      <c r="R37" s="11">
         <f>ROUND((Q37-G37)/G37,5)</f>
         <v/>
       </c>
-      <c r="S37" s="13">
+      <c r="S37" s="12">
         <f>ROUND((Q37-K37)/K37,5)</f>
         <v/>
       </c>
@@ -8028,12 +7635,12 @@
       <c r="V37" t="n">
         <v>855.9094820734193</v>
       </c>
-      <c r="W37" s="13">
+      <c r="W37" s="12">
         <f>ROUND((V37-U37)/U37,5)</f>
         <v/>
       </c>
     </row>
-    <row r="38" ht="15" customHeight="1" s="18">
+    <row r="38" ht="15" customHeight="1" s="15">
       <c r="A38" t="n">
         <v>6</v>
       </c>
@@ -8094,11 +7701,11 @@
       <c r="K38" t="n">
         <v>678.148251762738</v>
       </c>
-      <c r="M38" s="12">
+      <c r="M38" s="11">
         <f>ROUND((K38-G38)/G38,5)</f>
         <v/>
       </c>
-      <c r="N38" s="12" t="inlineStr">
+      <c r="N38" s="11" t="inlineStr">
         <is>
           <t>{"0": [[[5, 6], [6, 6]]], "1": [[[1, 7], [4, 13]], [[3, 19]], [[2, 15]]], "2": [[]]}</t>
         </is>
@@ -8121,11 +7728,11 @@
       <c r="Q38" t="n">
         <v>659.7577073740965</v>
       </c>
-      <c r="R38" s="12">
+      <c r="R38" s="11">
         <f>ROUND((Q38-G38)/G38,5)</f>
         <v/>
       </c>
-      <c r="S38" s="13">
+      <c r="S38" s="12">
         <f>ROUND((Q38-K38)/K38,5)</f>
         <v/>
       </c>
@@ -8135,12 +7742,12 @@
       <c r="V38" t="n">
         <v>604.4934696287221</v>
       </c>
-      <c r="W38" s="13">
+      <c r="W38" s="12">
         <f>ROUND((V38-U38)/U38,5)</f>
         <v/>
       </c>
     </row>
-    <row r="39" ht="15" customHeight="1" s="18">
+    <row r="39" ht="15" customHeight="1" s="15">
       <c r="A39" t="n">
         <v>6</v>
       </c>
@@ -8201,11 +7808,11 @@
       <c r="K39" t="n">
         <v>938.3525456101431</v>
       </c>
-      <c r="M39" s="12">
+      <c r="M39" s="11">
         <f>ROUND((K39-G39)/G39,5)</f>
         <v/>
       </c>
-      <c r="N39" s="12" t="inlineStr">
+      <c r="N39" s="11" t="inlineStr">
         <is>
           <t>{"0": [[[1, 11]], [[5, 14]]], "1": [[[6, 20], [2, 6]], [[4, 18], [3, 10]]]}</t>
         </is>
@@ -8227,11 +7834,11 @@
       <c r="Q39" t="n">
         <v>938.3525456101431</v>
       </c>
-      <c r="R39" s="12">
+      <c r="R39" s="11">
         <f>ROUND((Q39-G39)/G39,5)</f>
         <v/>
       </c>
-      <c r="S39" s="13">
+      <c r="S39" s="12">
         <f>ROUND((Q39-K39)/K39,5)</f>
         <v/>
       </c>
@@ -8241,7 +7848,7 @@
       <c r="V39" t="n">
         <v>868.0017542131443</v>
       </c>
-      <c r="W39" s="13">
+      <c r="W39" s="12">
         <f>ROUND((V39-U39)/U39,5)</f>
         <v/>
       </c>
@@ -8306,11 +7913,11 @@
       <c r="K40" t="n">
         <v>941.6268761430824</v>
       </c>
-      <c r="M40" s="12">
+      <c r="M40" s="11">
         <f>ROUND((K40-G40)/G40,5)</f>
         <v/>
       </c>
-      <c r="N40" s="12" t="inlineStr">
+      <c r="N40" s="11" t="inlineStr">
         <is>
           <t>{"0": [[[6, 10], [3, 6]]], "1": [[[5, 14], [2, 10]]], "2": [[[1, 14], [4, 4]]]}</t>
         </is>
@@ -8332,11 +7939,11 @@
       <c r="Q40" t="n">
         <v>941.6268761430824</v>
       </c>
-      <c r="R40" s="12">
+      <c r="R40" s="11">
         <f>ROUND((Q40-G40)/G40,5)</f>
         <v/>
       </c>
-      <c r="S40" s="13">
+      <c r="S40" s="12">
         <f>ROUND((Q40-K40)/K40,5)</f>
         <v/>
       </c>
@@ -8346,7 +7953,7 @@
       <c r="V40" t="n">
         <v>898.2859176189384</v>
       </c>
-      <c r="W40" s="13">
+      <c r="W40" s="12">
         <f>ROUND((V40-U40)/U40,5)</f>
         <v/>
       </c>
@@ -8411,11 +8018,11 @@
       <c r="K41" t="n">
         <v>672.476663216454</v>
       </c>
-      <c r="M41" s="12">
+      <c r="M41" s="11">
         <f>ROUND((K41-G41)/G41,5)</f>
         <v/>
       </c>
-      <c r="N41" s="12" t="inlineStr">
+      <c r="N41" s="11" t="inlineStr">
         <is>
           <t>{"0": [[[3, 10], [4, 8], [5, 2]], [[1, 11]]], "1": [[[2, 13], [6, 14]]], "2": [[]]}</t>
         </is>
@@ -8437,11 +8044,11 @@
       <c r="Q41" t="n">
         <v>672.476663216454</v>
       </c>
-      <c r="R41" s="12">
+      <c r="R41" s="11">
         <f>ROUND((Q41-G41)/G41,5)</f>
         <v/>
       </c>
-      <c r="S41" s="13">
+      <c r="S41" s="12">
         <f>ROUND((Q41-K41)/K41,5)</f>
         <v/>
       </c>
@@ -8451,7 +8058,7 @@
       <c r="V41" t="n">
         <v>640.3964061684818</v>
       </c>
-      <c r="W41" s="13">
+      <c r="W41" s="12">
         <f>ROUND((V41-U41)/U41,5)</f>
         <v/>
       </c>
@@ -8521,11 +8128,11 @@
       <c r="K42" t="n">
         <v>893.2598344845564</v>
       </c>
-      <c r="M42" s="12">
+      <c r="M42" s="11">
         <f>ROUND((K42-G42)/G42,5)</f>
         <v/>
       </c>
-      <c r="N42" s="12" t="inlineStr">
+      <c r="N42" s="11" t="inlineStr">
         <is>
           <t>{"0": [[[6, 3], [3, 5], [1, 4], [9, 6], [7, 10]], [[4, 11], [2, 2], [5, 8], [8, 1]]], "1": [[]], "2": [[]]}</t>
         </is>
@@ -8541,16 +8148,16 @@
         </is>
       </c>
       <c r="P42" t="n">
-        <v>257.9822673999997</v>
+        <v>210.1581165</v>
       </c>
       <c r="Q42" t="n">
         <v>893.2598344845563</v>
       </c>
-      <c r="R42" s="12">
+      <c r="R42" s="11">
         <f>ROUND((Q42-G42)/G42,5)</f>
         <v/>
       </c>
-      <c r="S42" s="13">
+      <c r="S42" s="12">
         <f>ROUND((Q42-K42)/K42,5)</f>
         <v/>
       </c>
@@ -8560,7 +8167,7 @@
       <c r="V42" t="n">
         <v>826.9229303309405</v>
       </c>
-      <c r="W42" s="13">
+      <c r="W42" s="12">
         <f>ROUND((V42-U42)/U42,5)</f>
         <v/>
       </c>
@@ -8629,38 +8236,38 @@
         </is>
       </c>
       <c r="K43" t="n">
-        <v>813.8242183113271</v>
-      </c>
-      <c r="M43" s="12">
+        <v>821.8736830120431</v>
+      </c>
+      <c r="M43" s="11">
         <f>ROUND((K43-G43)/G43,5)</f>
         <v/>
       </c>
-      <c r="N43" s="12" t="inlineStr">
-        <is>
-          <t>{"0": [[[1, 1], [5, 13], [2, 2], [8, 12]], [[9, 8], [7, 9]], [[4, 14], [3, 2], [6, 7]]], "1": [[]]}</t>
+      <c r="N43" s="11" t="inlineStr">
+        <is>
+          <t>{"0": [[[1, 1], [5, 13], [2, 2], [8, 12]], [[6, 7], [3, 2], [4, 14]], [[7, 9], [9, 8]]], "1": [[]]}</t>
         </is>
       </c>
       <c r="O43" t="inlineStr">
         <is>
           <t xml:space="preserve">11 metre (capacity 30):
 1 (1) -&gt; 5 (13) -&gt; 2 (2) -&gt; 8 (12)
-9 (8) -&gt; 7 (9)
-4 (14) -&gt; 3 (2) -&gt; 6 (7)
+6 (7) -&gt; 3 (2) -&gt; 4 (14)
+7 (9) -&gt; 9 (8)
 Rigid (capacity 16):
 </t>
         </is>
       </c>
       <c r="P43" t="n">
-        <v>274.2841185999996</v>
+        <v>251.2256288999999</v>
       </c>
       <c r="Q43" t="n">
         <v>821.8736830120431</v>
       </c>
-      <c r="R43" s="12">
+      <c r="R43" s="11">
         <f>ROUND((Q43-G43)/G43,5)</f>
         <v/>
       </c>
-      <c r="S43" s="13">
+      <c r="S43" s="12">
         <f>ROUND((Q43-K43)/K43,5)</f>
         <v/>
       </c>
@@ -8668,9 +8275,9 @@
         <v>743.6205606708595</v>
       </c>
       <c r="V43" t="n">
-        <v>743.6205606708596</v>
-      </c>
-      <c r="W43" s="13">
+        <v>743.6205606708594</v>
+      </c>
+      <c r="W43" s="12">
         <f>ROUND((V43-U43)/U43,5)</f>
         <v/>
       </c>
@@ -8742,11 +8349,11 @@
       <c r="K44" t="n">
         <v>777.7085678113841</v>
       </c>
-      <c r="M44" s="12">
+      <c r="M44" s="11">
         <f>ROUND((K44-G44)/G44,5)</f>
         <v/>
       </c>
-      <c r="N44" s="12" t="inlineStr">
+      <c r="N44" s="11" t="inlineStr">
         <is>
           <t>{"0": [[[1, 10], [9, 10], [5, 9], [7, 1]]], "1": [[[3, 1], [2, 15], [6, 3]]], "2": [[[4, 9], [8, 7]]]}</t>
         </is>
@@ -8768,11 +8375,11 @@
       <c r="Q44" t="n">
         <v>815.6774550162049</v>
       </c>
-      <c r="R44" s="12">
+      <c r="R44" s="11">
         <f>ROUND((Q44-G44)/G44,5)</f>
         <v/>
       </c>
-      <c r="S44" s="13">
+      <c r="S44" s="12">
         <f>ROUND((Q44-K44)/K44,5)</f>
         <v/>
       </c>
@@ -8782,7 +8389,7 @@
       <c r="V44" t="n">
         <v>738.6881272862269</v>
       </c>
-      <c r="W44" s="13">
+      <c r="W44" s="12">
         <f>ROUND((V44-U44)/U44,5)</f>
         <v/>
       </c>
@@ -8850,38 +8457,38 @@
         </is>
       </c>
       <c r="K45" t="n">
-        <v>908.1004723180679</v>
-      </c>
-      <c r="M45" s="12">
+        <v>914.6883021565079</v>
+      </c>
+      <c r="M45" s="11">
         <f>ROUND((K45-G45)/G45,5)</f>
         <v/>
       </c>
-      <c r="N45" s="12" t="inlineStr">
-        <is>
-          <t>{"0": [[[5, 3], [3, 7], [1, 13], [6, 3], [9, 4]], [[4, 2], [8, 11], [2, 7], [7, 1]]], "1": [[]], "2": [[]]}</t>
+      <c r="N45" s="11" t="inlineStr">
+        <is>
+          <t>{"0": [[[3, 7], [1, 13], [6, 3], [9, 4]], [[4, 2], [8, 11], [2, 7], [7, 1], [5, 3]]], "1": [[]], "2": [[]]}</t>
         </is>
       </c>
       <c r="O45" t="inlineStr">
         <is>
           <t xml:space="preserve">11 metre (capacity 30):
-5 (3) -&gt; 3 (7) -&gt; 1 (13) -&gt; 6 (3) -&gt; 9 (4)
-4 (2) -&gt; 8 (11) -&gt; 2 (7) -&gt; 7 (1)
+3 (7) -&gt; 1 (13) -&gt; 6 (3) -&gt; 9 (4)
+4 (2) -&gt; 8 (11) -&gt; 2 (7) -&gt; 7 (1) -&gt; 5 (3)
 8 metre (capacity 22):
 Rigid (capacity 16):
 </t>
         </is>
       </c>
       <c r="P45" t="n">
-        <v>274.9465521000002</v>
+        <v>258.476064</v>
       </c>
       <c r="Q45" t="n">
-        <v>916.2204632570621</v>
-      </c>
-      <c r="R45" s="12">
+        <v>914.6883021565079</v>
+      </c>
+      <c r="R45" s="11">
         <f>ROUND((Q45-G45)/G45,5)</f>
         <v/>
       </c>
-      <c r="S45" s="13">
+      <c r="S45" s="12">
         <f>ROUND((Q45-K45)/K45,5)</f>
         <v/>
       </c>
@@ -8889,9 +8496,9 @@
         <v>867.0337789998922</v>
       </c>
       <c r="V45" t="n">
-        <v>868.5659401004465</v>
-      </c>
-      <c r="W45" s="13">
+        <v>867.0337789998922</v>
+      </c>
+      <c r="W45" s="12">
         <f>ROUND((V45-U45)/U45,5)</f>
         <v/>
       </c>
@@ -8960,13 +8567,13 @@
         </is>
       </c>
       <c r="K46" t="n">
-        <v>1026.007817134059</v>
-      </c>
-      <c r="M46" s="12">
+        <v>1008.26305168901</v>
+      </c>
+      <c r="M46" s="11">
         <f>ROUND((K46-G46)/G46,5)</f>
         <v/>
       </c>
-      <c r="N46" s="12" t="inlineStr">
+      <c r="N46" s="11" t="inlineStr">
         <is>
           <t>{"0": [[[6, 3], [4, 4], [2, 13], [7, 6]], [[8, 14], [1, 9]], [[5, 11], [9, 1], [3, 8]]]}</t>
         </is>
@@ -8981,16 +8588,16 @@
         </is>
       </c>
       <c r="P46" t="n">
-        <v>439.0288809000003</v>
+        <v>406.0763162999997</v>
       </c>
       <c r="Q46" t="n">
-        <v>1049.547039018111</v>
-      </c>
-      <c r="R46" s="12">
+        <v>1044.262178499589</v>
+      </c>
+      <c r="R46" s="11">
         <f>ROUND((Q46-G46)/G46,5)</f>
         <v/>
       </c>
-      <c r="S46" s="13">
+      <c r="S46" s="12">
         <f>ROUND((Q46-K46)/K46,5)</f>
         <v/>
       </c>
@@ -9000,7 +8607,7 @@
       <c r="V46" t="n">
         <v>904.1962709155146</v>
       </c>
-      <c r="W46" s="13">
+      <c r="W46" s="12">
         <f>ROUND((V46-U46)/U46,5)</f>
         <v/>
       </c>
@@ -9071,11 +8678,11 @@
       <c r="K47" t="n">
         <v>843.3479719678728</v>
       </c>
-      <c r="M47" s="12">
+      <c r="M47" s="11">
         <f>ROUND((K47-G47)/G47,5)</f>
         <v/>
       </c>
-      <c r="N47" s="12" t="inlineStr">
+      <c r="N47" s="11" t="inlineStr">
         <is>
           <t>{"0": [[[7, 1], [2, 4], [4, 8], [9, 3], [5, 5]], [[6, 12]]], "1": [[]], "2": [[[3, 8], [8, 10], [1, 12]]]}</t>
         </is>
@@ -9097,11 +8704,11 @@
       <c r="Q47" t="n">
         <v>843.3479719678728</v>
       </c>
-      <c r="R47" s="12">
+      <c r="R47" s="11">
         <f>ROUND((Q47-G47)/G47,5)</f>
         <v/>
       </c>
-      <c r="S47" s="13">
+      <c r="S47" s="12">
         <f>ROUND((Q47-K47)/K47,5)</f>
         <v/>
       </c>
@@ -9111,7 +8718,7 @@
       <c r="V47" t="n">
         <v>790.211040984113</v>
       </c>
-      <c r="W47" s="13">
+      <c r="W47" s="12">
         <f>ROUND((V47-U47)/U47,5)</f>
         <v/>
       </c>
@@ -9180,39 +8787,39 @@
         </is>
       </c>
       <c r="K48" t="n">
-        <v>677.6161090392966</v>
-      </c>
-      <c r="M48" s="12">
+        <v>693.9133650269337</v>
+      </c>
+      <c r="M48" s="11">
         <f>ROUND((K48-G48)/G48,5)</f>
         <v/>
       </c>
-      <c r="N48" s="12" t="inlineStr">
-        <is>
-          <t>{"0": [[[3, 1], [1, 1], [2, 10]], [[6, 5], [8, 11], [7, 1], [4, 4]], [[5, 8], [9, 3]]], "1": [[]], "2": [[]]}</t>
+      <c r="N48" s="11" t="inlineStr">
+        <is>
+          <t>{"0": [[[2, 10], [1, 1], [3, 1]], [[5, 8], [9, 3]], [[4, 4], [7, 1], [8, 11], [6, 5]]], "1": [[]], "2": [[]]}</t>
         </is>
       </c>
       <c r="O48" t="inlineStr">
         <is>
           <t xml:space="preserve">11 metre (capacity 30):
-3 (1) -&gt; 1 (1) -&gt; 2 (10)
-6 (5) -&gt; 8 (11) -&gt; 7 (1) -&gt; 4 (4)
+2 (10) -&gt; 1 (1) -&gt; 3 (1)
 5 (8) -&gt; 9 (3)
+4 (4) -&gt; 7 (1) -&gt; 8 (11) -&gt; 6 (5)
 8 metre (capacity 22):
 Rigid (capacity 16):
 </t>
         </is>
       </c>
       <c r="P48" t="n">
-        <v>296.5032604999997</v>
+        <v>304.6506844</v>
       </c>
       <c r="Q48" t="n">
-        <v>693.9133650269338</v>
-      </c>
-      <c r="R48" s="12">
+        <v>693.9133650269337</v>
+      </c>
+      <c r="R48" s="11">
         <f>ROUND((Q48-G48)/G48,5)</f>
         <v/>
       </c>
-      <c r="S48" s="13">
+      <c r="S48" s="12">
         <f>ROUND((Q48-K48)/K48,5)</f>
         <v/>
       </c>
@@ -9220,9 +8827,9 @@
         <v>636.7042369162627</v>
       </c>
       <c r="V48" t="n">
-        <v>636.7042369162626</v>
-      </c>
-      <c r="W48" s="13">
+        <v>636.7042369162627</v>
+      </c>
+      <c r="W48" s="12">
         <f>ROUND((V48-U48)/U48,5)</f>
         <v/>
       </c>
@@ -9292,11 +8899,11 @@
       <c r="K49" t="n">
         <v>607.1439817452525</v>
       </c>
-      <c r="M49" s="12">
+      <c r="M49" s="11">
         <f>ROUND((K49-G49)/G49,5)</f>
         <v/>
       </c>
-      <c r="N49" s="12" t="inlineStr">
+      <c r="N49" s="11" t="inlineStr">
         <is>
           <t>{"0": [[]], "1": [[[5, 2], [9, 13], [4, 5], [7, 4]], [[2, 8], [6, 8], [3, 3], [8, 8], [1, 3]]], "2": [[]]}</t>
         </is>
@@ -9317,11 +8924,11 @@
       <c r="Q49" t="n">
         <v>607.1439817452524</v>
       </c>
-      <c r="R49" s="12">
+      <c r="R49" s="11">
         <f>ROUND((Q49-G49)/G49,5)</f>
         <v/>
       </c>
-      <c r="S49" s="13">
+      <c r="S49" s="12">
         <f>ROUND((Q49-K49)/K49,5)</f>
         <v/>
       </c>
@@ -9331,7 +8938,7 @@
       <c r="V49" t="n">
         <v>564.953581224465</v>
       </c>
-      <c r="W49" s="13">
+      <c r="W49" s="12">
         <f>ROUND((V49-U49)/U49,5)</f>
         <v/>
       </c>
@@ -9401,40 +9008,40 @@
         </is>
       </c>
       <c r="K50" t="n">
-        <v>1030.015770167636</v>
-      </c>
-      <c r="M50" s="12">
+        <v>1019.716741712636</v>
+      </c>
+      <c r="M50" s="11">
         <f>ROUND((K50-G50)/G50,5)</f>
         <v/>
       </c>
-      <c r="N50" s="12" t="inlineStr">
-        <is>
-          <t>{"0": [[[4, 10], [8, 2]], [[9, 3], [6, 11]]], "1": [[[7, 8], [1, 10]]], "2": [[[5, 12], [2, 2], [3, 11]]]}</t>
+      <c r="N50" s="11" t="inlineStr">
+        <is>
+          <t>{"0": [[[5, 12]], [[6, 11], [9, 3]]], "1": [[[1, 10], [7, 8]]], "2": [[[8, 2], [4, 10], [3, 11], [2, 2]]]}</t>
         </is>
       </c>
       <c r="O50" t="inlineStr">
         <is>
           <t xml:space="preserve">Rigid (capacity 16):
-4 (10) -&gt; 8 (2)
-9 (3) -&gt; 6 (11)
+5 (12)
+6 (11) -&gt; 9 (3)
 8 metre (capacity 22):
-7 (8) -&gt; 1 (10)
+1 (10) -&gt; 7 (8)
 11 metre (capacity 30):
-5 (12) -&gt; 2 (2) -&gt; 3 (11)
+8 (2) -&gt; 4 (10) -&gt; 3 (11) -&gt; 2 (2)
 </t>
         </is>
       </c>
       <c r="P50" t="n">
-        <v>272.1558544</v>
+        <v>284.4718016000002</v>
       </c>
       <c r="Q50" t="n">
-        <v>1022.05857548553</v>
-      </c>
-      <c r="R50" s="12">
+        <v>1019.716741712636</v>
+      </c>
+      <c r="R50" s="11">
         <f>ROUND((Q50-G50)/G50,5)</f>
         <v/>
       </c>
-      <c r="S50" s="13">
+      <c r="S50" s="12">
         <f>ROUND((Q50-K50)/K50,5)</f>
         <v/>
       </c>
@@ -9442,9 +9049,9 @@
         <v>945.8806700601344</v>
       </c>
       <c r="V50" t="n">
-        <v>952.3127395564161</v>
-      </c>
-      <c r="W50" s="13">
+        <v>945.8806700601344</v>
+      </c>
+      <c r="W50" s="12">
         <f>ROUND((V50-U50)/U50,5)</f>
         <v/>
       </c>
@@ -9516,37 +9123,37 @@
       <c r="K51" t="n">
         <v>904.5378082988403</v>
       </c>
-      <c r="M51" s="12">
+      <c r="M51" s="11">
         <f>ROUND((K51-G51)/G51,5)</f>
         <v/>
       </c>
-      <c r="N51" s="12" t="inlineStr">
-        <is>
-          <t>{"0": [[[9, 8], [2, 6]], [[6, 5]]], "1": [[[3, 8], [5, 9], [1, 1], [4, 2]], [[8, 11], [7, 10]]]}</t>
+      <c r="N51" s="11" t="inlineStr">
+        <is>
+          <t>{"0": [[[6, 5]], [[2, 6], [9, 8]]], "1": [[[4, 2], [1, 1], [5, 9], [3, 8]], [[8, 11], [7, 10]]]}</t>
         </is>
       </c>
       <c r="O51" t="inlineStr">
         <is>
           <t xml:space="preserve">Rigid (capacity 16):
-9 (8) -&gt; 2 (6)
 6 (5)
+2 (6) -&gt; 9 (8)
 8 metre (capacity 22):
-3 (8) -&gt; 5 (9) -&gt; 1 (1) -&gt; 4 (2)
+4 (2) -&gt; 1 (1) -&gt; 5 (9) -&gt; 3 (8)
 8 (11) -&gt; 7 (10)
 </t>
         </is>
       </c>
       <c r="P51" t="n">
-        <v>257.0605992</v>
+        <v>261.9934125</v>
       </c>
       <c r="Q51" t="n">
         <v>904.5378082988403</v>
       </c>
-      <c r="R51" s="12">
+      <c r="R51" s="11">
         <f>ROUND((Q51-G51)/G51,5)</f>
         <v/>
       </c>
-      <c r="S51" s="13">
+      <c r="S51" s="12">
         <f>ROUND((Q51-K51)/K51,5)</f>
         <v/>
       </c>
@@ -9556,7 +9163,7 @@
       <c r="V51" t="n">
         <v>861.6615285311618</v>
       </c>
-      <c r="W51" s="13">
+      <c r="W51" s="12">
         <f>ROUND((V51-U51)/U51,5)</f>
         <v/>
       </c>
@@ -9634,37 +9241,37 @@
       <c r="K52" t="n">
         <v>1210.828177855486</v>
       </c>
-      <c r="M52" s="12">
+      <c r="M52" s="11">
         <f>ROUND((K52-G52)/G52,5)</f>
         <v/>
       </c>
-      <c r="N52" s="12" t="inlineStr">
-        <is>
-          <t>{"0": [[[10, 5], [6, 10], [3, 8], [9, 5], [12, 2]], [[1, 2], [7, 6], [11, 9], [2, 7]]], "1": [[]], "2": [[[5, 5], [8, 6], [4, 8]]]}</t>
+      <c r="N52" s="11" t="inlineStr">
+        <is>
+          <t>{"0": [[[2, 7], [11, 9], [7, 6], [1, 2]], [[10, 5], [6, 10], [3, 8], [9, 5], [12, 2]]], "1": [[]], "2": [[[4, 8], [8, 6], [5, 5]]]}</t>
         </is>
       </c>
       <c r="O52" t="inlineStr">
         <is>
           <t xml:space="preserve">11 metre (capacity 30):
+2 (7) -&gt; 11 (9) -&gt; 7 (6) -&gt; 1 (2)
 10 (5) -&gt; 6 (10) -&gt; 3 (8) -&gt; 9 (5) -&gt; 12 (2)
-1 (2) -&gt; 7 (6) -&gt; 11 (9) -&gt; 2 (7)
 Rigid (capacity 16):
 8 metre (capacity 22):
-5 (5) -&gt; 8 (6) -&gt; 4 (8)
+4 (8) -&gt; 8 (6) -&gt; 5 (5)
 </t>
         </is>
       </c>
       <c r="P52" t="n">
-        <v>402.1164343</v>
+        <v>399.6152930000003</v>
       </c>
       <c r="Q52" t="n">
         <v>1222.399933248278</v>
       </c>
-      <c r="R52" s="12">
+      <c r="R52" s="11">
         <f>ROUND((Q52-G52)/G52,5)</f>
         <v/>
       </c>
-      <c r="S52" s="13">
+      <c r="S52" s="12">
         <f>ROUND((Q52-K52)/K52,5)</f>
         <v/>
       </c>
@@ -9674,7 +9281,7 @@
       <c r="V52" t="n">
         <v>1126.916567567835</v>
       </c>
-      <c r="W52" s="13">
+      <c r="W52" s="12">
         <f>ROUND((V52-U52)/U52,5)</f>
         <v/>
       </c>
@@ -9753,11 +9360,11 @@
       <c r="K53" t="n">
         <v>928.2943130868078</v>
       </c>
-      <c r="M53" s="12">
+      <c r="M53" s="11">
         <f>ROUND((K53-G53)/G53,5)</f>
         <v/>
       </c>
-      <c r="N53" s="12" t="inlineStr">
+      <c r="N53" s="11" t="inlineStr">
         <is>
           <t>{"0": [[[3, 2], [6, 2], [11, 5]], [[5, 5], [9, 4], [7, 4], [8, 3]], [[2, 8], [10, 1], [4, 1], [12, 3]]], "1": [[[1, 8]]]}</t>
         </is>
@@ -9779,11 +9386,11 @@
       <c r="Q53" t="n">
         <v>959.7170923181206</v>
       </c>
-      <c r="R53" s="12">
+      <c r="R53" s="11">
         <f>ROUND((Q53-G53)/G53,5)</f>
         <v/>
       </c>
-      <c r="S53" s="13">
+      <c r="S53" s="12">
         <f>ROUND((Q53-K53)/K53,5)</f>
         <v/>
       </c>
@@ -9793,7 +9400,7 @@
       <c r="V53" t="n">
         <v>900.9017217174928</v>
       </c>
-      <c r="W53" s="13">
+      <c r="W53" s="12">
         <f>ROUND((V53-U53)/U53,5)</f>
         <v/>
       </c>
@@ -9862,20 +9469,20 @@
 Solve time: 385349</t>
         </is>
       </c>
-      <c r="M54" s="12">
+      <c r="M54" s="11">
         <f>ROUND((K54-G54)/G54,5)</f>
         <v/>
       </c>
-      <c r="N54" s="12" t="n"/>
-      <c r="R54" s="12">
+      <c r="N54" s="11" t="n"/>
+      <c r="R54" s="11">
         <f>ROUND((Q54-G54)/G54,5)</f>
         <v/>
       </c>
-      <c r="S54" s="13">
+      <c r="S54" s="12">
         <f>ROUND((Q54-K54)/K54,5)</f>
         <v/>
       </c>
-      <c r="W54" s="13">
+      <c r="W54" s="12">
         <f>ROUND((V54-U54)/U54,5)</f>
         <v/>
       </c>
@@ -9944,20 +9551,20 @@
 Solve time: 145025</t>
         </is>
       </c>
-      <c r="M55" s="12">
+      <c r="M55" s="11">
         <f>ROUND((K55-G55)/G55,5)</f>
         <v/>
       </c>
-      <c r="N55" s="12" t="n"/>
-      <c r="R55" s="12">
+      <c r="N55" s="11" t="n"/>
+      <c r="R55" s="11">
         <f>ROUND((Q55-G55)/G55,5)</f>
         <v/>
       </c>
-      <c r="S55" s="13">
+      <c r="S55" s="12">
         <f>ROUND((Q55-K55)/K55,5)</f>
         <v/>
       </c>
-      <c r="W55" s="13">
+      <c r="W55" s="12">
         <f>ROUND((V55-U55)/U55,5)</f>
         <v/>
       </c>
@@ -10026,25 +9633,25 @@
 Solve time: 430708</t>
         </is>
       </c>
-      <c r="M56" s="12">
+      <c r="M56" s="11">
         <f>ROUND((K56-G56)/G56,5)</f>
         <v/>
       </c>
-      <c r="N56" s="12" t="n"/>
-      <c r="R56" s="12">
+      <c r="N56" s="11" t="n"/>
+      <c r="R56" s="11">
         <f>ROUND((Q56-G56)/G56,5)</f>
         <v/>
       </c>
-      <c r="S56" s="13">
+      <c r="S56" s="12">
         <f>ROUND((Q56-K56)/K56,5)</f>
         <v/>
       </c>
-      <c r="W56" s="13">
+      <c r="W56" s="12">
         <f>ROUND((V56-U56)/U56,5)</f>
         <v/>
       </c>
     </row>
-    <row r="57">
+    <row r="57" ht="15" customHeight="1" s="15">
       <c r="A57" t="n">
         <v>12</v>
       </c>
@@ -10062,26 +9669,71 @@
         <f>F57/1000</f>
         <v/>
       </c>
-      <c r="H57" s="16" t="n"/>
-      <c r="M57" s="12">
+      <c r="F57" t="n">
+        <v>2335436</v>
+      </c>
+      <c r="G57" t="n">
+        <v>1235.52305333</v>
+      </c>
+      <c r="H57" s="16" t="inlineStr">
+        <is>
+          <t>Input:
+Customer 1 has 2 pallets demand and window 0-24 at (9.323766392, -75.027154434) and average unload time 0.153863026
+Customer 2 has 5 pallets demand and window 0-24 at (-54.026006389, 31.120934846) and average unload time 0.16309667
+Customer 3 has 12 pallets demand and window 0-24 at (61.353022315, 9.197128971) and average unload time 0.081370108
+Customer 4 has 4 pallets demand and window 0-24 at (92.463302392, 34.781071736) and average unload time 0.051990036
+Customer 5 has 4 pallets demand and window 17-18 at (40.33825566, -89.267972485) and average unload time 0.038344625
+Customer 6 has 1 pallets demand and window 0-24 at (84.176793096, 18.764110183) and average unload time 0.089213447
+Customer 7 has 2 pallets demand and window 0-24 at (-25.143650218, 37.440034642) and average unload time 0.117293614
+Customer 8 has 10 pallets demand and window 0-24 at (-92.502826604, -45.905170828) and average unload time 0.041220897
+Customer 9 has 5 pallets demand and window 0-24 at (-30.383074534, -14.636752348) and average unload time 0.157216861
+Customer 10 has 9 pallets demand and window 0-24 at (36.88861806, -73.065528774) and average unload time 0.108515697
+Customer 11 has 9 pallets demand and window 0-24 at (-28.703191014, -43.834436797) and average unload time 0.15624806
+Customer 12 has 12 pallets demand and window 19-20 at (-55.176741996, 98.086344662) and average unload time 0.090735057
+Vehicle SP1 is a 8 metre with capacity 22, distance cost 1.110220405, and time cost 11.507600006
+Vehicle SP2 is a 11 metre with capacity 30, distance cost 1.30225705, and time cost 12.003990304
+Vehicle SP3 is a 8 metre with capacity 22, distance cost 1.110220405, and time cost 11.507600006
+Vehicle SP4 is a 11 metre with capacity 30, distance cost 1.30225705, and time cost 12.003990304
+Vehicle SP5 is a 11 metre with capacity 30, distance cost 1.30225705, and time cost 12.003990304
+Output:
+Vehicle SP2 travels from Depot to 8 to deliver 10 pallets. Expected unload start time is 16.8588464
+Vehicle SP2 travels from 2 to 12 to deliver 12 pallets. Expected unload start time is 20
+Vehicle SP2 travels from 7 to DepotReturn to deliver 0 pallets. Expected unload start time is 22.733093549
+Vehicle SP2 travels from 8 to 2 to deliver 5 pallets. Expected unload start time is 18.347325448
+Vehicle SP2 travels from 12 to 7 to deliver 2 pallets. Expected unload start time is 21.934763342
+Vehicle SP3 travels from Depot to 4 to deliver 4 pallets. Expected unload start time is 21.41613685
+Vehicle SP3 travels from 3 to DepotReturn to deliver 0 pallets. Expected unload start time is 24
+Vehicle SP3 travels from 4 to 6 to deliver 1 pallets. Expected unload start time is 21.849516495
+Vehicle SP3 travels from 6 to 3 to deliver 12 pallets. Expected unload start time is 22.248076947
+Vehicle SP4 travels from Depot to 10 to deliver 9 pallets. Expected unload start time is 16.816288701
+Vehicle SP4 travels from 1 to 11 to deliver 9 pallets. Expected unload start time is 19.50249681
+Vehicle SP4 travels from 5 to 1 to deliver 2 pallets. Expected unload start time is 18.579974664
+Vehicle SP4 travels from 9 to DepotReturn to deliver 0 pallets. Expected unload start time is 22.481948952
+Vehicle SP4 travels from 10 to 5 to deliver 4 pallets. Expected unload start time is 18
+Vehicle SP4 travels from 11 to 9 to deliver 5 pallets. Expected unload start time is 21.274303981
+Objective value: 1235.52305333
+Solve time: 2335436</t>
+        </is>
+      </c>
+      <c r="M57" s="11">
         <f>ROUND((K57-G57)/G57,5)</f>
         <v/>
       </c>
-      <c r="N57" s="12" t="n"/>
-      <c r="R57" s="12">
+      <c r="N57" s="11" t="n"/>
+      <c r="R57" s="11">
         <f>ROUND((Q57-G57)/G57,5)</f>
         <v/>
       </c>
-      <c r="S57" s="13">
+      <c r="S57" s="12">
         <f>ROUND((Q57-K57)/K57,5)</f>
         <v/>
       </c>
-      <c r="W57" s="13">
+      <c r="W57" s="12">
         <f>ROUND((V57-U57)/U57,5)</f>
         <v/>
       </c>
     </row>
-    <row r="58">
+    <row r="58" ht="15" customHeight="1" s="15">
       <c r="A58" t="n">
         <v>12</v>
       </c>
@@ -10099,26 +9751,71 @@
         <f>F58/1000</f>
         <v/>
       </c>
-      <c r="H58" s="16" t="n"/>
-      <c r="M58" s="12">
+      <c r="F58" t="n">
+        <v>2049569</v>
+      </c>
+      <c r="G58" t="n">
+        <v>1079.070671831</v>
+      </c>
+      <c r="H58" s="16" t="inlineStr">
+        <is>
+          <t>Input:
+Customer 1 has 6 pallets demand and window 0-24 at (-73.452381273, 54.047136339) and average unload time 0.056688615
+Customer 2 has 3 pallets demand and window 13-14 at (78.971068732, 92.091115195) and average unload time 0.164007106
+Customer 3 has 1 pallets demand and window 0-24 at (58.865778175, 12.797703305) and average unload time 0.133102341
+Customer 4 has 2 pallets demand and window 0-24 at (-50.643364047, -50.936646305) and average unload time 0.03605971
+Customer 5 has 2 pallets demand and window 0-24 at (-96.061971128, 78.200037067) and average unload time 0.088519892
+Customer 6 has 8 pallets demand and window 0-24 at (71.372072565, -38.643780593) and average unload time 0.153633964
+Customer 7 has 10 pallets demand and window 14-15 at (-66.614349811, -78.088687705) and average unload time 0.070560553
+Customer 8 has 6 pallets demand and window 0-24 at (-91.138642303, -18.646419267) and average unload time 0.133443936
+Customer 9 has 5 pallets demand and window 0-24 at (-76.707027158, 34.045959793) and average unload time 0.135998893
+Customer 10 has 1 pallets demand and window 0-24 at (-66.163558086, -14.947527817) and average unload time 0.024720712
+Customer 11 has 4 pallets demand and window 0-24 at (31.702870939, -1.159319746) and average unload time 0.143820536
+Customer 12 has 10 pallets demand and window 0-24 at (99.79328855, -32.38261543) and average unload time 0.114075372
+Vehicle SP1 is a 8 metre with capacity 22, distance cost 1.28417055, and time cost 9.780776843
+Vehicle SP2 is a 11 metre with capacity 30, distance cost 0.975382084, and time cost 13.518983981
+Vehicle SP3 is a Rigid with capacity 16, distance cost 0.924896712, and time cost 8.940937184
+Vehicle SP4 is a Rigid with capacity 16, distance cost 0.924896712, and time cost 8.940937184
+Vehicle SP5 is a 11 metre with capacity 30, distance cost 0.975382084, and time cost 13.518983981
+Output:
+Vehicle SP2 travels from Depot to 10 to deliver 1 pallets. Expected unload start time is 13.055239344
+Vehicle SP2 travels from 4 to DepotReturn to deliver 0 pallets. Expected unload start time is 17.069338678
+Vehicle SP2 travels from 7 to 4 to deliver 2 pallets. Expected unload start time is 16.09936659
+Vehicle SP2 travels from 8 to 7 to deliver 10 pallets. Expected unload start time is 15
+Vehicle SP2 travels from 10 to 8 to deliver 6 pallets. Expected unload start time is 13.395553898
+Vehicle SP4 travels from Depot to 1 to deliver 6 pallets. Expected unload start time is 1.139924974
+Vehicle SP4 travels from 1 to 5 to deliver 2 pallets. Expected unload start time is 1.893607629
+Vehicle SP4 travels from 5 to 9 to deliver 5 pallets. Expected unload start time is 2.673271414
+Vehicle SP4 travels from 9 to DepotReturn to deliver 0 pallets. Expected unload start time is 4.402305275
+Vehicle SP5 travels from Depot to 11 to deliver 4 pallets. Expected unload start time is 8.091231127
+Vehicle SP5 travels from 2 to DepotReturn to deliver 0 pallets. Expected unload start time is 16.008452326
+Vehicle SP5 travels from 3 to 2 to deliver 3 pallets. Expected unload start time is 14
+Vehicle SP5 travels from 6 to 12 to deliver 10 pallets. Expected unload start time is 10.941590673
+Vehicle SP5 travels from 11 to 6 to deliver 8 pallets. Expected unload start time is 9.348735094
+Vehicle SP5 travels from 12 to 3 to deliver 1 pallets. Expected unload start time is 12.844364968
+Objective value: 1079.070671831
+Solve time: 2049569</t>
+        </is>
+      </c>
+      <c r="M58" s="11">
         <f>ROUND((K58-G58)/G58,5)</f>
         <v/>
       </c>
-      <c r="N58" s="12" t="n"/>
-      <c r="R58" s="12">
+      <c r="N58" s="11" t="n"/>
+      <c r="R58" s="11">
         <f>ROUND((Q58-G58)/G58,5)</f>
         <v/>
       </c>
-      <c r="S58" s="13">
+      <c r="S58" s="12">
         <f>ROUND((Q58-K58)/K58,5)</f>
         <v/>
       </c>
-      <c r="W58" s="13">
+      <c r="W58" s="12">
         <f>ROUND((V58-U58)/U58,5)</f>
         <v/>
       </c>
     </row>
-    <row r="59">
+    <row r="59" ht="15" customHeight="1" s="15">
       <c r="A59" t="n">
         <v>12</v>
       </c>
@@ -10136,26 +9833,71 @@
         <f>F59/1000</f>
         <v/>
       </c>
-      <c r="H59" s="16" t="n"/>
-      <c r="M59" s="12">
+      <c r="F59" t="n">
+        <v>142587</v>
+      </c>
+      <c r="G59" t="n">
+        <v>1065.533632739</v>
+      </c>
+      <c r="H59" s="16" t="inlineStr">
+        <is>
+          <t>Input:
+Customer 1 has 9 pallets demand and window 0-24 at (-21.058710905, -85.732132641) and average unload time 0.08006281
+Customer 2 has 4 pallets demand and window 0-24 at (-61.530467477, 1.737117717) and average unload time 0.094669005
+Customer 3 has 1 pallets demand and window 0-24 at (-50.677734248, -53.936729153) and average unload time 0.022009121
+Customer 4 has 6 pallets demand and window 0-24 at (-69.054106936, -51.628713993) and average unload time 0.155332702
+Customer 5 has 7 pallets demand and window 0-24 at (72.066314682, 21.176732398) and average unload time 0.101851625
+Customer 6 has 4 pallets demand and window 0-24 at (99.703455051, -23.277342091) and average unload time 0.058345596
+Customer 7 has 9 pallets demand and window 0-24 at (-99.403509456, -74.089731337) and average unload time 0.138604905
+Customer 8 has 7 pallets demand and window 0-24 at (-94.024021409, -85.062275023) and average unload time 0.135408239
+Customer 9 has 9 pallets demand and window 20-21 at (33.467209204, -64.83280491) and average unload time 0.079560351
+Customer 10 has 2 pallets demand and window 6-7 at (-89.273295195, 57.58077261) and average unload time 0.03541879
+Customer 11 has 1 pallets demand and window 0-24 at (-23.053132966, 62.283270093) and average unload time 0.128154381
+Customer 12 has 6 pallets demand and window 16-17 at (60.17467471, -61.397482643) and average unload time 0.146222627
+Vehicle SP1 is a 11 metre with capacity 30, distance cost 0.963034084, and time cost 12.240195381
+Vehicle SP2 is a 8 metre with capacity 22, distance cost 1.28918797, and time cost 13.157882916
+Vehicle SP3 is a 11 metre with capacity 30, distance cost 0.963034084, and time cost 12.240195381
+Vehicle SP4 is a Rigid with capacity 16, distance cost 0.734679723, and time cost 14.412072107
+Vehicle SP5 is a 8 metre with capacity 22, distance cost 1.28918797, and time cost 13.157882916
+Output:
+Vehicle SP1 travels from Depot to 5 to deliver 7 pallets. Expected unload start time is 14.712907548
+Vehicle SP1 travels from 5 to 6 to deliver 4 pallets. Expected unload start time is 16.080178708
+Vehicle SP1 travels from 6 to 12 to deliver 6 pallets. Expected unload start time is 17
+Vehicle SP1 travels from 9 to DepotReturn to deliver 0 pallets. Expected unload start time is 21.628059012
+Vehicle SP1 travels from 12 to 9 to deliver 9 pallets. Expected unload start time is 20
+Vehicle SP3 travels from Depot to 11 to deliver 1 pallets. Expected unload start time is 6.042009098
+Vehicle SP3 travels from 2 to 7 to deliver 9 pallets. Expected unload start time is 9.288441114
+Vehicle SP3 travels from 3 to DepotReturn to deliver 0 pallets. Expected unload start time is 14.26874083
+Vehicle SP3 travels from 4 to 3 to deliver 1 pallets. Expected unload start time is 13.321613177
+Vehicle SP3 travels from 7 to 8 to deliver 7 pallets. Expected unload start time is 10.688638945
+Vehicle SP3 travels from 8 to 4 to deliver 6 pallets. Expected unload start time is 12.158107649
+Vehicle SP3 travels from 10 to 2 to deliver 4 pallets. Expected unload start time is 7.850278313
+Vehicle SP3 travels from 11 to 10 to deliver 2 pallets. Expected unload start time is 7
+Vehicle SP4 travels from Depot to 1 to deliver 9 pallets. Expected unload start time is 1.10350775
+Vehicle SP4 travels from 1 to DepotReturn to deliver 0 pallets. Expected unload start time is 2.927580787
+Objective value: 1065.533632739
+Solve time: 142587</t>
+        </is>
+      </c>
+      <c r="M59" s="11">
         <f>ROUND((K59-G59)/G59,5)</f>
         <v/>
       </c>
-      <c r="N59" s="12" t="n"/>
-      <c r="R59" s="12">
+      <c r="N59" s="11" t="n"/>
+      <c r="R59" s="11">
         <f>ROUND((Q59-G59)/G59,5)</f>
         <v/>
       </c>
-      <c r="S59" s="13">
+      <c r="S59" s="12">
         <f>ROUND((Q59-K59)/K59,5)</f>
         <v/>
       </c>
-      <c r="W59" s="13">
+      <c r="W59" s="12">
         <f>ROUND((V59-U59)/U59,5)</f>
         <v/>
       </c>
     </row>
-    <row r="60">
+    <row r="60" ht="15" customHeight="1" s="15">
       <c r="A60" t="n">
         <v>12</v>
       </c>
@@ -10173,26 +9915,72 @@
         <f>F60/1000</f>
         <v/>
       </c>
-      <c r="H60" s="16" t="n"/>
-      <c r="M60" s="12">
+      <c r="F60" t="n">
+        <v>100543</v>
+      </c>
+      <c r="G60" t="n">
+        <v>1187.542333671</v>
+      </c>
+      <c r="H60" s="16" t="inlineStr">
+        <is>
+          <t>Input:
+Customer 1 has 7 pallets demand and window 0-24 at (91.438134137, 17.447596608) and average unload time 0.084138119
+Customer 2 has 8 pallets demand and window 0-24 at (20.623928657, -14.412303451) and average unload time 0.05011469
+Customer 3 has 2 pallets demand and window 0-24 at (-83.6329276, 1.252347453) and average unload time 0.147704323
+Customer 4 has 8 pallets demand and window 0-24 at (-37.294681917, 10.731904881) and average unload time 0.047134934
+Customer 5 has 9 pallets demand and window 0-24 at (-25.465924875, -60.961725972) and average unload time 0.086974199
+Customer 6 has 8 pallets demand and window 0-24 at (-76.288102705, 97.421796628) and average unload time 0.128563048
+Customer 7 has 5 pallets demand and window 0-24 at (-30.298270095, -74.514043051) and average unload time 0.124786882
+Customer 8 has 3 pallets demand and window 19-20 at (-79.6590541, -7.765564004) and average unload time 0.098181791
+Customer 9 has 3 pallets demand and window 0-24 at (82.043986031, 86.067861937) and average unload time 0.160404827
+Customer 10 has 9 pallets demand and window 10-11 at (83.432869817, 85.176582798) and average unload time 0.025520839
+Customer 11 has 9 pallets demand and window 0-24 at (-55.963300913, 93.273855672) and average unload time 0.072386171
+Customer 12 has 2 pallets demand and window 0-24 at (77.559232238, -37.089194511) and average unload time 0.113464765
+Vehicle SP1 is a 8 metre with capacity 22, distance cost 1.069854724, and time cost 14.736412156
+Vehicle SP2 is a Rigid with capacity 16, distance cost 1.073487361, and time cost 8.473161214
+Vehicle SP3 is a Rigid with capacity 16, distance cost 1.073487361, and time cost 8.473161214
+Vehicle SP4 is a Rigid with capacity 16, distance cost 1.073487361, and time cost 8.473161214
+Vehicle SP5 is a 11 metre with capacity 30, distance cost 1.207594963, and time cost 14.728007226
+Output:
+Vehicle SP1 travels from Depot to 9 to deliver 3 pallets. Expected unload start time is 9.4981572
+Vehicle SP1 travels from 1 to 12 to deliver 2 pallets. Expected unload start time is 12.374598469
+Vehicle SP1 travels from 9 to 10 to deliver 9 pallets. Expected unload start time is 10
+Vehicle SP1 travels from 10 to 1 to deliver 7 pallets. Expected unload start time is 11.082193038
+Vehicle SP1 travels from 12 to DepotReturn to deliver 0 pallets. Expected unload start time is 13.676167681
+Vehicle SP3 travels from Depot to 2 to deliver 8 pallets. Expected unload start time is 0.314508775
+Vehicle SP3 travels from 2 to DepotReturn to deliver 0 pallets. Expected unload start time is 1.029935067
+Vehicle SP4 travels from Depot to 7 to deliver 5 pallets. Expected unload start time is 1.005479346
+Vehicle SP4 travels from 5 to DepotReturn to deliver 0 pallets. Expected unload start time is 3.417869754
+Vehicle SP4 travels from 7 to 5 to deliver 9 pallets. Expected unload start time is 1.809264761
+Vehicle SP5 travels from Depot to 11 to deliver 9 pallets. Expected unload start time is 16.436512346
+Vehicle SP5 travels from 3 to 8 to deliver 3 pallets. Expected unload start time is 20
+Vehicle SP5 travels from 4 to DepotReturn to deliver 0 pallets. Expected unload start time is 21.734558054
+Vehicle SP5 travels from 6 to 3 to deliver 2 pallets. Expected unload start time is 19.581408057
+Vehicle SP5 travels from 8 to 4 to deliver 8 pallets. Expected unload start time is 20.87237758
+Vehicle SP5 travels from 11 to 6 to deliver 8 pallets. Expected unload start time is 17.347284702
+Objective value: 1187.542333671
+Solve time: 100543</t>
+        </is>
+      </c>
+      <c r="M60" s="11">
         <f>ROUND((K60-G60)/G60,5)</f>
         <v/>
       </c>
-      <c r="N60" s="12" t="n"/>
-      <c r="R60" s="12">
+      <c r="N60" s="11" t="n"/>
+      <c r="R60" s="11">
         <f>ROUND((Q60-G60)/G60,5)</f>
         <v/>
       </c>
-      <c r="S60" s="13">
+      <c r="S60" s="12">
         <f>ROUND((Q60-K60)/K60,5)</f>
         <v/>
       </c>
-      <c r="W60" s="13">
+      <c r="W60" s="12">
         <f>ROUND((V60-U60)/U60,5)</f>
         <v/>
       </c>
     </row>
-    <row r="61">
+    <row r="61" ht="15" customHeight="1" s="15">
       <c r="A61" t="n">
         <v>12</v>
       </c>
@@ -10210,37 +9998,83 @@
         <f>F61/1000</f>
         <v/>
       </c>
-      <c r="H61" s="16" t="n"/>
-      <c r="M61" s="12">
+      <c r="F61" t="n">
+        <v>3916742</v>
+      </c>
+      <c r="G61" t="n">
+        <v>1014.184533394</v>
+      </c>
+      <c r="H61" s="16" t="inlineStr">
+        <is>
+          <t>Input:
+Customer 1 has 4 pallets demand and window 0-24 at (-29.236009491, 13.763775838) and average unload time 0.028283481
+Customer 2 has 4 pallets demand and window 0-24 at (70.149307077, 13.79415784) and average unload time 0.071559976
+Customer 3 has 1 pallets demand and window 0-24 at (-42.049988492, -84.896454508) and average unload time 0.102735431
+Customer 4 has 11 pallets demand and window 0-24 at (47.755556562, -11.732306242) and average unload time 0.096625309
+Customer 5 has 9 pallets demand and window 0-24 at (91.110804245, -45.197705153) and average unload time 0.137938956
+Customer 6 has 9 pallets demand and window 12-13 at (-57.200885301, -12.54838386) and average unload time 0.028373223
+Customer 7 has 4 pallets demand and window 0-24 at (78.032734314, 40.08765245) and average unload time 0.166425632
+Customer 8 has 3 pallets demand and window 14-15 at (-78.467693829, -20.077883184) and average unload time 0.08331469
+Customer 9 has 9 pallets demand and window 0-24 at (-68.401786042, 4.948386826) and average unload time 0.077273626
+Customer 10 has 6 pallets demand and window 0-24 at (72.527057688, -0.556721134) and average unload time 0.02137963
+Customer 11 has 11 pallets demand and window 0-24 at (83.57894321, 10.511544341) and average unload time 0.094713115
+Customer 12 has 2 pallets demand and window 0-24 at (-42.817211399, -51.000071044) and average unload time 0.020278036
+Vehicle SP1 is a 8 metre with capacity 22, distance cost 1.389215585, and time cost 8.60907932
+Vehicle SP2 is a 11 metre with capacity 30, distance cost 1.285845201, and time cost 7.081749349
+Vehicle SP3 is a 11 metre with capacity 30, distance cost 1.285845201, and time cost 7.081749349
+Vehicle SP4 is a Rigid with capacity 16, distance cost 1.088041369, and time cost 14.33111071
+Vehicle SP5 is a 11 metre with capacity 30, distance cost 1.285845201, and time cost 7.081749349
+Output:
+Vehicle SP2 travels from Depot to 7 to deliver 4 pallets. Expected unload start time is 1.096594692
+Vehicle SP2 travels from 2 to 11 to deliver 11 pallets. Expected unload start time is 2.564473233
+Vehicle SP2 travels from 4 to DepotReturn to deliver 0 pallets. Expected unload start time is 5.367630083
+Vehicle SP2 travels from 7 to 2 to deliver 4 pallets. Expected unload start time is 2.105420806
+Vehicle SP2 travels from 10 to 4 to deliver 5 pallets. Expected unload start time is 4.269808466
+Vehicle SP2 travels from 11 to 10 to deliver 6 pallets. Expected unload start time is 3.801833905
+Vehicle SP4 travels from Depot to 5 to deliver 9 pallets. Expected unload start time is 0.732013833
+Vehicle SP4 travels from 4 to DepotReturn to deliver 0 pallets. Expected unload start time is 3.8525201
+Vehicle SP4 travels from 5 to 4 to deliver 6 pallets. Expected unload start time is 2.658073174
+Vehicle SP5 travels from Depot to 1 to deliver 4 pallets. Expected unload start time is 11.429896998
+Vehicle SP5 travels from 1 to 9 to deliver 9 pallets. Expected unload start time is 12.04485091
+Vehicle SP5 travels from 3 to 12 to deliver 2 pallets. Expected unload start time is 15.70584881
+Vehicle SP5 travels from 6 to 8 to deliver 3 pallets. Expected unload start time is 13.999999997
+Vehicle SP5 travels from 8 to 3 to deliver 1 pallets. Expected unload start time is 15.179300064
+Vehicle SP5 travels from 9 to 6 to deliver 9 pallets. Expected unload start time is 13.000000001
+Vehicle SP5 travels from 12 to DepotReturn to deliver 0 pallets. Expected unload start time is 16.578788585
+Objective value: 1014.184533394
+Solve time: 3916742</t>
+        </is>
+      </c>
+      <c r="M61" s="11">
         <f>ROUND((K61-G61)/G61,5)</f>
         <v/>
       </c>
-      <c r="N61" s="12" t="n"/>
-      <c r="R61" s="12">
+      <c r="N61" s="11" t="n"/>
+      <c r="R61" s="11">
         <f>ROUND((Q61-G61)/G61,5)</f>
         <v/>
       </c>
-      <c r="S61" s="13">
+      <c r="S61" s="12">
         <f>ROUND((Q61-K61)/K61,5)</f>
         <v/>
       </c>
-      <c r="W61" s="13">
+      <c r="W61" s="12">
         <f>ROUND((V61-U61)/U61,5)</f>
         <v/>
       </c>
     </row>
-    <row r="62">
+    <row r="62" ht="15" customHeight="1" s="15">
       <c r="H62" s="16" t="n"/>
-      <c r="M62" s="12" t="n"/>
-      <c r="N62" s="12" t="n"/>
-      <c r="R62" s="12" t="n"/>
-      <c r="S62" s="13" t="n"/>
-      <c r="W62" s="13" t="n"/>
-    </row>
-    <row r="63">
+      <c r="M62" s="11" t="n"/>
+      <c r="N62" s="11" t="n"/>
+      <c r="R62" s="11" t="n"/>
+      <c r="S62" s="12" t="n"/>
+      <c r="W62" s="12" t="n"/>
+    </row>
+    <row r="63" ht="15" customHeight="1" s="15">
       <c r="H63" s="16" t="n"/>
     </row>
-    <row r="64">
+    <row r="64" ht="15" customHeight="1" s="15">
       <c r="H64" s="16" t="n"/>
     </row>
     <row r="65">
@@ -10886,12 +10720,12 @@
     <mergeCell ref="H151:I151"/>
   </mergeCells>
   <conditionalFormatting sqref="R63:R1048576 R1:R61">
-    <cfRule type="cellIs" priority="35" operator="lessThan" dxfId="1">
+    <cfRule type="cellIs" priority="35" operator="lessThan" dxfId="0">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R62">
-    <cfRule type="cellIs" priority="18" operator="lessThan" dxfId="1">
+    <cfRule type="cellIs" priority="18" operator="lessThan" dxfId="0">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -10903,7 +10737,7 @@
     <cfRule type="cellIs" priority="34" operator="lessThan" dxfId="4">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" priority="36" operator="equal" dxfId="0">
+    <cfRule type="cellIs" priority="36" operator="equal" dxfId="3">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -10915,33 +10749,33 @@
     <cfRule type="cellIs" priority="11" operator="lessThan" dxfId="4">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" priority="12" operator="equal" dxfId="0">
+    <cfRule type="cellIs" priority="12" operator="equal" dxfId="3">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M2:M1048576">
-    <cfRule type="cellIs" priority="5" operator="lessThan" dxfId="1">
+    <cfRule type="cellIs" priority="5" operator="lessThan" dxfId="0">
       <formula>-0.01</formula>
     </cfRule>
     <cfRule type="cellIs" priority="6" operator="greaterThan" dxfId="4">
       <formula>0.01</formula>
     </cfRule>
-    <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
+    <cfRule type="cellIs" priority="1" operator="equal" dxfId="3">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P2:P11 P63:P1048576 P19:P61">
-    <cfRule type="cellIs" priority="4" operator="greaterThan" dxfId="1">
+    <cfRule type="cellIs" priority="4" operator="greaterThan" dxfId="0">
       <formula>1800</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P62">
-    <cfRule type="cellIs" priority="3" operator="greaterThan" dxfId="1">
+    <cfRule type="cellIs" priority="3" operator="greaterThan" dxfId="0">
       <formula>1800</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P12:P18">
-    <cfRule type="cellIs" priority="2" operator="greaterThan" dxfId="1">
+    <cfRule type="cellIs" priority="2" operator="greaterThan" dxfId="0">
       <formula>1800</formula>
     </cfRule>
   </conditionalFormatting>
@@ -10965,19 +10799,19 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="12.28515625" bestFit="1" customWidth="1" style="18" min="1" max="1"/>
-    <col width="14.42578125" bestFit="1" customWidth="1" style="18" min="2" max="2"/>
-    <col width="14.42578125" customWidth="1" style="18" min="3" max="3"/>
-    <col width="12" bestFit="1" customWidth="1" style="18" min="4" max="4"/>
-    <col width="15" bestFit="1" customWidth="1" style="18" min="5" max="5"/>
-    <col width="19" bestFit="1" customWidth="1" style="18" min="6" max="6"/>
-    <col width="51.140625" customWidth="1" style="18" min="7" max="7"/>
-    <col width="16" bestFit="1" customWidth="1" style="18" min="8" max="8"/>
-    <col width="12" bestFit="1" customWidth="1" style="18" min="9" max="9"/>
-    <col width="12.85546875" bestFit="1" customWidth="1" style="18" min="10" max="10"/>
-    <col width="13.5703125" bestFit="1" customWidth="1" style="18" min="11" max="11"/>
-    <col width="14" bestFit="1" customWidth="1" style="18" min="12" max="12"/>
-    <col width="41.7109375" customWidth="1" style="18" min="13" max="13"/>
+    <col width="12.28515625" bestFit="1" customWidth="1" style="15" min="1" max="1"/>
+    <col width="14.42578125" bestFit="1" customWidth="1" style="15" min="2" max="2"/>
+    <col width="14.42578125" customWidth="1" style="15" min="3" max="3"/>
+    <col width="12" bestFit="1" customWidth="1" style="15" min="4" max="4"/>
+    <col width="15" bestFit="1" customWidth="1" style="15" min="5" max="5"/>
+    <col width="19" bestFit="1" customWidth="1" style="15" min="6" max="6"/>
+    <col width="51.140625" customWidth="1" style="15" min="7" max="7"/>
+    <col width="16" bestFit="1" customWidth="1" style="15" min="8" max="8"/>
+    <col width="12" bestFit="1" customWidth="1" style="15" min="9" max="9"/>
+    <col width="12.85546875" bestFit="1" customWidth="1" style="15" min="10" max="10"/>
+    <col width="13.5703125" bestFit="1" customWidth="1" style="15" min="11" max="11"/>
+    <col width="14" bestFit="1" customWidth="1" style="15" min="12" max="12"/>
+    <col width="41.7109375" customWidth="1" style="15" min="13" max="13"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -11148,12 +10982,12 @@
         <f>D2-I2</f>
         <v/>
       </c>
-      <c r="L2" s="12">
+      <c r="L2" s="11">
         <f>K2/D2</f>
         <v/>
       </c>
     </row>
-    <row r="3" ht="14.25" customHeight="1" s="18">
+    <row r="3" ht="14.25" customHeight="1" s="15">
       <c r="A3" s="10" t="n">
         <v>43768</v>
       </c>
@@ -11265,7 +11099,7 @@
         <f>D3-I3</f>
         <v/>
       </c>
-      <c r="L3" s="12">
+      <c r="L3" s="11">
         <f>K3/D3</f>
         <v/>
       </c>
@@ -11393,7 +11227,7 @@
         <f>D4-(I4+J4*10)</f>
         <v/>
       </c>
-      <c r="L4" s="12">
+      <c r="L4" s="11">
         <f>K4/D4</f>
         <v/>
       </c>
@@ -11553,7 +11387,7 @@
         <f>D5-(I5+J5*10)</f>
         <v/>
       </c>
-      <c r="L5" s="12">
+      <c r="L5" s="11">
         <f>K5/D5</f>
         <v/>
       </c>
@@ -11676,7 +11510,7 @@
         <f>D6-(I6+J6*10)</f>
         <v/>
       </c>
-      <c r="L6" s="12">
+      <c r="L6" s="11">
         <f>K6/D6</f>
         <v/>
       </c>
@@ -11766,7 +11600,7 @@
         <f>D7-(I7+J7*10)</f>
         <v/>
       </c>
-      <c r="L7" s="12">
+      <c r="L7" s="11">
         <f>K7/D7</f>
         <v/>
       </c>
@@ -11892,7 +11726,7 @@
         <f>D8-(I8+J8*10)</f>
         <v/>
       </c>
-      <c r="L8" s="12">
+      <c r="L8" s="11">
         <f>K8/D8</f>
         <v/>
       </c>
@@ -12006,7 +11840,7 @@
         <f>D9-(I9+J9*10)</f>
         <v/>
       </c>
-      <c r="L9" s="12">
+      <c r="L9" s="11">
         <f>K9/D9</f>
         <v/>
       </c>
@@ -12096,7 +11930,7 @@
         <f>D10-(I10+J10*10)</f>
         <v/>
       </c>
-      <c r="L10" s="12">
+      <c r="L10" s="11">
         <f>K10/D10</f>
         <v/>
       </c>
@@ -12220,7 +12054,7 @@
         <f>D11-(I11+J11*10)</f>
         <v/>
       </c>
-      <c r="L11" s="12">
+      <c r="L11" s="11">
         <f>K11/D11</f>
         <v/>
       </c>
@@ -12324,7 +12158,7 @@
         <f>D12-(I12+J12*10)</f>
         <v/>
       </c>
-      <c r="L12" s="12">
+      <c r="L12" s="11">
         <f>K12/D12</f>
         <v/>
       </c>
@@ -12454,7 +12288,7 @@
         <f>D13-(I13+J13*10)</f>
         <v/>
       </c>
-      <c r="L13" s="12">
+      <c r="L13" s="11">
         <f>K13/D13</f>
         <v/>
       </c>
@@ -12640,7 +12474,7 @@
         <f>D14-(I14+J14*10)</f>
         <v/>
       </c>
-      <c r="L14" s="12">
+      <c r="L14" s="11">
         <f>K14/D14</f>
         <v/>
       </c>
@@ -12761,7 +12595,7 @@
         <f>D15-(I15+J15*10)</f>
         <v/>
       </c>
-      <c r="L15" s="12">
+      <c r="L15" s="11">
         <f>K15/D15</f>
         <v/>
       </c>
@@ -12864,7 +12698,7 @@
         <f>D16-(I16+J16*10)</f>
         <v/>
       </c>
-      <c r="L16" s="12">
+      <c r="L16" s="11">
         <f>K16/D16</f>
         <v/>
       </c>
@@ -13003,7 +12837,7 @@
         <f>D17-(I17+J17*10)</f>
         <v/>
       </c>
-      <c r="L17" s="12">
+      <c r="L17" s="11">
         <f>K17/D17</f>
         <v/>
       </c>
@@ -13187,7 +13021,7 @@
         <f>D18-(I18+J18*10)</f>
         <v/>
       </c>
-      <c r="L18" s="12">
+      <c r="L18" s="11">
         <f>K18/D18</f>
         <v/>
       </c>
@@ -13290,7 +13124,7 @@
         <f>D19-(I19+J19*10)</f>
         <v/>
       </c>
-      <c r="L19" s="12">
+      <c r="L19" s="11">
         <f>K19/D19</f>
         <v/>
       </c>
@@ -13421,7 +13255,7 @@
         <f>D20-(I20+J20*10)</f>
         <v/>
       </c>
-      <c r="L20" s="12">
+      <c r="L20" s="11">
         <f>K20/D20</f>
         <v/>
       </c>
@@ -13608,7 +13442,7 @@
         <f>D21-(I21+J21*10)</f>
         <v/>
       </c>
-      <c r="L21" s="12">
+      <c r="L21" s="11">
         <f>K21/D21</f>
         <v/>
       </c>
@@ -13704,7 +13538,7 @@
         <f>D22-(I22+J22*10)</f>
         <v/>
       </c>
-      <c r="L22" s="12">
+      <c r="L22" s="11">
         <f>K22/D22</f>
         <v/>
       </c>
@@ -13835,7 +13669,7 @@
         <f>D23-(I23+J23*10)</f>
         <v/>
       </c>
-      <c r="L23" s="12">
+      <c r="L23" s="11">
         <f>K23/D23</f>
         <v/>
       </c>
@@ -14021,7 +13855,7 @@
         <f>D24-(I24+J24*10)</f>
         <v/>
       </c>
-      <c r="L24" s="12">
+      <c r="L24" s="11">
         <f>K24/D24</f>
         <v/>
       </c>
@@ -14035,7 +13869,7 @@
           <t>{"2": [[[17, 24], [164, 4]], [[44, 30]], [[111, 2], [77, 28]], [[149, 27], [148, 3]], [[165, 30]], [[159, 19], [194, 11]], [[41, 30]], [[172, 30]], [[79, 30]], [[104, 30]], [[6, 23], [187, 7]], [[176, 30]], [[153, 30]], [[208, 30]], [[35, 30]], [[100, 30]], [[83, 20]], [[40, 30]], [[117, 7], [126, 14], [125, 9]], [[121, 12], [143, 11], [193, 7]], [[80, 20], [168, 9]], [[135, 5], [182, 15], [95, 10]], [[81, 30]], [[193, 12], [143, 18]], [[121, 19], [135, 10]]], "1": [[[75, 19]], [[149, 22]], [[24, 8], [25, 14]], [[207, 21]], [[72, 22]], [[119, 10], [2, 12]], [[157, 22]], [[46, 20]], [[188, 22]], [[186, 9], [53, 12]], [[130, 22]], [[83, 20]], [[116, 10], [177, 11], [203, 1]], [[27, 22]]], "0": [[[194, 16]], [[16, 10], [165, 4]], [[156, 15], [39, 1]], [[77, 11]], [[120, 11], [198, 5]], [[151, 16]], [[196, 8], [48, 5]], [[34, 14]], [[9, 15]], [[154, 14]], [[8, 16]], [[108, 11]], [[152, 15]], [[120, 12]], [[199, 1], [91, 6], [81, 6]], [[197, 14]], [[131, 16]], [[151, 9], [173, 7]], [[144, 12]], [[166, 6], [28, 2], [3, 8]], [[97, 13]], [[66, 15]], [[101, 5], [19, 11]]]}</t>
         </is>
       </c>
-      <c r="D25" s="14" t="n">
+      <c r="D25" s="13" t="n">
         <v>496052.9814666667</v>
       </c>
       <c r="F25" t="inlineStr">
@@ -14100,18 +13934,18 @@
 </t>
         </is>
       </c>
-      <c r="H25" s="14" t="n">
+      <c r="H25" s="13" t="n">
         <v>7048.7007023</v>
       </c>
-      <c r="I25" s="14" t="n">
+      <c r="I25" s="13" t="n">
         <v>448073.0931333331</v>
       </c>
-      <c r="J25" s="14" t="n"/>
-      <c r="K25" s="14">
+      <c r="J25" s="13" t="n"/>
+      <c r="K25" s="13">
         <f>D25-(I25+J25*10)</f>
         <v/>
       </c>
-      <c r="L25" s="12">
+      <c r="L25" s="11">
         <f>K25/D25</f>
         <v/>
       </c>
@@ -14133,7 +13967,7 @@
           <t>{"2": [[[149, 30]], [[172, 30]], [[165, 30]], [[44, 30]], [[149, 24], [148, 6]], [[159, 24], [41, 6]], [[77, 30]], [[15, 28]], [[150, 8], [172, 20]], [[98, 16], [153, 14]], [[194, 30]], [[79, 30]], [[6, 14], [187, 8], [194, 8]], [[104, 30]], [[41, 30]], [[153, 30]], [[176, 16], [35, 5], [209, 9]], [[100, 30]], [[208, 24], [152, 4]], [[16, 30]], [[24, 25], [25, 4], [66, 1]], [[110, 19], [174, 5], [104, 6]], [[35, 30]], [[156, 11], [168, 9], [132, 10]], [[25, 30]], [[59, 28]], [[117, 6], [126, 10], [125, 14]], [[40, 30]], [[92, 30]], [[72, 30]], [[29, 29]], [[139, 15], [40, 15]], [[121, 6], [143, 5], [193, 4], [19, 6], [97, 9]], [[186, 1], [95, 12], [182, 6], [101, 10], [75, 1]], [[33, 30]], [[4, 30]], [[49, 21], [197, 9]], [[32, 27]], [[81, 30]], [[8, 30]], [[55, 30]], [[97, 28]], [[140, 30]]], "0": [[[79, 7], [77, 7]], [[120, 10], [198, 6]], [[96, 16]], [[188, 15], [39, 1]], [[151, 14], [123, 1]], [[46, 16]], [[17, 15], [164, 1]], [[42, 12]], [[134, 10], [171, 2]], [[37, 10], [123, 1]], [[9, 10], [48, 5]], [[62, 1], [155, 1], [87, 1], [57, 13]], [[191, 2], [94, 5]], [[196, 13], [157, 3]], [[34, 16]], [[154, 15]], [[144, 3], [49, 3]], [[63, 16]], [[108, 9], [120, 7]], [[199, 10], [74, 5]], [[93, 9], [70, 7]], [[186, 14], [151, 1]], [[91, 13], [81, 2]], [[53, 13], [95, 3]], [[197, 16]], [[66, 12]], [[131, 12], [8, 4]], [[83, 13]], [[75, 5], [28, 6], [135, 5]]], "1": [[[207, 20]], [[83, 18], [2, 4]], [[82, 22]], [[119, 12], [2, 10]], [[68, 10], [1, 3], [18, 8], [112, 1]], [[18, 7], [200, 15]], [[157, 21]], [[163, 17], [3, 5]], [[192, 22]], [[66, 22]], [[38, 22]], [[33, 9], [4, 11]], [[88, 22]], [[3, 22]]]}</t>
         </is>
       </c>
-      <c r="D26" s="14" t="n">
+      <c r="D26" s="13" t="n">
         <v>595195.3826666666</v>
       </c>
       <c r="F26" t="inlineStr">
@@ -14221,18 +14055,18 @@
 </t>
         </is>
       </c>
-      <c r="H26" s="14" t="n">
+      <c r="H26" s="13" t="n">
         <v>7200.4963603</v>
       </c>
-      <c r="I26" s="14" t="n">
+      <c r="I26" s="13" t="n">
         <v>559057.7403333329</v>
       </c>
-      <c r="J26" s="14" t="n"/>
-      <c r="K26" s="14">
+      <c r="J26" s="13" t="n"/>
+      <c r="K26" s="13">
         <f>D26-(I26+J26*10)</f>
         <v/>
       </c>
-      <c r="L26" s="12">
+      <c r="L26" s="11">
         <f>K26/D26</f>
         <v/>
       </c>
@@ -14249,7 +14083,7 @@
           <t>{"3": [[[22, 36]], [[41, 39]], [[23, 40]], [[85, 30]]], "1": [[[156, 17], [132, 5]], [[17, 10], [164, 1], [197, 11]], [[207, 22]], [[83, 22]], [[119, 12], [2, 10]], [[46, 20]], [[188, 20]], [[151, 20]], [[56, 11], [118, 9]], [[72, 15], [18, 7]], [[58, 15], [22, 7]], [[142, 22]], [[50, 2], [78, 6], [113, 4], [94, 6], [102, 4]], [[35, 21]], [[168, 13], [17, 7]], [[163, 18], [3, 4]], [[186, 22]], [[205, 9], [45, 6], [206, 7]], [[144, 21], [106, 1]], [[157, 10], [28, 11], [11, 1]], [[121, 4], [143, 6], [193, 7], [185, 5]], [[135, 11], [95, 3], [182, 7]], [[151, 22]], [[173, 13], [131, 7]], [[40, 22]], [[57, 21]], [[89, 22]], [[158, 22]], [[84, 22]]], "2": [[[59, 30]], [[154, 1], [68, 8], [1, 21]], [[72, 30]], [[29, 30]], [[18, 17], [200, 13]], [[96, 27]], [[152, 4], [15, 26]], [[139, 30]], [[24, 9], [25, 7], [59, 11]], [[40, 30]], [[117, 2], [126, 14], [125, 14]], [[157, 15], [95, 15]], [[135, 15], [33, 5], [182, 10]], [[121, 14], [143, 15]], [[66, 19], [168, 11]], [[69, 30]], [[153, 30]], [[91, 27]], [[49, 30]], [[208, 30]], [[29, 10], [1, 20]], [[12, 20]], [[81, 5], [91, 23]], [[193, 6], [19, 12], [101, 10]], [[104, 12], [100, 15], [153, 3]], [[95, 30]], [[201, 30]], [[111, 30]], [[99, 30]], [[124, 30]], [[150, 30]], [[109, 30]], [[104, 30]], [[15, 30]], [[98, 30]], [[99, 10], [26, 20]], [[149, 30]], [[150, 19], [149, 7], [165, 4]], [[110, 7], [176, 8], [174, 14], [60, 1]], [[172, 20], [111, 10]], [[109, 28]], [[156, 20], [132, 10]], [[10, 30]], [[76, 20], [10, 10]], [[17, 29], [164, 1]], [[53, 14], [130, 16]], [[3, 26], [51, 4]], [[29, 28]], [[154, 30]], [[11, 2], [208, 11], [97, 14]], [[69, 30]], [[157, 1], [193, 6], [143, 12], [121, 11]], [[178, 28], [61, 2]], [[45, 7], [175, 23]], [[185, 17]], [[19, 2], [28, 17], [101, 11]], [[69, 30]], [[147, 7]], [[85, 30]], [[20, 30]], [[84, 30]], [[116, 5], [85, 23]], [[20, 18]], [[92, 30]]], "0": [[[7, 4], [188, 6], [39, 5]], [[120, 9], [198, 6]], [[80, 16]], [[69, 15]], [[134, 13]], [[92, 16]], [[112, 2], [198, 7], [42, 1]], [[51, 12]], [[62, 13], [155, 1], [87, 2]], [[47, 12], [166, 4]], [[128, 14]], [[105, 5], [46, 4], [115, 7]], [[191, 4], [48, 10], [96, 2]], [[186, 16]], [[134, 8], [171, 5]], [[93, 10], [151, 6]], [[8, 5], [33, 5]], [[142, 4], [12, 11]], [[130, 3], [53, 13]], [[13, 16]], [[9, 11]], [[97, 15]], [[75, 3], [135, 6]], [[90, 16]], [[128, 1]], [[128, 1]], [[128, 1]], [[195, 1]], [[83, 16]], [[69, 7]], [[158, 13]]]}</t>
         </is>
       </c>
-      <c r="D27" s="14" t="n">
+      <c r="D27" s="13" t="n">
         <v>1381861.717933334</v>
       </c>
       <c r="F27" t="inlineStr">
@@ -14391,18 +14225,18 @@
 </t>
         </is>
       </c>
-      <c r="H27" s="14" t="n">
+      <c r="H27" s="13" t="n">
         <v>7888.9231545</v>
       </c>
-      <c r="I27" s="14" t="n">
+      <c r="I27" s="13" t="n">
         <v>1204977.810166667</v>
       </c>
-      <c r="J27" s="14" t="n"/>
-      <c r="K27" s="14">
+      <c r="J27" s="13" t="n"/>
+      <c r="K27" s="13">
         <f>D27-(I27+J27*10)</f>
         <v/>
       </c>
-      <c r="L27" s="12">
+      <c r="L27" s="11">
         <f>K27/D27</f>
         <v/>
       </c>
@@ -14491,11 +14325,11 @@
       <c r="I28" t="n">
         <v>541168.9366666665</v>
       </c>
-      <c r="K28" s="14">
+      <c r="K28" s="13">
         <f>D28-(I28+J28*10)</f>
         <v/>
       </c>
-      <c r="L28" s="12">
+      <c r="L28" s="11">
         <f>K28/D28</f>
         <v/>
       </c>
@@ -14612,11 +14446,11 @@
       <c r="I29" t="n">
         <v>661103.9565833332</v>
       </c>
-      <c r="K29" s="14">
+      <c r="K29" s="13">
         <f>D29-(I29+J29*10)</f>
         <v/>
       </c>
-      <c r="L29" s="12">
+      <c r="L29" s="11">
         <f>K29/D29</f>
         <v/>
       </c>
@@ -14766,11 +14600,11 @@
       <c r="I30" t="n">
         <v>1410468.586666666</v>
       </c>
-      <c r="K30" s="14">
+      <c r="K30" s="13">
         <f>D30-(I30+J30*10)</f>
         <v/>
       </c>
-      <c r="L30" s="12">
+      <c r="L30" s="11">
         <f>K30/D30</f>
         <v/>
       </c>
@@ -14779,7 +14613,7 @@
       </c>
     </row>
     <row r="31">
-      <c r="L31" s="12" t="n"/>
+      <c r="L31" s="11" t="n"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:A28"/>

</xml_diff>